<commit_message>
Added new commands to gsutil cheatsheet.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7230"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gcloud cheatsheet" sheetId="4" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="86">
   <si>
     <t>Details</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Command</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
   <si>
     <t>Copy this</t>
@@ -151,12 +154,6 @@
   <si>
     <t xml:space="preserve">gcloud config
 </t>
-  </si>
-  <si>
-    <t>gsutil mb gs://unique-name</t>
-  </si>
-  <si>
-    <t>gsutil cp test.dat gs://unique-name</t>
   </si>
   <si>
     <t>Bucket name:</t>
@@ -293,6 +290,94 @@
   </si>
   <si>
     <t>Mount Point Name:</t>
+  </si>
+  <si>
+    <t>gsutil mb</t>
+  </si>
+  <si>
+    <t>gsutil cp</t>
+  </si>
+  <si>
+    <t>Copies files and objects from/to Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>Source Bucket name:</t>
+  </si>
+  <si>
+    <t>Source file:</t>
+  </si>
+  <si>
+    <t>Destination Bucket Name:</t>
+  </si>
+  <si>
+    <t>Destination file:</t>
+  </si>
+  <si>
+    <t>ada.jpg</t>
+  </si>
+  <si>
+    <t>ioso-bucket</t>
+  </si>
+  <si>
+    <t>Source dir:</t>
+  </si>
+  <si>
+    <t>Destination dir:</t>
+  </si>
+  <si>
+    <t>Copies files from/to Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>Copies directories from/to Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>image-folder/</t>
+  </si>
+  <si>
+    <t>gsutil ls</t>
+  </si>
+  <si>
+    <t>File name:</t>
+  </si>
+  <si>
+    <t>File/dir name:</t>
+  </si>
+  <si>
+    <t>Lists files and directories in Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>Lists details of files and directories in Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>gsutil rm</t>
+  </si>
+  <si>
+    <t>image-dir</t>
+  </si>
+  <si>
+    <t>image-dir/ada.jpg</t>
+  </si>
+  <si>
+    <t>Removes files and directories from Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>Removes files from Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>gsutil acl</t>
+  </si>
+  <si>
+    <t>Manages access rights to files and objectes in Google Cloud Storage buckets.</t>
+  </si>
+  <si>
+    <t>Grants read access to all users to a file in a Google Cloud Storage Bucket.</t>
+  </si>
+  <si>
+    <t>Revokes read access from all users to a file in a Google Cloud Storage Bucket.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
@@ -825,7 +910,7 @@
   </sheetPr>
   <dimension ref="B1:AK63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C33" sqref="C33:Z33"/>
     </sheetView>
   </sheetViews>
@@ -875,7 +960,7 @@
       <c r="Y1" s="21"/>
       <c r="Z1" s="21"/>
       <c r="AA1" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB1" s="18" t="s">
         <v>2</v>
@@ -896,7 +981,7 @@
     </row>
     <row r="2" spans="2:37" ht="30">
       <c r="B2" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -927,7 +1012,7 @@
         <v>gcloud compute</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
@@ -937,7 +1022,7 @@
       <c r="AH2" s="2"/>
       <c r="AI2" s="2"/>
       <c r="AJ2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AK2" s="1"/>
     </row>
@@ -975,7 +1060,7 @@
         <v>gcloud compute instances</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
@@ -985,7 +1070,7 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AK3" s="1"/>
     </row>
@@ -1023,23 +1108,23 @@
         <v>gcloud compute instances create gcp-test-1 --zone us-central1-a</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AK4" s="1"/>
     </row>
@@ -1077,31 +1162,31 @@
         <v>gcloud compute instances attach-disk gcelab --disk mydisk --device-name mydevice --zone us-central1-a</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AG5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="AK5" s="1"/>
     </row>
@@ -1139,7 +1224,7 @@
         <v>gcloud compute disks</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
@@ -1149,7 +1234,7 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AK6" s="1"/>
     </row>
@@ -1187,27 +1272,27 @@
         <v>gcloud compute disks create mydisk --size=200GB --zone us-central1-a</v>
       </c>
       <c r="AB7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AC7" s="5" t="s">
+      <c r="AD7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AD7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF7" s="2" t="s">
+      <c r="AG7" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="AG7" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AK7" s="1"/>
     </row>
@@ -1245,16 +1330,16 @@
         <v>gcloud compute disks ...</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
@@ -1297,7 +1382,7 @@
         <v>gcloud compute ssh</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
@@ -1307,7 +1392,7 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AK9" s="1"/>
     </row>
@@ -1345,23 +1430,23 @@
         <v>gcloud compute ssh gcelab --zone us-central1-a</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AK10" s="1"/>
     </row>
@@ -1396,7 +1481,7 @@
         <v/>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
@@ -1410,7 +1495,7 @@
     </row>
     <row r="12" spans="2:37">
       <c r="B12" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -1441,7 +1526,7 @@
         <v>gcloud auth</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
@@ -1451,7 +1536,7 @@
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AK12" s="1"/>
     </row>
@@ -1489,7 +1574,7 @@
         <v>gcloud auth list</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
@@ -1499,7 +1584,7 @@
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AK13" s="1"/>
     </row>
@@ -1534,7 +1619,7 @@
         <v/>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
@@ -1548,7 +1633,7 @@
     </row>
     <row r="15" spans="2:37">
       <c r="B15" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -1580,7 +1665,7 @@
 </v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
@@ -1590,7 +1675,7 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AK15" s="1"/>
     </row>
@@ -1630,7 +1715,7 @@
  list project</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
@@ -1640,7 +1725,7 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AK16" s="1"/>
     </row>
@@ -1680,7 +1765,7 @@
  list --all</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
@@ -1690,7 +1775,7 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AK17" s="1"/>
     </row>
@@ -1725,7 +1810,7 @@
         <v/>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
@@ -1771,10 +1856,10 @@
         <v>gcloud help config</v>
       </c>
       <c r="AB19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC19" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
@@ -1783,13 +1868,13 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="2:37">
       <c r="B20" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1820,7 +1905,7 @@
         <v>gcloud init</v>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
@@ -1830,7 +1915,7 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AK20" s="1"/>
     </row>
@@ -1868,7 +1953,7 @@
         <v>gcloud init --console-only</v>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
@@ -1878,7 +1963,7 @@
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AK21" s="1"/>
     </row>
@@ -1913,7 +1998,7 @@
         <v/>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
@@ -1927,7 +2012,7 @@
     </row>
     <row r="23" spans="2:37" ht="30">
       <c r="B23" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -1958,7 +2043,7 @@
         <v>gcloud info</v>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -1968,7 +2053,7 @@
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AK23" s="1"/>
     </row>
@@ -2003,7 +2088,7 @@
         <v/>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
@@ -2046,7 +2131,7 @@
         <v/>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
@@ -2089,7 +2174,7 @@
         <v/>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
@@ -2132,7 +2217,7 @@
         <v/>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -2146,9 +2231,7 @@
     </row>
     <row r="28" spans="2:37" outlineLevel="1">
       <c r="B28" s="10"/>
-      <c r="C28" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="C28" s="15"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
@@ -2174,11 +2257,10 @@
       <c r="Z28" s="17"/>
       <c r="AA28" s="8" t="str">
         <f t="shared" ref="AA28:AA31" ca="1" si="10">IFERROR(OFFSET(A28,0,MATCH("",B28:Z28,-1)),"")</f>
-        <v xml:space="preserve">
-</v>
+        <v/>
       </c>
       <c r="AB28" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
@@ -2192,7 +2274,9 @@
     </row>
     <row r="29" spans="2:37" outlineLevel="1">
       <c r="B29" s="12"/>
-      <c r="C29" s="15"/>
+      <c r="C29" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -2218,10 +2302,11 @@
       <c r="Z29" s="17"/>
       <c r="AA29" s="8" t="str">
         <f t="shared" ref="AA29:AA30" ca="1" si="11">IFERROR(OFFSET(A29,0,MATCH("",B29:Z29,-1)),"")</f>
-        <v/>
+        <v xml:space="preserve">
+</v>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
@@ -2235,9 +2320,7 @@
     </row>
     <row r="30" spans="2:37" outlineLevel="1">
       <c r="B30" s="12"/>
-      <c r="C30" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="C30" s="15"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -2263,11 +2346,10 @@
       <c r="Z30" s="17"/>
       <c r="AA30" s="8" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">
-</v>
+        <v/>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>
@@ -2310,7 +2392,7 @@
         <v/>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
@@ -2325,7 +2407,7 @@
     <row r="32" spans="2:37" outlineLevel="1">
       <c r="B32" s="12"/>
       <c r="C32" s="15" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -2356,7 +2438,7 @@
 </v>
       </c>
       <c r="AB32" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
@@ -2399,7 +2481,7 @@
         <v/>
       </c>
       <c r="AB33" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
@@ -2442,7 +2524,7 @@
         <v/>
       </c>
       <c r="AB34" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
@@ -2485,7 +2567,7 @@
         <v/>
       </c>
       <c r="AB35" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC35" s="2"/>
       <c r="AD35" s="2"/>
@@ -2528,7 +2610,7 @@
         <v/>
       </c>
       <c r="AB36" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC36" s="2"/>
       <c r="AD36" s="2"/>
@@ -2571,7 +2653,7 @@
         <v/>
       </c>
       <c r="AB37" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -2614,7 +2696,7 @@
         <v/>
       </c>
       <c r="AB38" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC38" s="2"/>
       <c r="AD38" s="2"/>
@@ -2657,7 +2739,7 @@
         <v/>
       </c>
       <c r="AB39" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC39" s="2"/>
       <c r="AD39" s="2"/>
@@ -2700,7 +2782,7 @@
         <v/>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC40" s="2"/>
       <c r="AD40" s="2"/>
@@ -2743,7 +2825,7 @@
         <v/>
       </c>
       <c r="AB41" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" s="2"/>
@@ -2786,7 +2868,7 @@
         <v/>
       </c>
       <c r="AB42" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC42" s="2"/>
       <c r="AD42" s="2"/>
@@ -2829,7 +2911,7 @@
         <v/>
       </c>
       <c r="AB43" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC43" s="2"/>
       <c r="AD43" s="2"/>
@@ -2872,7 +2954,7 @@
         <v/>
       </c>
       <c r="AB44" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" s="2"/>
@@ -2915,7 +2997,7 @@
         <v/>
       </c>
       <c r="AB45" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" s="2"/>
@@ -2958,7 +3040,7 @@
         <v/>
       </c>
       <c r="AB46" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC46" s="2"/>
       <c r="AD46" s="2"/>
@@ -3001,7 +3083,7 @@
         <v/>
       </c>
       <c r="AB47" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" s="2"/>
@@ -3044,7 +3126,7 @@
         <v/>
       </c>
       <c r="AB48" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" s="2"/>
@@ -3087,7 +3169,7 @@
         <v/>
       </c>
       <c r="AB49" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" s="2"/>
@@ -3130,7 +3212,7 @@
         <v/>
       </c>
       <c r="AB50" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" s="2"/>
@@ -3173,7 +3255,7 @@
         <v/>
       </c>
       <c r="AB51" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" s="2"/>
@@ -3216,7 +3298,7 @@
         <v/>
       </c>
       <c r="AB52" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC52" s="2"/>
       <c r="AD52" s="2"/>
@@ -3259,7 +3341,7 @@
         <v/>
       </c>
       <c r="AB53" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC53" s="2"/>
       <c r="AD53" s="2"/>
@@ -3302,7 +3384,7 @@
         <v/>
       </c>
       <c r="AB54" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" s="2"/>
@@ -3345,7 +3427,7 @@
         <v/>
       </c>
       <c r="AB55" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC55" s="2"/>
       <c r="AD55" s="2"/>
@@ -3388,7 +3470,7 @@
         <v/>
       </c>
       <c r="AB56" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC56" s="2"/>
       <c r="AD56" s="2"/>
@@ -3431,7 +3513,7 @@
         <v/>
       </c>
       <c r="AB57" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
@@ -3474,7 +3556,7 @@
         <v/>
       </c>
       <c r="AB58" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC58" s="2"/>
       <c r="AD58" s="2"/>
@@ -3517,7 +3599,7 @@
         <v/>
       </c>
       <c r="AB59" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC59" s="2"/>
       <c r="AD59" s="2"/>
@@ -3560,7 +3642,7 @@
         <v/>
       </c>
       <c r="AB60" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC60" s="2"/>
       <c r="AD60" s="2"/>
@@ -3648,26 +3730,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AG34"/>
+  <dimension ref="B1:AK47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:Z31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="26" width="2.85546875" customWidth="1"/>
-    <col min="27" max="27" width="50" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="47.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="20.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="44.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="65.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="46" customWidth="1"/>
-    <col min="34" max="34" width="68.140625" customWidth="1"/>
+    <col min="27" max="27" width="15" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="19.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="13.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="17" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="24.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="14.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="28.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="46" customWidth="1"/>
+    <col min="38" max="38" width="68.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33">
+    <row r="1" spans="2:37">
       <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
@@ -3696,7 +3782,7 @@
       <c r="Y1" s="21"/>
       <c r="Z1" s="21"/>
       <c r="AA1" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB1" s="18" t="s">
         <v>2</v>
@@ -3704,17 +3790,21 @@
       <c r="AC1" s="19"/>
       <c r="AD1" s="19"/>
       <c r="AE1" s="20"/>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AK1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:33">
+    <row r="2" spans="2:37">
       <c r="B2" s="15" t="str">
-        <f>"gsutil mb gs://"&amp;AC2</f>
-        <v>gsutil mb gs://unique-name-1</v>
+        <f>"gsutil cp "&amp;AC2&amp;" gs://"&amp;AE2</f>
+        <v>gsutil cp test.dat gs://unique-name-1</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -3742,25 +3832,32 @@
       <c r="Z2" s="17"/>
       <c r="AA2" s="8" t="str">
         <f t="shared" ref="AA2" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
-        <v>gsutil mb gs://unique-name-1</v>
+        <v>gsutil cp test.dat gs://unique-name-1</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG2" s="1"/>
-    </row>
-    <row r="3" spans="2:33">
-      <c r="B3" s="15" t="str">
-        <f>"gsutil cp "&amp;AC3&amp;" gs://"&amp;AE3</f>
-        <v>gsutil cp test.dat gs://unique-name-1</v>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK2" s="1"/>
+    </row>
+    <row r="3" spans="2:37">
+      <c r="B3" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -3787,29 +3884,30 @@
       <c r="Y3" s="16"/>
       <c r="Z3" s="17"/>
       <c r="AA3" s="8" t="str">
-        <f t="shared" ref="AA3" ca="1" si="1">IFERROR(OFFSET(A3,0,MATCH("",B3:Z3,-1)),"")</f>
-        <v>gsutil cp test.dat gs://unique-name-1</v>
+        <f t="shared" ref="AA3:AA33" ca="1" si="1">IFERROR(OFFSET(A3,0,MATCH("",B3:Z3,-1)),"")</f>
+        <v>gsutil mb</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG3" s="1"/>
-    </row>
-    <row r="4" spans="2:33">
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
+      <c r="AK3" s="1"/>
+    </row>
+    <row r="4" spans="2:37" outlineLevel="1">
+      <c r="B4" s="10"/>
+      <c r="C4" s="16" t="str">
+        <f>B$3&amp;" gs://"&amp;AC4</f>
+        <v>gsutil mb gs://unique-name-1</v>
+      </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
@@ -3834,23 +3932,29 @@
       <c r="Y4" s="16"/>
       <c r="Z4" s="17"/>
       <c r="AA4" s="8" t="str">
-        <f t="shared" ref="AA4:AA20" ca="1" si="2">IFERROR(OFFSET(A4,0,MATCH("",B4:Z4,-1)),"")</f>
-        <v/>
+        <f t="shared" ca="1" si="1"/>
+        <v>gsutil mb gs://unique-name-1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC4" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-    </row>
-    <row r="5" spans="2:33" outlineLevel="1">
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK4" s="1"/>
+    </row>
+    <row r="5" spans="2:37" outlineLevel="1">
       <c r="B5" s="10"/>
-      <c r="C5" s="16" t="s">
-        <v>15</v>
-      </c>
+      <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -3875,23 +3979,25 @@
       <c r="Y5" s="16"/>
       <c r="Z5" s="17"/>
       <c r="AA5" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>gsutil mb gs://unique-name</v>
+        <f t="shared" ca="1" si="1"/>
+        <v/>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-    </row>
-    <row r="6" spans="2:33" outlineLevel="1">
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+    </row>
+    <row r="6" spans="2:37" outlineLevel="1">
       <c r="B6" s="10"/>
-      <c r="C6" s="16" t="s">
-        <v>16</v>
-      </c>
+      <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -3916,19 +4022,23 @@
       <c r="Y6" s="16"/>
       <c r="Z6" s="17"/>
       <c r="AA6" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>gsutil cp test.dat gs://unique-name</v>
+        <f t="shared" ca="1" si="1"/>
+        <v/>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-    </row>
-    <row r="7" spans="2:33" outlineLevel="1">
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+    </row>
+    <row r="7" spans="2:37" outlineLevel="1">
       <c r="B7" s="10"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -3955,20 +4065,26 @@
       <c r="Y7" s="16"/>
       <c r="Z7" s="17"/>
       <c r="AA7" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-    </row>
-    <row r="8" spans="2:33" outlineLevel="1">
-      <c r="B8" s="10"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+    </row>
+    <row r="8" spans="2:37">
+      <c r="B8" s="15" t="s">
+        <v>58</v>
+      </c>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -3994,23 +4110,30 @@
       <c r="Y8" s="16"/>
       <c r="Z8" s="17"/>
       <c r="AA8" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ref="AA8:AA9" ca="1" si="2">IFERROR(OFFSET(A8,0,MATCH("",B8:Z8,-1)),"")</f>
+        <v>gsutil cp</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-    </row>
-    <row r="9" spans="2:33" collapsed="1">
-      <c r="B9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="16"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK8" s="1"/>
+    </row>
+    <row r="9" spans="2:37" outlineLevel="1">
+      <c r="B9" s="12"/>
+      <c r="C9" s="16" t="str">
+        <f>B$8&amp;" "&amp;IF(ISBLANK(AC9),"","gs://"&amp;AC9&amp;"/")&amp;AE9&amp;" "&amp;IF(ISBLANK(AG9),"","gs://"&amp;AG9&amp;"/")&amp;AI9</f>
+        <v>gsutil cp gs://ioso-bucket/ada.jpg gs://ioso-bucket/image-folder/</v>
+      </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -4036,21 +4159,43 @@
       <c r="Z9" s="17"/>
       <c r="AA9" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">
-</v>
+        <v>gsutil cp gs://ioso-bucket/ada.jpg gs://ioso-bucket/image-folder/</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-    </row>
-    <row r="10" spans="2:33">
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK9" s="1"/>
+    </row>
+    <row r="10" spans="2:37" outlineLevel="1">
+      <c r="B10" s="12"/>
+      <c r="C10" s="16" t="str">
+        <f>B$8&amp;" -r "&amp;IF(ISBLANK(AC10),"","gs://"&amp;AC10&amp;"/")&amp;AE10&amp;" "&amp;IF(ISBLANK(AG10),"","gs://"&amp;AG10&amp;"/")&amp;AI10</f>
+        <v>gsutil cp -r gs://ioso-bucket/ada.jpg .</v>
+      </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -4075,20 +4220,40 @@
       <c r="Y10" s="16"/>
       <c r="Z10" s="17"/>
       <c r="AA10" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ref="AA10:AA12" ca="1" si="3">IFERROR(OFFSET(A10,0,MATCH("",B10:Z10,-1)),"")</f>
+        <v>gsutil cp -r gs://ioso-bucket/ada.jpg .</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-    </row>
-    <row r="11" spans="2:33" outlineLevel="1">
-      <c r="B11" s="10"/>
+        <v>60</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK10" s="1"/>
+    </row>
+    <row r="11" spans="2:37">
+      <c r="B11" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -4114,21 +4279,30 @@
       <c r="Y11" s="16"/>
       <c r="Z11" s="17"/>
       <c r="AA11" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>gsutil ls</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-    </row>
-    <row r="12" spans="2:33" outlineLevel="1">
-      <c r="B12" s="10"/>
-      <c r="C12" s="16"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK11" s="1"/>
+    </row>
+    <row r="12" spans="2:37" outlineLevel="1">
+      <c r="B12" s="12"/>
+      <c r="C12" s="16" t="str">
+        <f>B$11&amp;" gs://"&amp;AC12&amp;"/"&amp;AE12</f>
+        <v>gsutil ls gs://ioso-bucket/image-dir</v>
+      </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -4153,21 +4327,36 @@
       <c r="Y12" s="16"/>
       <c r="Z12" s="17"/>
       <c r="AA12" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="3"/>
+        <v>gsutil ls gs://ioso-bucket/image-dir</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-    </row>
-    <row r="13" spans="2:33" outlineLevel="2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK12" s="1"/>
+    </row>
+    <row r="13" spans="2:37" outlineLevel="1">
+      <c r="B13" s="12"/>
+      <c r="C13" s="16" t="str">
+        <f>B$11&amp;" -l gs://"&amp;AC13&amp;"/"&amp;AE13</f>
+        <v>gsutil ls -l gs://ioso-bucket/image-dir/ada.jpg</v>
+      </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -4192,21 +4381,35 @@
       <c r="Y13" s="16"/>
       <c r="Z13" s="17"/>
       <c r="AA13" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ref="AA13:AA15" ca="1" si="4">IFERROR(OFFSET(A13,0,MATCH("",B13:Z13,-1)),"")</f>
+        <v>gsutil ls -l gs://ioso-bucket/image-dir/ada.jpg</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-    </row>
-    <row r="14" spans="2:33" outlineLevel="2" collapsed="1">
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="AC13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK13" s="1"/>
+    </row>
+    <row r="14" spans="2:37">
+      <c r="B14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -4231,22 +4434,31 @@
       <c r="Y14" s="16"/>
       <c r="Z14" s="17"/>
       <c r="AA14" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>gsutil rm</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
-      <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
-    </row>
-    <row r="15" spans="2:33" hidden="1" outlineLevel="3">
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK14" s="1"/>
+    </row>
+    <row r="15" spans="2:37" outlineLevel="1">
+      <c r="B15" s="12"/>
+      <c r="C15" s="16" t="str">
+        <f>B$14&amp;" gs://"&amp;AC15&amp;"/"&amp;AE15</f>
+        <v>gsutil rm gs://ioso-bucket/ada.jpg</v>
+      </c>
+      <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -4270,22 +4482,34 @@
       <c r="Y15" s="16"/>
       <c r="Z15" s="17"/>
       <c r="AA15" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>gsutil rm gs://ioso-bucket/ada.jpg</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
-    </row>
-    <row r="16" spans="2:33" hidden="1" outlineLevel="3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK15" s="1"/>
+    </row>
+    <row r="16" spans="2:37" outlineLevel="1">
+      <c r="B16" s="12"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -4309,23 +4533,35 @@
       <c r="Y16" s="16"/>
       <c r="Z16" s="17"/>
       <c r="AA16" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="AA16:AA21" ca="1" si="5">IFERROR(OFFSET(A16,0,MATCH("",B16:Z16,-1)),"")</f>
         <v/>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-    </row>
-    <row r="17" spans="2:33" hidden="1" outlineLevel="4">
-      <c r="B17" s="10"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+    </row>
+    <row r="17" spans="2:37" ht="30">
+      <c r="B17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
@@ -4348,23 +4584,32 @@
       <c r="Y17" s="16"/>
       <c r="Z17" s="17"/>
       <c r="AA17" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="5"/>
+        <v>gsutil acl</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
-      <c r="AF17" s="1"/>
-      <c r="AG17" s="1"/>
-    </row>
-    <row r="18" spans="2:33" hidden="1" outlineLevel="4">
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK17" s="1"/>
+    </row>
+    <row r="18" spans="2:37" outlineLevel="1">
+      <c r="B18" s="12"/>
+      <c r="C18" s="16" t="str">
+        <f>B$17&amp;" ch"</f>
+        <v>gsutil acl ch</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
@@ -4387,24 +4632,31 @@
       <c r="Y18" s="16"/>
       <c r="Z18" s="17"/>
       <c r="AA18" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="5"/>
+        <v>gsutil acl ch</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
-      <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
-    </row>
-    <row r="19" spans="2:33" hidden="1" outlineLevel="5">
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+    </row>
+    <row r="19" spans="2:37" ht="30" outlineLevel="2">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="16" t="str">
+        <f>C$18&amp;" -u AllUsers:R gs://"&amp;AC19&amp;"/"&amp;AE19</f>
+        <v>gsutil acl ch -u AllUsers:R gs://ioso-bucket/ada.jpg</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -4426,24 +4678,39 @@
       <c r="Y19" s="16"/>
       <c r="Z19" s="17"/>
       <c r="AA19" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ca="1" si="5"/>
+        <v>gsutil acl ch -u AllUsers:R gs://ioso-bucket/ada.jpg</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
-    </row>
-    <row r="20" spans="2:33" hidden="1" outlineLevel="5">
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK19" s="1"/>
+    </row>
+    <row r="20" spans="2:37" ht="30" outlineLevel="2">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="16" t="str">
+        <f>C$18&amp;" -d AllUsers gs://"&amp;AC20&amp;"/"&amp;AE20</f>
+        <v>gsutil acl ch -d AllUsers gs://ioso-bucket/ada.jpg</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
@@ -4465,25 +4732,37 @@
       <c r="Y20" s="16"/>
       <c r="Z20" s="17"/>
       <c r="AA20" s="8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
+        <f t="shared" ref="AA20" ca="1" si="6">IFERROR(OFFSET(A20,0,MATCH("",B20:Z20,-1)),"")</f>
+        <v>gsutil acl ch -d AllUsers gs://ioso-bucket/ada.jpg</v>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="1"/>
-      <c r="AG20" s="1"/>
-    </row>
-    <row r="21" spans="2:33" hidden="1" outlineLevel="6">
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK20" s="1"/>
+    </row>
+    <row r="21" spans="2:37" outlineLevel="1">
+      <c r="B21" s="12"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
@@ -4504,25 +4783,29 @@
       <c r="Y21" s="16"/>
       <c r="Z21" s="17"/>
       <c r="AA21" s="8" t="str">
-        <f t="shared" ref="AA21:AA31" ca="1" si="3">IFERROR(OFFSET(A21,0,MATCH("",B21:Z21,-1)),"")</f>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
-      <c r="AF21" s="1"/>
-      <c r="AG21" s="1"/>
-    </row>
-    <row r="22" spans="2:33" hidden="1" outlineLevel="6">
-      <c r="B22" s="10"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+    </row>
+    <row r="22" spans="2:37" collapsed="1">
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
@@ -4543,26 +4826,30 @@
       <c r="Y22" s="16"/>
       <c r="Z22" s="17"/>
       <c r="AA22" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
-      <c r="AF22" s="1"/>
-      <c r="AG22" s="1"/>
-    </row>
-    <row r="23" spans="2:33" hidden="1" outlineLevel="7">
-      <c r="B23" s="10"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+    </row>
+    <row r="23" spans="2:37">
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
@@ -4582,26 +4869,30 @@
       <c r="Y23" s="16"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
-      <c r="AF23" s="1"/>
-      <c r="AG23" s="1"/>
-    </row>
-    <row r="24" spans="2:33" hidden="1" outlineLevel="7">
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+    </row>
+    <row r="24" spans="2:37" outlineLevel="1">
       <c r="B24" s="10"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
@@ -4621,25 +4912,29 @@
       <c r="Y24" s="16"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
       <c r="AE24" s="2"/>
-      <c r="AF24" s="1"/>
-      <c r="AG24" s="1"/>
-    </row>
-    <row r="25" spans="2:33" hidden="1" outlineLevel="6">
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+    </row>
+    <row r="25" spans="2:37" outlineLevel="1">
       <c r="B25" s="10"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
@@ -4660,24 +4955,28 @@
       <c r="Y25" s="16"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
-      <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
-    </row>
-    <row r="26" spans="2:33" hidden="1" outlineLevel="5">
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+    </row>
+    <row r="26" spans="2:37" outlineLevel="2">
       <c r="B26" s="10"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
@@ -4699,23 +4998,27 @@
       <c r="Y26" s="16"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
-      <c r="AF26" s="1"/>
-      <c r="AG26" s="1"/>
-    </row>
-    <row r="27" spans="2:33" hidden="1" outlineLevel="4">
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+    </row>
+    <row r="27" spans="2:37" outlineLevel="2" collapsed="1">
       <c r="B27" s="10"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
@@ -4738,19 +5041,23 @@
       <c r="Y27" s="16"/>
       <c r="Z27" s="17"/>
       <c r="AA27" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
-      <c r="AF27" s="1"/>
-      <c r="AG27" s="1"/>
-    </row>
-    <row r="28" spans="2:33" hidden="1" outlineLevel="3">
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+    </row>
+    <row r="28" spans="2:37" hidden="1" outlineLevel="3">
       <c r="B28" s="10"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -4777,22 +5084,26 @@
       <c r="Y28" s="16"/>
       <c r="Z28" s="17"/>
       <c r="AA28" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB28" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-    </row>
-    <row r="29" spans="2:33" hidden="1" outlineLevel="3">
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+    </row>
+    <row r="29" spans="2:37" hidden="1" outlineLevel="3">
       <c r="B29" s="10"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -4816,23 +5127,27 @@
       <c r="Y29" s="16"/>
       <c r="Z29" s="17"/>
       <c r="AA29" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
-      <c r="AF29" s="1"/>
-      <c r="AG29" s="1"/>
-    </row>
-    <row r="30" spans="2:33" outlineLevel="2">
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+    </row>
+    <row r="30" spans="2:37" hidden="1" outlineLevel="4">
       <c r="B30" s="10"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
@@ -4855,23 +5170,27 @@
       <c r="Y30" s="16"/>
       <c r="Z30" s="17"/>
       <c r="AA30" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
-      <c r="AF30" s="1"/>
-      <c r="AG30" s="1"/>
-    </row>
-    <row r="31" spans="2:33">
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+    </row>
+    <row r="31" spans="2:37" hidden="1" outlineLevel="4">
+      <c r="B31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
@@ -4894,53 +5213,629 @@
       <c r="Y31" s="16"/>
       <c r="Z31" s="17"/>
       <c r="AA31" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
-    </row>
-    <row r="34" ht="15" customHeight="1"/>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="2"/>
+      <c r="AJ31" s="1"/>
+      <c r="AK31" s="1"/>
+    </row>
+    <row r="32" spans="2:37" hidden="1" outlineLevel="5">
+      <c r="B32" s="10"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="16"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="AB32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="1"/>
+      <c r="AK32" s="1"/>
+    </row>
+    <row r="33" spans="2:37" hidden="1" outlineLevel="5">
+      <c r="B33" s="10"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="1"/>
+      <c r="AK33" s="1"/>
+    </row>
+    <row r="34" spans="2:37" hidden="1" outlineLevel="6">
+      <c r="B34" s="10"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
+      <c r="Y34" s="16"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="8" t="str">
+        <f t="shared" ref="AA34:AA44" ca="1" si="7">IFERROR(OFFSET(A34,0,MATCH("",B34:Z34,-1)),"")</f>
+        <v/>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
+      <c r="AJ34" s="1"/>
+      <c r="AK34" s="1"/>
+    </row>
+    <row r="35" spans="2:37" hidden="1" outlineLevel="6">
+      <c r="B35" s="10"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2"/>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2"/>
+      <c r="AI35" s="2"/>
+      <c r="AJ35" s="1"/>
+      <c r="AK35" s="1"/>
+    </row>
+    <row r="36" spans="2:37" hidden="1" outlineLevel="7">
+      <c r="B36" s="10"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="2"/>
+      <c r="AJ36" s="1"/>
+      <c r="AK36" s="1"/>
+    </row>
+    <row r="37" spans="2:37" hidden="1" outlineLevel="7">
+      <c r="B37" s="10"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
+      <c r="Y37" s="16"/>
+      <c r="Z37" s="17"/>
+      <c r="AA37" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="2"/>
+      <c r="AG37" s="2"/>
+      <c r="AH37" s="2"/>
+      <c r="AI37" s="2"/>
+      <c r="AJ37" s="1"/>
+      <c r="AK37" s="1"/>
+    </row>
+    <row r="38" spans="2:37" hidden="1" outlineLevel="6">
+      <c r="B38" s="10"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="16"/>
+      <c r="Z38" s="17"/>
+      <c r="AA38" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AI38" s="2"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+    </row>
+    <row r="39" spans="2:37" hidden="1" outlineLevel="5">
+      <c r="B39" s="10"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="17"/>
+      <c r="AA39" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AI39" s="2"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+    </row>
+    <row r="40" spans="2:37" hidden="1" outlineLevel="4">
+      <c r="B40" s="10"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="16"/>
+      <c r="Y40" s="16"/>
+      <c r="Z40" s="17"/>
+      <c r="AA40" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AI40" s="2"/>
+      <c r="AJ40" s="1"/>
+      <c r="AK40" s="1"/>
+    </row>
+    <row r="41" spans="2:37" hidden="1" outlineLevel="3">
+      <c r="B41" s="10"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="17"/>
+      <c r="AA41" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+      <c r="AG41" s="2"/>
+      <c r="AH41" s="2"/>
+      <c r="AI41" s="2"/>
+      <c r="AJ41" s="1"/>
+      <c r="AK41" s="1"/>
+    </row>
+    <row r="42" spans="2:37" hidden="1" outlineLevel="3">
+      <c r="B42" s="10"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="16"/>
+      <c r="X42" s="16"/>
+      <c r="Y42" s="16"/>
+      <c r="Z42" s="17"/>
+      <c r="AA42" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AI42" s="2"/>
+      <c r="AJ42" s="1"/>
+      <c r="AK42" s="1"/>
+    </row>
+    <row r="43" spans="2:37" outlineLevel="2">
+      <c r="B43" s="10"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="17"/>
+      <c r="AA43" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="2"/>
+      <c r="AI43" s="2"/>
+      <c r="AJ43" s="1"/>
+      <c r="AK43" s="1"/>
+    </row>
+    <row r="44" spans="2:37">
+      <c r="B44" s="15"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="16"/>
+      <c r="X44" s="16"/>
+      <c r="Y44" s="16"/>
+      <c r="Z44" s="17"/>
+      <c r="AA44" s="8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v/>
+      </c>
+      <c r="AB44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="2"/>
+      <c r="AI44" s="2"/>
+      <c r="AJ44" s="1"/>
+      <c r="AK44" s="1"/>
+    </row>
+    <row r="47" spans="2:37" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="45">
+    <mergeCell ref="C18:Z18"/>
+    <mergeCell ref="D19:Z19"/>
+    <mergeCell ref="D20:Z20"/>
     <mergeCell ref="B1:Z1"/>
     <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="B4:Z4"/>
+    <mergeCell ref="B8:Z8"/>
+    <mergeCell ref="C9:Z9"/>
+    <mergeCell ref="C10:Z10"/>
+    <mergeCell ref="B3:Z3"/>
+    <mergeCell ref="C4:Z4"/>
     <mergeCell ref="C5:Z5"/>
     <mergeCell ref="C6:Z6"/>
+    <mergeCell ref="B2:Z2"/>
+    <mergeCell ref="G32:Z32"/>
     <mergeCell ref="C7:Z7"/>
-    <mergeCell ref="B2:Z2"/>
-    <mergeCell ref="B3:Z3"/>
-    <mergeCell ref="G19:Z19"/>
-    <mergeCell ref="C8:Z8"/>
-    <mergeCell ref="B9:Z9"/>
-    <mergeCell ref="B10:Z10"/>
-    <mergeCell ref="C11:Z11"/>
+    <mergeCell ref="B22:Z22"/>
+    <mergeCell ref="B23:Z23"/>
+    <mergeCell ref="C24:Z24"/>
+    <mergeCell ref="C25:Z25"/>
+    <mergeCell ref="D26:Z26"/>
+    <mergeCell ref="B11:Z11"/>
     <mergeCell ref="C12:Z12"/>
-    <mergeCell ref="D13:Z13"/>
-    <mergeCell ref="D14:Z14"/>
-    <mergeCell ref="E15:Z15"/>
-    <mergeCell ref="E16:Z16"/>
-    <mergeCell ref="F17:Z17"/>
-    <mergeCell ref="F18:Z18"/>
-    <mergeCell ref="B31:Z31"/>
-    <mergeCell ref="G20:Z20"/>
-    <mergeCell ref="H21:Z21"/>
-    <mergeCell ref="H22:Z22"/>
-    <mergeCell ref="I23:Z23"/>
-    <mergeCell ref="I24:Z24"/>
-    <mergeCell ref="H25:Z25"/>
-    <mergeCell ref="G26:Z26"/>
-    <mergeCell ref="F27:Z27"/>
+    <mergeCell ref="C13:Z13"/>
+    <mergeCell ref="B14:Z14"/>
+    <mergeCell ref="C15:Z15"/>
+    <mergeCell ref="C16:Z16"/>
+    <mergeCell ref="B17:Z17"/>
+    <mergeCell ref="C21:Z21"/>
+    <mergeCell ref="D27:Z27"/>
     <mergeCell ref="E28:Z28"/>
-    <mergeCell ref="D29:Z29"/>
-    <mergeCell ref="C30:Z30"/>
+    <mergeCell ref="E29:Z29"/>
+    <mergeCell ref="F30:Z30"/>
+    <mergeCell ref="F31:Z31"/>
+    <mergeCell ref="B44:Z44"/>
+    <mergeCell ref="G33:Z33"/>
+    <mergeCell ref="H34:Z34"/>
+    <mergeCell ref="H35:Z35"/>
+    <mergeCell ref="I36:Z36"/>
+    <mergeCell ref="I37:Z37"/>
+    <mergeCell ref="H38:Z38"/>
+    <mergeCell ref="G39:Z39"/>
+    <mergeCell ref="F40:Z40"/>
+    <mergeCell ref="E41:Z41"/>
+    <mergeCell ref="D42:Z42"/>
+    <mergeCell ref="C43:Z43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5000,7 +5895,7 @@
       <c r="Y1" s="21"/>
       <c r="Z1" s="21"/>
       <c r="AA1" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB1" s="18" t="s">
         <v>2</v>
@@ -5017,7 +5912,7 @@
     </row>
     <row r="2" spans="2:33" ht="219" customHeight="1">
       <c r="B2" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -5048,21 +5943,21 @@
         <v/>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AG2" s="1"/>
     </row>
     <row r="3" spans="2:33" collapsed="1">
       <c r="B3" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -5093,13 +5988,13 @@
         <v>ls -l /dev/disk/by-id/</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG3" s="1"/>
     </row>
@@ -5137,15 +6032,15 @@
         <v>sudo mkdir /mnt/mydisk</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG4" s="1"/>
     </row>
@@ -5183,15 +6078,15 @@
         <v>sudo mkfs.ext4 -F -E lazy_itable_init=0,lazy_journal_init=0,discard /dev/disk/by-id/scsi-0Google_PersistentDisk_persistent-disk-1</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG5" s="1"/>
     </row>
@@ -5229,19 +6124,19 @@
         <v>sudo mount -o discard,defaults /dev/disk/by-id/scsi-0Google_PersistentDisk_persistent-disk-1 /mnt/mydisk</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AC6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF6" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="AG6" s="1"/>
     </row>
@@ -5276,7 +6171,7 @@
         <v/>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
@@ -5315,7 +6210,7 @@
         <v/>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
@@ -5354,7 +6249,7 @@
         <v/>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
@@ -5393,7 +6288,7 @@
         <v/>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
@@ -5432,7 +6327,7 @@
         <v/>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
@@ -5471,7 +6366,7 @@
         <v/>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
@@ -5510,7 +6405,7 @@
         <v/>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
@@ -5549,7 +6444,7 @@
         <v/>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
@@ -5588,7 +6483,7 @@
         <v/>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
@@ -5627,7 +6522,7 @@
         <v/>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
@@ -5666,7 +6561,7 @@
         <v/>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
@@ -5705,7 +6600,7 @@
         <v/>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
@@ -5744,7 +6639,7 @@
         <v/>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
@@ -5783,7 +6678,7 @@
         <v/>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
@@ -5822,7 +6717,7 @@
         <v/>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
@@ -5861,7 +6756,7 @@
         <v/>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
@@ -5900,7 +6795,7 @@
         <v/>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -5939,7 +6834,7 @@
         <v/>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
@@ -5978,7 +6873,7 @@
         <v/>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
@@ -6017,7 +6912,7 @@
         <v/>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
@@ -6056,7 +6951,7 @@
         <v/>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -6095,7 +6990,7 @@
         <v/>
       </c>
       <c r="AB28" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
@@ -6134,7 +7029,7 @@
         <v/>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
@@ -6173,7 +7068,7 @@
         <v/>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>

</xml_diff>

<commit_message>
Fine tuned some commands.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
@@ -112,6 +112,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="AE32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Must be one of: HTTP, HTTPS, HTTP2, SSL, TCP or UDP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This could be a drop-down since regions are a fixed set.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AG33" authorId="0">
       <text>
         <r>
@@ -125,7 +151,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC45" authorId="0">
+    <comment ref="AE39" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This should be a drop-down since only custom and aute are valid values.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This could be a drop-down since regions are a fixed set.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC50" authorId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC46" authorId="0">
+    <comment ref="AC51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC48" authorId="0">
+    <comment ref="AC53" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="169">
   <si>
     <t>Details</t>
   </si>
@@ -510,15 +562,6 @@
     <t>Lists all instances.</t>
   </si>
   <si>
-    <t>Manages firewall-rules?</t>
-  </si>
-  <si>
-    <t>Port:</t>
-  </si>
-  <si>
-    <t>Creates a firewall? With a rule to enable access on a port?</t>
-  </si>
-  <si>
     <t>nginx-lb</t>
   </si>
   <si>
@@ -546,12 +589,6 @@
     <t>nginx-backend</t>
   </si>
   <si>
-    <t>Manages backend services(?).</t>
-  </si>
-  <si>
-    <t>Creates a backend service(?).</t>
-  </si>
-  <si>
     <t>Creates a basic HTTP(S) health check.</t>
   </si>
   <si>
@@ -610,13 +647,115 @@
   </si>
   <si>
     <t>Forwards traffic to an HTTP proxy.</t>
+  </si>
+  <si>
+    <t>Network name:</t>
+  </si>
+  <si>
+    <t>taw-custom-network</t>
+  </si>
+  <si>
+    <t>Sub-net mode:</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>Creates a network.</t>
+  </si>
+  <si>
+    <t>Manages networks.</t>
+  </si>
+  <si>
+    <t>Manages sub-networks.</t>
+  </si>
+  <si>
+    <t>Creates a sub-network.</t>
+  </si>
+  <si>
+    <t>Subnet name:</t>
+  </si>
+  <si>
+    <t>subnet-us-central</t>
+  </si>
+  <si>
+    <t>IP range:</t>
+  </si>
+  <si>
+    <t>10.0.0.0/16</t>
+  </si>
+  <si>
+    <t>rule name:</t>
+  </si>
+  <si>
+    <t>Source range:</t>
+  </si>
+  <si>
+    <t>Tag:</t>
+  </si>
+  <si>
+    <t>Creates a firewall rule. This enables external access to a port.</t>
+  </si>
+  <si>
+    <t>Manages firewall rules.</t>
+  </si>
+  <si>
+    <t>Allow protocol(:port)</t>
+  </si>
+  <si>
+    <t>us-test-01</t>
+  </si>
+  <si>
+    <t>Subnet:</t>
+  </si>
+  <si>
+    <t>Tags:</t>
+  </si>
+  <si>
+    <t>ssh,http,rules</t>
+  </si>
+  <si>
+    <t>Lists sub-networks.</t>
+  </si>
+  <si>
+    <t>Parent network:</t>
+  </si>
+  <si>
+    <t>nw101-allow-rdp</t>
+  </si>
+  <si>
+    <t>tcp:3389</t>
+  </si>
+  <si>
+    <t>http-basic-check</t>
+  </si>
+  <si>
+    <t>Health-check name:</t>
+  </si>
+  <si>
+    <t>Health-checks:</t>
+  </si>
+  <si>
+    <t>Protocol:</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>Creates a backend service.</t>
+  </si>
+  <si>
+    <t>Manages backend services.</t>
+  </si>
+  <si>
+    <t>Backend services define groups of "tasks" that can receive traffic. Currently, the group of tasks can be one or more Google Compute Engine virtual machine instances grouped together using an instance group. Each backend group has parameters that define the group's capacity (e.g. max CPU utilization, max queries per second, ...). URL maps define which requests are sent to which backend services.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,6 +793,20 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -796,7 +949,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -859,6 +1012,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1169,10 +1328,10 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AM89"/>
+  <dimension ref="B1:AM94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:Z27"/>
+      <selection activeCell="D33" sqref="D33:Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -1180,15 +1339,15 @@
     <col min="1" max="26" width="2.85546875" customWidth="1"/>
     <col min="27" max="27" width="20.5703125" customWidth="1"/>
     <col min="28" max="28" width="13.140625" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="19.7109375" customWidth="1" outlineLevel="1"/>
     <col min="30" max="30" width="16.85546875" customWidth="1" outlineLevel="1"/>
     <col min="31" max="31" width="12.5703125" customWidth="1" outlineLevel="1"/>
     <col min="32" max="32" width="15.42578125" customWidth="1" outlineLevel="1"/>
     <col min="33" max="33" width="14.7109375" customWidth="1" outlineLevel="1"/>
     <col min="34" max="34" width="13.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="13.140625" customWidth="1" outlineLevel="1"/>
     <col min="36" max="36" width="5.140625" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="2" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="5.42578125" customWidth="1" outlineLevel="1"/>
     <col min="38" max="38" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="46" customWidth="1"/>
     <col min="40" max="40" width="68.140625" customWidth="1"/>
@@ -1273,7 +1432,7 @@
       <c r="Y2" s="18"/>
       <c r="Z2" s="19"/>
       <c r="AA2" s="8" t="str">
-        <f t="shared" ref="AA2:AA67" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
+        <f t="shared" ref="AA2:AA72" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
         <v>gcloud compute</v>
       </c>
       <c r="AB2" s="2" t="s">
@@ -1343,12 +1502,12 @@
       </c>
       <c r="AM3" s="1"/>
     </row>
-    <row r="4" spans="2:39" ht="30.75" hidden="1" customHeight="1" outlineLevel="2">
+    <row r="4" spans="2:39" ht="41.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B4" s="10"/>
       <c r="C4" s="9"/>
       <c r="D4" s="25" t="str">
-        <f>C$3&amp;" create "&amp;AC4&amp;IF(ISBLANK(AE4),""," --zone "&amp;AE4)</f>
-        <v>gcloud compute instances create gcp-test-1 --zone us-central1-a</v>
+        <f>C$3&amp;" create "&amp;AC4&amp;IF(ISBLANK(AE4),""," --zone "&amp;AE4)&amp;IF(ISBLANK(AG4),""," --subnet "&amp;AG4)&amp;IF(ISBLANK(AI4),""," --tags "&amp;AI4)</f>
+        <v>gcloud compute instances create us-test-01 --zone us-central1-a --subnet subnet-us-central --tags ssh,http,rules</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
@@ -1374,13 +1533,13 @@
       <c r="Z4" s="27"/>
       <c r="AA4" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>gcloud compute instances create gcp-test-1 --zone us-central1-a</v>
+        <v>gcloud compute instances create us-test-01 --zone us-central1-a --subnet subnet-us-central --tags ssh,http,rules</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="AD4" s="2" t="s">
         <v>11</v>
@@ -1388,10 +1547,18 @@
       <c r="AE4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
+      <c r="AF4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>156</v>
+      </c>
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="1" t="s">
@@ -1549,7 +1716,7 @@
       <c r="Y7" s="18"/>
       <c r="Z7" s="19"/>
       <c r="AA7" s="8" t="str">
-        <f t="shared" ref="AA7:AA38" ca="1" si="3">IFERROR(OFFSET(A7,0,MATCH("",B7:Z7,-1)),"")</f>
+        <f t="shared" ref="AA7:AA43" ca="1" si="3">IFERROR(OFFSET(A7,0,MATCH("",B7:Z7,-1)),"")</f>
         <v>gcloud compute disks</v>
       </c>
       <c r="AB7" s="2" t="s">
@@ -1895,7 +2062,7 @@
       </c>
       <c r="AM13" s="1"/>
     </row>
-    <row r="14" spans="2:39" outlineLevel="1">
+    <row r="14" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B14" s="15"/>
       <c r="C14" s="18" t="str">
         <f>B$2&amp;" target-pools"</f>
@@ -1941,11 +2108,11 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="AM14" s="1"/>
     </row>
-    <row r="15" spans="2:39" outlineLevel="2">
+    <row r="15" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="18" t="str">
@@ -1993,7 +2160,7 @@
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
       <c r="AL15" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AM15" s="1"/>
     </row>
@@ -2205,10 +2372,10 @@
         <v>100</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AE19" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
@@ -2217,7 +2384,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="AM19" s="1"/>
     </row>
@@ -2267,7 +2434,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="AM20" s="1"/>
     </row>
@@ -2317,63 +2484,75 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="1" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="AM21" s="1"/>
     </row>
-    <row r="22" spans="2:39" hidden="1" outlineLevel="2">
+    <row r="22" spans="2:39" ht="50.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="18" t="str">
-        <f>C$21&amp;" create www-firewall --allow tcp:"&amp;AC22</f>
-        <v>gcloud compute firewall-rules create www-firewall --allow tcp:80</v>
-      </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="19"/>
+      <c r="D22" s="25" t="str">
+        <f>C$21&amp;" create "&amp;AC22&amp;" --allow "&amp;AE22&amp;IF(ISBLANK(AG22),""," --network "&amp;AG22)&amp;IF(ISBLANK(AI22),""," --source-ranges "&amp;AI22)&amp;IF(ISBLANK(AK22),""," --target-tags "&amp;AK22)</f>
+        <v>gcloud compute firewall-rules create nw101-allow-rdp --allow tcp:3389 --network taw-custom-network</v>
+      </c>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="27"/>
       <c r="AA22" s="8" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>gcloud compute firewall-rules create www-firewall --allow tcp:80</v>
+        <v>gcloud compute firewall-rules create nw101-allow-rdp --allow tcp:3389 --network taw-custom-network</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC22" s="5">
-        <v>80</v>
-      </c>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="2"/>
-      <c r="AH22" s="2"/>
-      <c r="AI22" s="2"/>
-      <c r="AJ22" s="2"/>
-      <c r="AK22" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="AC22" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG22" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK22" s="5"/>
       <c r="AL22" s="1" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="AM22" s="1"/>
     </row>
-    <row r="23" spans="2:39" ht="30" outlineLevel="1">
+    <row r="23" spans="2:39" ht="30" outlineLevel="1" collapsed="1">
       <c r="B23" s="15"/>
       <c r="C23" s="18" t="str">
         <f>B$2&amp;" forwarding-rules"</f>
@@ -2419,11 +2598,11 @@
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="AM23" s="1"/>
     </row>
-    <row r="24" spans="2:39" outlineLevel="2">
+    <row r="24" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
       <c r="D24" s="25" t="str">
@@ -2469,11 +2648,11 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="AM24" s="1"/>
     </row>
-    <row r="25" spans="2:39" ht="30.75" customHeight="1" outlineLevel="3">
+    <row r="25" spans="2:39" ht="30.75" hidden="1" customHeight="1" outlineLevel="3">
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -2507,10 +2686,10 @@
         <v>gcloud compute forwarding-rules create nginx-lb --target-pool nginx-pool --ports=80 --region us-central1</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AC25" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AD25" s="2" t="s">
         <v>96</v>
@@ -2519,7 +2698,7 @@
         <v>97</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AG25" s="5">
         <v>80</v>
@@ -2533,11 +2712,11 @@
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="AM25" s="1"/>
     </row>
-    <row r="26" spans="2:39" ht="38.25" customHeight="1" outlineLevel="3" collapsed="1">
+    <row r="26" spans="2:39" ht="38.25" hidden="1" customHeight="1" outlineLevel="3" collapsed="1">
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -2571,19 +2750,19 @@
         <v>gcloud compute forwarding-rules create http-content-rule --target-http-proxy http-lb-proxy --ports=80 --global</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="AC26" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AE26" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AF26" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AG26" s="5">
         <v>80</v>
@@ -2595,11 +2774,11 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
       <c r="AL26" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="AM26" s="1"/>
     </row>
-    <row r="27" spans="2:39" outlineLevel="2">
+    <row r="27" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="25"/>
@@ -2644,7 +2823,7 @@
       <c r="AL27" s="1"/>
       <c r="AM27" s="1"/>
     </row>
-    <row r="28" spans="2:39" outlineLevel="2">
+    <row r="28" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B28" s="15"/>
       <c r="C28" s="16"/>
       <c r="D28" s="18" t="str">
@@ -2690,7 +2869,7 @@
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
       <c r="AL28" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AM28" s="1"/>
     </row>
@@ -2740,47 +2919,49 @@
       <c r="AJ29" s="2"/>
       <c r="AK29" s="2"/>
       <c r="AL29" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AM29" s="1"/>
     </row>
-    <row r="30" spans="2:39" hidden="1" outlineLevel="2">
+    <row r="30" spans="2:39" ht="30" hidden="1" outlineLevel="2">
       <c r="B30" s="15"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="18" t="str">
-        <f>C$29&amp;" create http-basic-check"</f>
+      <c r="D30" s="25" t="str">
+        <f>C$29&amp;" create "&amp;AC30</f>
         <v>gcloud compute http-health-checks create http-basic-check</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18"/>
-      <c r="Y30" s="18"/>
-      <c r="Z30" s="19"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+      <c r="U30" s="26"/>
+      <c r="V30" s="26"/>
+      <c r="W30" s="26"/>
+      <c r="X30" s="26"/>
+      <c r="Y30" s="26"/>
+      <c r="Z30" s="27"/>
       <c r="AA30" s="8" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>gcloud compute http-health-checks create http-basic-check</v>
       </c>
-      <c r="AB30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC30" s="2"/>
+      <c r="AB30" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC30" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
@@ -2790,11 +2971,11 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
       <c r="AL30" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="AM30" s="1"/>
     </row>
-    <row r="31" spans="2:39" outlineLevel="1" collapsed="1">
+    <row r="31" spans="2:39" ht="135" outlineLevel="1">
       <c r="B31" s="15"/>
       <c r="C31" s="18" t="str">
         <f>B$2&amp;" backend-services"</f>
@@ -2840,15 +3021,17 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AM31" s="1"/>
-    </row>
-    <row r="32" spans="2:39" ht="45" hidden="1" outlineLevel="2">
+        <v>167</v>
+      </c>
+      <c r="AM31" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="2:39" ht="45" outlineLevel="2">
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
       <c r="D32" s="25" t="str">
-        <f>C$31&amp;" create "&amp;AC32&amp;" --protocol HTTP --http-health-checks http-basic-check --global"</f>
+        <f>C$31&amp;" create "&amp;AC32&amp;" --protocol "&amp;AE32&amp;IF(ISBLANK(AG32),""," --http-health-checks "&amp;AG32)&amp;IF(ISBLANK(AI32)," --global"," --region "&amp;AI32)</f>
         <v>gcloud compute backend-services create nginx-backend --protocol HTTP --http-health-checks http-basic-check --global</v>
       </c>
       <c r="E32" s="26"/>
@@ -2877,26 +3060,36 @@
         <f t="shared" ca="1" si="13"/>
         <v>gcloud compute backend-services create nginx-backend --protocol HTTP --http-health-checks http-basic-check --global</v>
       </c>
-      <c r="AB32" s="2" t="s">
-        <v>116</v>
+      <c r="AB32" s="28" t="s">
+        <v>113</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD32" s="2"/>
-      <c r="AE32" s="2"/>
-      <c r="AF32" s="2"/>
-      <c r="AG32" s="2"/>
-      <c r="AH32" s="2"/>
-      <c r="AI32" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="AD32" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE32" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF32" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="AG32" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI32" s="5"/>
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="1" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="AM32" s="1"/>
     </row>
-    <row r="33" spans="2:39" ht="45" hidden="1" outlineLevel="2">
+    <row r="33" spans="2:39" ht="45" outlineLevel="2">
       <c r="B33" s="15"/>
       <c r="C33" s="16"/>
       <c r="D33" s="25" t="str">
@@ -2929,13 +3122,13 @@
         <f t="shared" ref="AA33:AA35" ca="1" si="14">IFERROR(OFFSET(A33,0,MATCH("",B33:Z33,-1)),"")</f>
         <v>gcloud compute backend-services add-backend nginx-backend --instance-group nginx-group --instance-group-zone us-central1-a --global</v>
       </c>
-      <c r="AB33" s="2" t="s">
-        <v>116</v>
+      <c r="AB33" s="28" t="s">
+        <v>113</v>
       </c>
       <c r="AC33" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD33" s="28" t="s">
         <v>99</v>
       </c>
       <c r="AE33" s="5" t="s">
@@ -2952,7 +3145,7 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
       <c r="AL33" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="AM33" s="1"/>
     </row>
@@ -3002,7 +3195,7 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
       <c r="AL34" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AM34" s="1"/>
     </row>
@@ -3040,16 +3233,16 @@
         <v>gcloud compute url-maps create web-map --default-service nginx-backend</v>
       </c>
       <c r="AB35" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AC35" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AD35" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AE35" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
@@ -3058,7 +3251,7 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
       <c r="AL35" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="AM35" s="1"/>
     </row>
@@ -3108,7 +3301,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
       <c r="AL36" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="AM36" s="1"/>
     </row>
@@ -3146,16 +3339,16 @@
         <v>gcloud compute target-http-proxies create http-lb-proxy --url-map web-map</v>
       </c>
       <c r="AB37" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="AC37" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="AD37" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="AE37" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
@@ -3164,13 +3357,16 @@
       <c r="AJ37" s="2"/>
       <c r="AK37" s="2"/>
       <c r="AL37" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AM37" s="1"/>
     </row>
     <row r="38" spans="2:39" outlineLevel="1" collapsed="1">
-      <c r="B38" s="12"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="18" t="str">
+        <f>B$2&amp;" networks"</f>
+        <v>gcloud compute networks</v>
+      </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
@@ -3195,8 +3391,8 @@
       <c r="Y38" s="18"/>
       <c r="Z38" s="19"/>
       <c r="AA38" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
+        <f t="shared" ref="AA38:AA42" ca="1" si="16">IFERROR(OFFSET(A38,0,MATCH("",B38:Z38,-1)),"")</f>
+        <v>gcloud compute networks</v>
       </c>
       <c r="AB38" s="2" t="s">
         <v>6</v>
@@ -3210,47 +3406,56 @@
       <c r="AI38" s="2"/>
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
-      <c r="AL38" s="1"/>
+      <c r="AL38" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="AM38" s="1"/>
     </row>
-    <row r="39" spans="2:39">
-      <c r="B39" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-      <c r="Y39" s="18"/>
-      <c r="Z39" s="19"/>
+    <row r="39" spans="2:39" ht="30" hidden="1" outlineLevel="2">
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="25" t="str">
+        <f>C$38&amp;" create "&amp;AC39&amp;" --subnet-mode "&amp;AE39</f>
+        <v>gcloud compute networks create taw-custom-network --subnet-mode custom</v>
+      </c>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="27"/>
       <c r="AA39" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>gcloud auth</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>gcloud compute networks create taw-custom-network --subnet-mode custom</v>
       </c>
       <c r="AB39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="AC39" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE39" s="5" t="s">
+        <v>138</v>
+      </c>
       <c r="AF39" s="2"/>
       <c r="AG39" s="2"/>
       <c r="AH39" s="2"/>
@@ -3258,42 +3463,42 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="1" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="AM39" s="1"/>
     </row>
-    <row r="40" spans="2:39" outlineLevel="1">
-      <c r="B40" s="10"/>
-      <c r="C40" s="18" t="str">
-        <f>B39&amp;" list"</f>
-        <v>gcloud auth list</v>
-      </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="18"/>
-      <c r="X40" s="18"/>
-      <c r="Y40" s="18"/>
-      <c r="Z40" s="19"/>
+    <row r="40" spans="2:39" hidden="1" outlineLevel="2">
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="25" t="str">
+        <f>C$38&amp;" subnets"</f>
+        <v>gcloud compute networks subnets</v>
+      </c>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="27"/>
       <c r="AA40" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>gcloud auth list</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>gcloud compute networks subnets</v>
       </c>
       <c r="AB40" s="2" t="s">
         <v>6</v>
@@ -3308,91 +3513,113 @@
       <c r="AJ40" s="2"/>
       <c r="AK40" s="2"/>
       <c r="AL40" s="1" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="AM40" s="1"/>
     </row>
-    <row r="41" spans="2:39" outlineLevel="1">
-      <c r="B41" s="10"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-      <c r="V41" s="18"/>
-      <c r="W41" s="18"/>
-      <c r="X41" s="18"/>
-      <c r="Y41" s="18"/>
-      <c r="Z41" s="19"/>
+    <row r="41" spans="2:39" ht="39.75" hidden="1" customHeight="1" outlineLevel="3">
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="25" t="str">
+        <f>D$40&amp;" create "&amp;AC41&amp;" --network "&amp;AE41&amp;" --region "&amp;AG41&amp;" --range "&amp;AI41</f>
+        <v>gcloud compute networks subnets create subnet-us-central --network taw-custom-network --region us-central1 --range 10.0.0.0/16</v>
+      </c>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="27"/>
       <c r="AA41" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
+        <f t="shared" ca="1" si="16"/>
+        <v>gcloud compute networks subnets create subnet-us-central --network taw-custom-network --region us-central1 --range 10.0.0.0/16</v>
       </c>
       <c r="AB41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="2"/>
-      <c r="AE41" s="2"/>
-      <c r="AF41" s="2"/>
-      <c r="AG41" s="2"/>
-      <c r="AH41" s="2"/>
-      <c r="AI41" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="AC41" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD41" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE41" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG41" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH41" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI41" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="AJ41" s="2"/>
       <c r="AK41" s="2"/>
-      <c r="AL41" s="1"/>
+      <c r="AL41" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="AM41" s="1"/>
     </row>
-    <row r="42" spans="2:39">
-      <c r="B42" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
-      <c r="W42" s="18"/>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="18"/>
-      <c r="Z42" s="19"/>
+    <row r="42" spans="2:39" ht="30" hidden="1" outlineLevel="3" collapsed="1">
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="25" t="str">
+        <f>D$40&amp;" list"&amp;IF(ISBLANK(AC42),""," --network "&amp;AC42)</f>
+        <v>gcloud compute networks subnets list --network taw-custom-network</v>
+      </c>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="U42" s="26"/>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="27"/>
       <c r="AA42" s="8" t="str">
-        <f t="shared" ref="AA42:AA47" ca="1" si="16">IFERROR(OFFSET(A42,0,MATCH("",B42:Z42,-1)),"")</f>
-        <v>gcloud config</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>gcloud compute networks subnets list --network taw-custom-network</v>
       </c>
       <c r="AB42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC42" s="2"/>
+        <v>158</v>
+      </c>
+      <c r="AC42" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="AD42" s="2"/>
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
@@ -3402,16 +3629,13 @@
       <c r="AJ42" s="2"/>
       <c r="AK42" s="2"/>
       <c r="AL42" s="1" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="AM42" s="1"/>
     </row>
-    <row r="43" spans="2:39" outlineLevel="1">
-      <c r="B43" s="10"/>
-      <c r="C43" s="18" t="str">
-        <f>B$42&amp;" list project"</f>
-        <v>gcloud config list project</v>
-      </c>
+    <row r="43" spans="2:39" outlineLevel="1" collapsed="1">
+      <c r="B43" s="12"/>
+      <c r="C43" s="20"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
@@ -3436,8 +3660,8 @@
       <c r="Y43" s="18"/>
       <c r="Z43" s="19"/>
       <c r="AA43" s="8" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v>gcloud config list project</v>
+        <f t="shared" ca="1" si="3"/>
+        <v/>
       </c>
       <c r="AB43" s="2" t="s">
         <v>6</v>
@@ -3451,17 +3675,14 @@
       <c r="AI43" s="2"/>
       <c r="AJ43" s="2"/>
       <c r="AK43" s="2"/>
-      <c r="AL43" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="AL43" s="1"/>
       <c r="AM43" s="1"/>
     </row>
-    <row r="44" spans="2:39" outlineLevel="1">
-      <c r="B44" s="10"/>
-      <c r="C44" s="18" t="str">
-        <f>B$42&amp;" list --all"</f>
-        <v>gcloud config list --all</v>
-      </c>
+    <row r="44" spans="2:39">
+      <c r="B44" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
@@ -3486,8 +3707,8 @@
       <c r="Y44" s="18"/>
       <c r="Z44" s="19"/>
       <c r="AA44" s="8" t="str">
-        <f t="shared" ref="AA44" ca="1" si="17">IFERROR(OFFSET(A44,0,MATCH("",B44:Z44,-1)),"")</f>
-        <v>gcloud config list --all</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>gcloud auth</v>
       </c>
       <c r="AB44" s="2" t="s">
         <v>6</v>
@@ -3502,15 +3723,15 @@
       <c r="AJ44" s="2"/>
       <c r="AK44" s="2"/>
       <c r="AL44" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="AM44" s="1"/>
     </row>
     <row r="45" spans="2:39" outlineLevel="1">
-      <c r="B45" s="15"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="18" t="str">
-        <f>B$42&amp;" set compute/zone "&amp;AC45</f>
-        <v>gcloud config set compute/zone us-central1-a</v>
+        <f>B44&amp;" list"</f>
+        <v>gcloud auth list</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -3536,15 +3757,13 @@
       <c r="Y45" s="18"/>
       <c r="Z45" s="19"/>
       <c r="AA45" s="8" t="str">
-        <f t="shared" ref="AA45" ca="1" si="18">IFERROR(OFFSET(A45,0,MATCH("",B45:Z45,-1)),"")</f>
-        <v>gcloud config set compute/zone us-central1-a</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>gcloud auth list</v>
       </c>
       <c r="AB45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC45" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC45" s="2"/>
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
       <c r="AF45" s="2"/>
@@ -3554,16 +3773,13 @@
       <c r="AJ45" s="2"/>
       <c r="AK45" s="2"/>
       <c r="AL45" s="1" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="AM45" s="1"/>
     </row>
     <row r="46" spans="2:39" outlineLevel="1">
-      <c r="B46" s="15"/>
-      <c r="C46" s="18" t="str">
-        <f>B$42&amp;" set compute/region "&amp;AC46</f>
-        <v>gcloud config set compute/region us-central1</v>
-      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
@@ -3588,15 +3804,13 @@
       <c r="Y46" s="18"/>
       <c r="Z46" s="19"/>
       <c r="AA46" s="8" t="str">
-        <f t="shared" ref="AA46" ca="1" si="19">IFERROR(OFFSET(A46,0,MATCH("",B46:Z46,-1)),"")</f>
-        <v>gcloud config set compute/region us-central1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v/>
       </c>
       <c r="AB46" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AC46" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC46" s="2"/>
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
       <c r="AF46" s="2"/>
@@ -3605,13 +3819,13 @@
       <c r="AI46" s="2"/>
       <c r="AJ46" s="2"/>
       <c r="AK46" s="2"/>
-      <c r="AL46" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="AL46" s="1"/>
       <c r="AM46" s="1"/>
     </row>
-    <row r="47" spans="2:39" outlineLevel="1">
-      <c r="B47" s="10"/>
+    <row r="47" spans="2:39">
+      <c r="B47" s="20" t="s">
+        <v>126</v>
+      </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
@@ -3637,8 +3851,8 @@
       <c r="Y47" s="18"/>
       <c r="Z47" s="19"/>
       <c r="AA47" s="8" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v/>
+        <f t="shared" ref="AA47:AA52" ca="1" si="17">IFERROR(OFFSET(A47,0,MATCH("",B47:Z47,-1)),"")</f>
+        <v>gcloud config</v>
       </c>
       <c r="AB47" s="2" t="s">
         <v>6</v>
@@ -3652,15 +3866,17 @@
       <c r="AI47" s="2"/>
       <c r="AJ47" s="2"/>
       <c r="AK47" s="2"/>
-      <c r="AL47" s="1"/>
+      <c r="AL47" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="AM47" s="1"/>
     </row>
-    <row r="48" spans="2:39">
-      <c r="B48" s="20" t="str">
-        <f>"gcloud help "&amp;AC48</f>
-        <v>gcloud help config</v>
-      </c>
-      <c r="C48" s="18"/>
+    <row r="48" spans="2:39" outlineLevel="1">
+      <c r="B48" s="10"/>
+      <c r="C48" s="18" t="str">
+        <f>B$47&amp;" list project"</f>
+        <v>gcloud config list project</v>
+      </c>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
@@ -3685,15 +3901,13 @@
       <c r="Y48" s="18"/>
       <c r="Z48" s="19"/>
       <c r="AA48" s="8" t="str">
-        <f t="shared" ref="AA48:AA52" ca="1" si="20">IFERROR(OFFSET(A48,0,MATCH("",B48:Z48,-1)),"")</f>
-        <v>gcloud help config</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>gcloud config list project</v>
       </c>
       <c r="AB48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC48" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC48" s="2"/>
       <c r="AD48" s="2"/>
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
@@ -3703,15 +3917,16 @@
       <c r="AJ48" s="2"/>
       <c r="AK48" s="2"/>
       <c r="AL48" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="AM48" s="1"/>
     </row>
-    <row r="49" spans="2:39">
-      <c r="B49" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="18"/>
+    <row r="49" spans="2:39" outlineLevel="1">
+      <c r="B49" s="10"/>
+      <c r="C49" s="18" t="str">
+        <f>B$47&amp;" list --all"</f>
+        <v>gcloud config list --all</v>
+      </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
@@ -3736,8 +3951,8 @@
       <c r="Y49" s="18"/>
       <c r="Z49" s="19"/>
       <c r="AA49" s="8" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v>gcloud init</v>
+        <f t="shared" ref="AA49" ca="1" si="18">IFERROR(OFFSET(A49,0,MATCH("",B49:Z49,-1)),"")</f>
+        <v>gcloud config list --all</v>
       </c>
       <c r="AB49" s="2" t="s">
         <v>6</v>
@@ -3752,15 +3967,15 @@
       <c r="AJ49" s="2"/>
       <c r="AK49" s="2"/>
       <c r="AL49" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AM49" s="1"/>
     </row>
-    <row r="50" spans="2:39" ht="45" outlineLevel="1">
-      <c r="B50" s="10"/>
+    <row r="50" spans="2:39" outlineLevel="1">
+      <c r="B50" s="15"/>
       <c r="C50" s="18" t="str">
-        <f>B49&amp;" --console-only"</f>
-        <v>gcloud init --console-only</v>
+        <f>B$47&amp;" set compute/zone "&amp;AC50</f>
+        <v>gcloud config set compute/zone us-central1-a</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
@@ -3786,13 +4001,15 @@
       <c r="Y50" s="18"/>
       <c r="Z50" s="19"/>
       <c r="AA50" s="8" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v>gcloud init --console-only</v>
+        <f t="shared" ref="AA50" ca="1" si="19">IFERROR(OFFSET(A50,0,MATCH("",B50:Z50,-1)),"")</f>
+        <v>gcloud config set compute/zone us-central1-a</v>
       </c>
       <c r="AB50" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC50" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="AC50" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AD50" s="2"/>
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
@@ -3802,13 +4019,16 @@
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
       <c r="AL50" s="1" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="AM50" s="1"/>
     </row>
     <row r="51" spans="2:39" outlineLevel="1">
-      <c r="B51" s="10"/>
-      <c r="C51" s="18"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="18" t="str">
+        <f>B$47&amp;" set compute/region "&amp;AC51</f>
+        <v>gcloud config set compute/region us-central1</v>
+      </c>
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
@@ -3833,13 +4053,15 @@
       <c r="Y51" s="18"/>
       <c r="Z51" s="19"/>
       <c r="AA51" s="8" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v/>
+        <f t="shared" ref="AA51" ca="1" si="20">IFERROR(OFFSET(A51,0,MATCH("",B51:Z51,-1)),"")</f>
+        <v>gcloud config set compute/region us-central1</v>
       </c>
       <c r="AB51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC51" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="AC51" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="AD51" s="2"/>
       <c r="AE51" s="2"/>
       <c r="AF51" s="2"/>
@@ -3848,13 +4070,13 @@
       <c r="AI51" s="2"/>
       <c r="AJ51" s="2"/>
       <c r="AK51" s="2"/>
-      <c r="AL51" s="1"/>
+      <c r="AL51" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="AM51" s="1"/>
     </row>
-    <row r="52" spans="2:39" ht="30">
-      <c r="B52" s="20" t="s">
-        <v>26</v>
-      </c>
+    <row r="52" spans="2:39" outlineLevel="1">
+      <c r="B52" s="10"/>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
@@ -3880,8 +4102,8 @@
       <c r="Y52" s="18"/>
       <c r="Z52" s="19"/>
       <c r="AA52" s="8" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v>gcloud info</v>
+        <f t="shared" ca="1" si="17"/>
+        <v/>
       </c>
       <c r="AB52" s="2" t="s">
         <v>6</v>
@@ -3895,13 +4117,14 @@
       <c r="AI52" s="2"/>
       <c r="AJ52" s="2"/>
       <c r="AK52" s="2"/>
-      <c r="AL52" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="AL52" s="1"/>
       <c r="AM52" s="1"/>
     </row>
     <row r="53" spans="2:39">
-      <c r="B53" s="20"/>
+      <c r="B53" s="20" t="str">
+        <f>"gcloud help "&amp;AC53</f>
+        <v>gcloud help config</v>
+      </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
@@ -3927,13 +4150,15 @@
       <c r="Y53" s="18"/>
       <c r="Z53" s="19"/>
       <c r="AA53" s="8" t="str">
-        <f t="shared" ref="AA53:AA55" ca="1" si="21">IFERROR(OFFSET(A53,0,MATCH("",B53:Z53,-1)),"")</f>
-        <v/>
+        <f t="shared" ref="AA53:AA57" ca="1" si="21">IFERROR(OFFSET(A53,0,MATCH("",B53:Z53,-1)),"")</f>
+        <v>gcloud help config</v>
       </c>
       <c r="AB53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC53" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="AC53" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="AD53" s="2"/>
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
@@ -3942,12 +4167,16 @@
       <c r="AI53" s="2"/>
       <c r="AJ53" s="2"/>
       <c r="AK53" s="2"/>
-      <c r="AL53" s="1"/>
+      <c r="AL53" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="AM53" s="1"/>
     </row>
-    <row r="54" spans="2:39" outlineLevel="1">
-      <c r="B54" s="10"/>
-      <c r="C54" s="20"/>
+    <row r="54" spans="2:39">
+      <c r="B54" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="18"/>
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
@@ -3973,7 +4202,7 @@
       <c r="Z54" s="19"/>
       <c r="AA54" s="8" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v/>
+        <v>gcloud init</v>
       </c>
       <c r="AB54" s="2" t="s">
         <v>6</v>
@@ -3987,12 +4216,17 @@
       <c r="AI54" s="2"/>
       <c r="AJ54" s="2"/>
       <c r="AK54" s="2"/>
-      <c r="AL54" s="1"/>
+      <c r="AL54" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="AM54" s="1"/>
     </row>
-    <row r="55" spans="2:39" outlineLevel="1">
+    <row r="55" spans="2:39" ht="45" outlineLevel="1">
       <c r="B55" s="10"/>
-      <c r="C55" s="20"/>
+      <c r="C55" s="18" t="str">
+        <f>B54&amp;" --console-only"</f>
+        <v>gcloud init --console-only</v>
+      </c>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
@@ -4018,7 +4252,7 @@
       <c r="Z55" s="19"/>
       <c r="AA55" s="8" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v/>
+        <v>gcloud init --console-only</v>
       </c>
       <c r="AB55" s="2" t="s">
         <v>6</v>
@@ -4032,12 +4266,14 @@
       <c r="AI55" s="2"/>
       <c r="AJ55" s="2"/>
       <c r="AK55" s="2"/>
-      <c r="AL55" s="1"/>
+      <c r="AL55" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="AM55" s="1"/>
     </row>
     <row r="56" spans="2:39" outlineLevel="1">
       <c r="B56" s="10"/>
-      <c r="C56" s="20"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
@@ -4062,7 +4298,7 @@
       <c r="Y56" s="18"/>
       <c r="Z56" s="19"/>
       <c r="AA56" s="8" t="str">
-        <f t="shared" ref="AA56" ca="1" si="22">IFERROR(OFFSET(A56,0,MATCH("",B56:Z56,-1)),"")</f>
+        <f t="shared" ca="1" si="21"/>
         <v/>
       </c>
       <c r="AB56" s="2" t="s">
@@ -4080,9 +4316,11 @@
       <c r="AL56" s="1"/>
       <c r="AM56" s="1"/>
     </row>
-    <row r="57" spans="2:39" outlineLevel="1">
-      <c r="B57" s="10"/>
-      <c r="C57" s="20"/>
+    <row r="57" spans="2:39" ht="30">
+      <c r="B57" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="18"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
@@ -4107,8 +4345,8 @@
       <c r="Y57" s="18"/>
       <c r="Z57" s="19"/>
       <c r="AA57" s="8" t="str">
-        <f t="shared" ref="AA57:AA60" ca="1" si="23">IFERROR(OFFSET(A57,0,MATCH("",B57:Z57,-1)),"")</f>
-        <v/>
+        <f t="shared" ca="1" si="21"/>
+        <v>gcloud info</v>
       </c>
       <c r="AB57" s="2" t="s">
         <v>6</v>
@@ -4122,14 +4360,14 @@
       <c r="AI57" s="2"/>
       <c r="AJ57" s="2"/>
       <c r="AK57" s="2"/>
-      <c r="AL57" s="1"/>
+      <c r="AL57" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="AM57" s="1"/>
     </row>
-    <row r="58" spans="2:39" outlineLevel="1">
-      <c r="B58" s="12"/>
-      <c r="C58" s="20" t="s">
-        <v>13</v>
-      </c>
+    <row r="58" spans="2:39">
+      <c r="B58" s="20"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
@@ -4154,9 +4392,8 @@
       <c r="Y58" s="18"/>
       <c r="Z58" s="19"/>
       <c r="AA58" s="8" t="str">
-        <f t="shared" ref="AA58:AA59" ca="1" si="24">IFERROR(OFFSET(A58,0,MATCH("",B58:Z58,-1)),"")</f>
-        <v xml:space="preserve">
-</v>
+        <f t="shared" ref="AA58:AA60" ca="1" si="22">IFERROR(OFFSET(A58,0,MATCH("",B58:Z58,-1)),"")</f>
+        <v/>
       </c>
       <c r="AB58" s="2" t="s">
         <v>6</v>
@@ -4174,7 +4411,7 @@
       <c r="AM58" s="1"/>
     </row>
     <row r="59" spans="2:39" outlineLevel="1">
-      <c r="B59" s="12"/>
+      <c r="B59" s="10"/>
       <c r="C59" s="20"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
@@ -4200,7 +4437,7 @@
       <c r="Y59" s="18"/>
       <c r="Z59" s="19"/>
       <c r="AA59" s="8" t="str">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AB59" s="2" t="s">
@@ -4219,7 +4456,7 @@
       <c r="AM59" s="1"/>
     </row>
     <row r="60" spans="2:39" outlineLevel="1">
-      <c r="B60" s="12"/>
+      <c r="B60" s="10"/>
       <c r="C60" s="20"/>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
@@ -4245,7 +4482,7 @@
       <c r="Y60" s="18"/>
       <c r="Z60" s="19"/>
       <c r="AA60" s="8" t="str">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="22"/>
         <v/>
       </c>
       <c r="AB60" s="2" t="s">
@@ -4264,10 +4501,8 @@
       <c r="AM60" s="1"/>
     </row>
     <row r="61" spans="2:39" outlineLevel="1">
-      <c r="B61" s="12"/>
-      <c r="C61" s="20" t="s">
-        <v>84</v>
-      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="20"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
@@ -4292,9 +4527,8 @@
       <c r="Y61" s="18"/>
       <c r="Z61" s="19"/>
       <c r="AA61" s="8" t="str">
-        <f t="shared" ref="AA61:AA65" ca="1" si="25">IFERROR(OFFSET(A61,0,MATCH("",B61:Z61,-1)),"")</f>
-        <v xml:space="preserve">
-</v>
+        <f t="shared" ref="AA61" ca="1" si="23">IFERROR(OFFSET(A61,0,MATCH("",B61:Z61,-1)),"")</f>
+        <v/>
       </c>
       <c r="AB61" s="2" t="s">
         <v>6</v>
@@ -4312,7 +4546,7 @@
       <c r="AM61" s="1"/>
     </row>
     <row r="62" spans="2:39" outlineLevel="1">
-      <c r="B62" s="12"/>
+      <c r="B62" s="10"/>
       <c r="C62" s="20"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
@@ -4338,7 +4572,7 @@
       <c r="Y62" s="18"/>
       <c r="Z62" s="19"/>
       <c r="AA62" s="8" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ref="AA62:AA65" ca="1" si="24">IFERROR(OFFSET(A62,0,MATCH("",B62:Z62,-1)),"")</f>
         <v/>
       </c>
       <c r="AB62" s="2" t="s">
@@ -4358,7 +4592,9 @@
     </row>
     <row r="63" spans="2:39" outlineLevel="1">
       <c r="B63" s="12"/>
-      <c r="C63" s="20"/>
+      <c r="C63" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
@@ -4383,8 +4619,9 @@
       <c r="Y63" s="18"/>
       <c r="Z63" s="19"/>
       <c r="AA63" s="8" t="str">
-        <f t="shared" ca="1" si="25"/>
-        <v/>
+        <f t="shared" ref="AA63:AA64" ca="1" si="25">IFERROR(OFFSET(A63,0,MATCH("",B63:Z63,-1)),"")</f>
+        <v xml:space="preserve">
+</v>
       </c>
       <c r="AB63" s="2" t="s">
         <v>6</v>
@@ -4473,7 +4710,7 @@
       <c r="Y65" s="18"/>
       <c r="Z65" s="19"/>
       <c r="AA65" s="8" t="str">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="24"/>
         <v/>
       </c>
       <c r="AB65" s="2" t="s">
@@ -4493,7 +4730,9 @@
     </row>
     <row r="66" spans="2:39" outlineLevel="1">
       <c r="B66" s="12"/>
-      <c r="C66" s="20"/>
+      <c r="C66" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="D66" s="18"/>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
@@ -4518,8 +4757,9 @@
       <c r="Y66" s="18"/>
       <c r="Z66" s="19"/>
       <c r="AA66" s="8" t="str">
-        <f t="shared" ref="AA66" ca="1" si="26">IFERROR(OFFSET(A66,0,MATCH("",B66:Z66,-1)),"")</f>
-        <v/>
+        <f t="shared" ref="AA66:AA70" ca="1" si="26">IFERROR(OFFSET(A66,0,MATCH("",B66:Z66,-1)),"")</f>
+        <v xml:space="preserve">
+</v>
       </c>
       <c r="AB66" s="2" t="s">
         <v>6</v>
@@ -4536,9 +4776,9 @@
       <c r="AL66" s="1"/>
       <c r="AM66" s="1"/>
     </row>
-    <row r="67" spans="2:39" collapsed="1">
-      <c r="B67" s="20"/>
-      <c r="C67" s="18"/>
+    <row r="67" spans="2:39" outlineLevel="1">
+      <c r="B67" s="12"/>
+      <c r="C67" s="20"/>
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
       <c r="F67" s="18"/>
@@ -4563,7 +4803,7 @@
       <c r="Y67" s="18"/>
       <c r="Z67" s="19"/>
       <c r="AA67" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AB67" s="2" t="s">
@@ -4581,9 +4821,9 @@
       <c r="AL67" s="1"/>
       <c r="AM67" s="1"/>
     </row>
-    <row r="68" spans="2:39">
-      <c r="B68" s="20"/>
-      <c r="C68" s="18"/>
+    <row r="68" spans="2:39" outlineLevel="1">
+      <c r="B68" s="12"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
       <c r="F68" s="18"/>
@@ -4608,7 +4848,7 @@
       <c r="Y68" s="18"/>
       <c r="Z68" s="19"/>
       <c r="AA68" s="8" t="str">
-        <f t="shared" ref="AA68:AA89" ca="1" si="27">IFERROR(OFFSET(A68,0,MATCH("",B68:Z68,-1)),"")</f>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AB68" s="2" t="s">
@@ -4627,8 +4867,8 @@
       <c r="AM68" s="1"/>
     </row>
     <row r="69" spans="2:39" outlineLevel="1">
-      <c r="B69" s="3"/>
-      <c r="C69" s="18"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="20"/>
       <c r="D69" s="18"/>
       <c r="E69" s="18"/>
       <c r="F69" s="18"/>
@@ -4653,7 +4893,7 @@
       <c r="Y69" s="18"/>
       <c r="Z69" s="19"/>
       <c r="AA69" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AB69" s="2" t="s">
@@ -4672,8 +4912,8 @@
       <c r="AM69" s="1"/>
     </row>
     <row r="70" spans="2:39" outlineLevel="1">
-      <c r="B70" s="3"/>
-      <c r="C70" s="18"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="18"/>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
@@ -4698,7 +4938,7 @@
       <c r="Y70" s="18"/>
       <c r="Z70" s="19"/>
       <c r="AA70" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="26"/>
         <v/>
       </c>
       <c r="AB70" s="2" t="s">
@@ -4716,9 +4956,9 @@
       <c r="AL70" s="1"/>
       <c r="AM70" s="1"/>
     </row>
-    <row r="71" spans="2:39" outlineLevel="2">
-      <c r="B71" s="3"/>
-      <c r="C71" s="4"/>
+    <row r="71" spans="2:39" outlineLevel="1">
+      <c r="B71" s="12"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="18"/>
       <c r="E71" s="18"/>
       <c r="F71" s="18"/>
@@ -4743,7 +4983,7 @@
       <c r="Y71" s="18"/>
       <c r="Z71" s="19"/>
       <c r="AA71" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ref="AA71" ca="1" si="27">IFERROR(OFFSET(A71,0,MATCH("",B71:Z71,-1)),"")</f>
         <v/>
       </c>
       <c r="AB71" s="2" t="s">
@@ -4761,9 +5001,9 @@
       <c r="AL71" s="1"/>
       <c r="AM71" s="1"/>
     </row>
-    <row r="72" spans="2:39" outlineLevel="2">
-      <c r="B72" s="3"/>
-      <c r="C72" s="4"/>
+    <row r="72" spans="2:39" collapsed="1">
+      <c r="B72" s="20"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
@@ -4788,7 +5028,7 @@
       <c r="Y72" s="18"/>
       <c r="Z72" s="19"/>
       <c r="AA72" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="AB72" s="2" t="s">
@@ -4806,10 +5046,10 @@
       <c r="AL72" s="1"/>
       <c r="AM72" s="1"/>
     </row>
-    <row r="73" spans="2:39" outlineLevel="3">
-      <c r="B73" s="3"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+    <row r="73" spans="2:39">
+      <c r="B73" s="20"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
       <c r="E73" s="18"/>
       <c r="F73" s="18"/>
       <c r="G73" s="18"/>
@@ -4833,7 +5073,7 @@
       <c r="Y73" s="18"/>
       <c r="Z73" s="19"/>
       <c r="AA73" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ref="AA73:AA94" ca="1" si="28">IFERROR(OFFSET(A73,0,MATCH("",B73:Z73,-1)),"")</f>
         <v/>
       </c>
       <c r="AB73" s="2" t="s">
@@ -4851,10 +5091,10 @@
       <c r="AL73" s="1"/>
       <c r="AM73" s="1"/>
     </row>
-    <row r="74" spans="2:39" outlineLevel="3" collapsed="1">
+    <row r="74" spans="2:39" outlineLevel="1">
       <c r="B74" s="3"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
       <c r="E74" s="18"/>
       <c r="F74" s="18"/>
       <c r="G74" s="18"/>
@@ -4878,7 +5118,7 @@
       <c r="Y74" s="18"/>
       <c r="Z74" s="19"/>
       <c r="AA74" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB74" s="2" t="s">
@@ -4896,11 +5136,11 @@
       <c r="AL74" s="1"/>
       <c r="AM74" s="1"/>
     </row>
-    <row r="75" spans="2:39" hidden="1" outlineLevel="4">
+    <row r="75" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B75" s="3"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
       <c r="H75" s="18"/>
@@ -4923,7 +5163,7 @@
       <c r="Y75" s="18"/>
       <c r="Z75" s="19"/>
       <c r="AA75" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB75" s="2" t="s">
@@ -4941,11 +5181,11 @@
       <c r="AL75" s="1"/>
       <c r="AM75" s="1"/>
     </row>
-    <row r="76" spans="2:39" hidden="1" outlineLevel="4">
+    <row r="76" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B76" s="3"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
       <c r="H76" s="18"/>
@@ -4968,7 +5208,7 @@
       <c r="Y76" s="18"/>
       <c r="Z76" s="19"/>
       <c r="AA76" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB76" s="2" t="s">
@@ -4986,12 +5226,12 @@
       <c r="AL76" s="1"/>
       <c r="AM76" s="1"/>
     </row>
-    <row r="77" spans="2:39" hidden="1" outlineLevel="5">
+    <row r="77" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B77" s="3"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
       <c r="G77" s="18"/>
       <c r="H77" s="18"/>
       <c r="I77" s="18"/>
@@ -5013,7 +5253,7 @@
       <c r="Y77" s="18"/>
       <c r="Z77" s="19"/>
       <c r="AA77" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB77" s="2" t="s">
@@ -5031,12 +5271,12 @@
       <c r="AL77" s="1"/>
       <c r="AM77" s="1"/>
     </row>
-    <row r="78" spans="2:39" hidden="1" outlineLevel="5">
+    <row r="78" spans="2:39" hidden="1" outlineLevel="3">
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
       <c r="G78" s="18"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18"/>
@@ -5058,7 +5298,7 @@
       <c r="Y78" s="18"/>
       <c r="Z78" s="19"/>
       <c r="AA78" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB78" s="2" t="s">
@@ -5076,13 +5316,13 @@
       <c r="AL78" s="1"/>
       <c r="AM78" s="1"/>
     </row>
-    <row r="79" spans="2:39" hidden="1" outlineLevel="6">
+    <row r="79" spans="2:39" hidden="1" outlineLevel="3">
       <c r="B79" s="3"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="18"/>
       <c r="I79" s="18"/>
       <c r="J79" s="18"/>
@@ -5103,7 +5343,7 @@
       <c r="Y79" s="18"/>
       <c r="Z79" s="19"/>
       <c r="AA79" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB79" s="2" t="s">
@@ -5121,13 +5361,13 @@
       <c r="AL79" s="1"/>
       <c r="AM79" s="1"/>
     </row>
-    <row r="80" spans="2:39" hidden="1" outlineLevel="6">
+    <row r="80" spans="2:39" hidden="1" outlineLevel="4">
       <c r="B80" s="3"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
       <c r="H80" s="18"/>
       <c r="I80" s="18"/>
       <c r="J80" s="18"/>
@@ -5148,7 +5388,7 @@
       <c r="Y80" s="18"/>
       <c r="Z80" s="19"/>
       <c r="AA80" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB80" s="2" t="s">
@@ -5166,14 +5406,14 @@
       <c r="AL80" s="1"/>
       <c r="AM80" s="1"/>
     </row>
-    <row r="81" spans="2:39" hidden="1" outlineLevel="7">
+    <row r="81" spans="2:39" hidden="1" outlineLevel="4">
       <c r="B81" s="3"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
       <c r="I81" s="18"/>
       <c r="J81" s="18"/>
       <c r="K81" s="18"/>
@@ -5193,7 +5433,7 @@
       <c r="Y81" s="18"/>
       <c r="Z81" s="19"/>
       <c r="AA81" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB81" s="2" t="s">
@@ -5211,14 +5451,14 @@
       <c r="AL81" s="1"/>
       <c r="AM81" s="1"/>
     </row>
-    <row r="82" spans="2:39" hidden="1" outlineLevel="7">
+    <row r="82" spans="2:39" hidden="1" outlineLevel="5">
       <c r="B82" s="3"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
       <c r="I82" s="18"/>
       <c r="J82" s="18"/>
       <c r="K82" s="18"/>
@@ -5238,7 +5478,7 @@
       <c r="Y82" s="18"/>
       <c r="Z82" s="19"/>
       <c r="AA82" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB82" s="2" t="s">
@@ -5256,13 +5496,13 @@
       <c r="AL82" s="1"/>
       <c r="AM82" s="1"/>
     </row>
-    <row r="83" spans="2:39" hidden="1" outlineLevel="6">
+    <row r="83" spans="2:39" hidden="1" outlineLevel="5">
       <c r="B83" s="3"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
+      <c r="G83" s="18"/>
       <c r="H83" s="18"/>
       <c r="I83" s="18"/>
       <c r="J83" s="18"/>
@@ -5283,7 +5523,7 @@
       <c r="Y83" s="18"/>
       <c r="Z83" s="19"/>
       <c r="AA83" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB83" s="2" t="s">
@@ -5301,13 +5541,13 @@
       <c r="AL83" s="1"/>
       <c r="AM83" s="1"/>
     </row>
-    <row r="84" spans="2:39" hidden="1" outlineLevel="5">
+    <row r="84" spans="2:39" hidden="1" outlineLevel="6">
       <c r="B84" s="3"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
-      <c r="G84" s="18"/>
+      <c r="G84" s="4"/>
       <c r="H84" s="18"/>
       <c r="I84" s="18"/>
       <c r="J84" s="18"/>
@@ -5328,7 +5568,7 @@
       <c r="Y84" s="18"/>
       <c r="Z84" s="19"/>
       <c r="AA84" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB84" s="2" t="s">
@@ -5346,13 +5586,13 @@
       <c r="AL84" s="1"/>
       <c r="AM84" s="1"/>
     </row>
-    <row r="85" spans="2:39" hidden="1" outlineLevel="4">
+    <row r="85" spans="2:39" hidden="1" outlineLevel="6">
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
       <c r="H85" s="18"/>
       <c r="I85" s="18"/>
       <c r="J85" s="18"/>
@@ -5373,7 +5613,7 @@
       <c r="Y85" s="18"/>
       <c r="Z85" s="19"/>
       <c r="AA85" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB85" s="2" t="s">
@@ -5391,14 +5631,14 @@
       <c r="AL85" s="1"/>
       <c r="AM85" s="1"/>
     </row>
-    <row r="86" spans="2:39" outlineLevel="3">
+    <row r="86" spans="2:39" hidden="1" outlineLevel="7">
       <c r="B86" s="3"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
       <c r="I86" s="18"/>
       <c r="J86" s="18"/>
       <c r="K86" s="18"/>
@@ -5418,7 +5658,7 @@
       <c r="Y86" s="18"/>
       <c r="Z86" s="19"/>
       <c r="AA86" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB86" s="2" t="s">
@@ -5436,14 +5676,14 @@
       <c r="AL86" s="1"/>
       <c r="AM86" s="1"/>
     </row>
-    <row r="87" spans="2:39" outlineLevel="3">
+    <row r="87" spans="2:39" hidden="1" outlineLevel="7">
       <c r="B87" s="3"/>
       <c r="C87" s="4"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="18"/>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
-      <c r="H87" s="18"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
       <c r="I87" s="18"/>
       <c r="J87" s="18"/>
       <c r="K87" s="18"/>
@@ -5463,7 +5703,7 @@
       <c r="Y87" s="18"/>
       <c r="Z87" s="19"/>
       <c r="AA87" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB87" s="2" t="s">
@@ -5481,13 +5721,13 @@
       <c r="AL87" s="1"/>
       <c r="AM87" s="1"/>
     </row>
-    <row r="88" spans="2:39" outlineLevel="2">
+    <row r="88" spans="2:39" hidden="1" outlineLevel="6">
       <c r="B88" s="3"/>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
       <c r="H88" s="18"/>
       <c r="I88" s="18"/>
       <c r="J88" s="18"/>
@@ -5508,7 +5748,7 @@
       <c r="Y88" s="18"/>
       <c r="Z88" s="19"/>
       <c r="AA88" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB88" s="2" t="s">
@@ -5526,12 +5766,12 @@
       <c r="AL88" s="1"/>
       <c r="AM88" s="1"/>
     </row>
-    <row r="89" spans="2:39">
-      <c r="B89" s="20"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
+    <row r="89" spans="2:39" hidden="1" outlineLevel="5">
+      <c r="B89" s="3"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
       <c r="G89" s="18"/>
       <c r="H89" s="18"/>
       <c r="I89" s="18"/>
@@ -5553,7 +5793,7 @@
       <c r="Y89" s="18"/>
       <c r="Z89" s="19"/>
       <c r="AA89" s="8" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v/>
       </c>
       <c r="AB89" s="2" t="s">
@@ -5571,8 +5811,238 @@
       <c r="AL89" s="1"/>
       <c r="AM89" s="1"/>
     </row>
+    <row r="90" spans="2:39" hidden="1" outlineLevel="4">
+      <c r="B90" s="3"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="18"/>
+      <c r="S90" s="18"/>
+      <c r="T90" s="18"/>
+      <c r="U90" s="18"/>
+      <c r="V90" s="18"/>
+      <c r="W90" s="18"/>
+      <c r="X90" s="18"/>
+      <c r="Y90" s="18"/>
+      <c r="Z90" s="19"/>
+      <c r="AA90" s="8" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AB90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC90" s="2"/>
+      <c r="AD90" s="2"/>
+      <c r="AE90" s="2"/>
+      <c r="AF90" s="2"/>
+      <c r="AG90" s="2"/>
+      <c r="AH90" s="2"/>
+      <c r="AI90" s="2"/>
+      <c r="AJ90" s="2"/>
+      <c r="AK90" s="2"/>
+      <c r="AL90" s="1"/>
+      <c r="AM90" s="1"/>
+    </row>
+    <row r="91" spans="2:39" hidden="1" outlineLevel="3">
+      <c r="B91" s="3"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="18"/>
+      <c r="M91" s="18"/>
+      <c r="N91" s="18"/>
+      <c r="O91" s="18"/>
+      <c r="P91" s="18"/>
+      <c r="Q91" s="18"/>
+      <c r="R91" s="18"/>
+      <c r="S91" s="18"/>
+      <c r="T91" s="18"/>
+      <c r="U91" s="18"/>
+      <c r="V91" s="18"/>
+      <c r="W91" s="18"/>
+      <c r="X91" s="18"/>
+      <c r="Y91" s="18"/>
+      <c r="Z91" s="19"/>
+      <c r="AA91" s="8" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AB91" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC91" s="2"/>
+      <c r="AD91" s="2"/>
+      <c r="AE91" s="2"/>
+      <c r="AF91" s="2"/>
+      <c r="AG91" s="2"/>
+      <c r="AH91" s="2"/>
+      <c r="AI91" s="2"/>
+      <c r="AJ91" s="2"/>
+      <c r="AK91" s="2"/>
+      <c r="AL91" s="1"/>
+      <c r="AM91" s="1"/>
+    </row>
+    <row r="92" spans="2:39" hidden="1" outlineLevel="3">
+      <c r="B92" s="3"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="18"/>
+      <c r="E92" s="18"/>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="18"/>
+      <c r="M92" s="18"/>
+      <c r="N92" s="18"/>
+      <c r="O92" s="18"/>
+      <c r="P92" s="18"/>
+      <c r="Q92" s="18"/>
+      <c r="R92" s="18"/>
+      <c r="S92" s="18"/>
+      <c r="T92" s="18"/>
+      <c r="U92" s="18"/>
+      <c r="V92" s="18"/>
+      <c r="W92" s="18"/>
+      <c r="X92" s="18"/>
+      <c r="Y92" s="18"/>
+      <c r="Z92" s="19"/>
+      <c r="AA92" s="8" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AB92" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC92" s="2"/>
+      <c r="AD92" s="2"/>
+      <c r="AE92" s="2"/>
+      <c r="AF92" s="2"/>
+      <c r="AG92" s="2"/>
+      <c r="AH92" s="2"/>
+      <c r="AI92" s="2"/>
+      <c r="AJ92" s="2"/>
+      <c r="AK92" s="2"/>
+      <c r="AL92" s="1"/>
+      <c r="AM92" s="1"/>
+    </row>
+    <row r="93" spans="2:39" hidden="1" outlineLevel="2">
+      <c r="B93" s="3"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="18"/>
+      <c r="M93" s="18"/>
+      <c r="N93" s="18"/>
+      <c r="O93" s="18"/>
+      <c r="P93" s="18"/>
+      <c r="Q93" s="18"/>
+      <c r="R93" s="18"/>
+      <c r="S93" s="18"/>
+      <c r="T93" s="18"/>
+      <c r="U93" s="18"/>
+      <c r="V93" s="18"/>
+      <c r="W93" s="18"/>
+      <c r="X93" s="18"/>
+      <c r="Y93" s="18"/>
+      <c r="Z93" s="19"/>
+      <c r="AA93" s="8" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AB93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC93" s="2"/>
+      <c r="AD93" s="2"/>
+      <c r="AE93" s="2"/>
+      <c r="AF93" s="2"/>
+      <c r="AG93" s="2"/>
+      <c r="AH93" s="2"/>
+      <c r="AI93" s="2"/>
+      <c r="AJ93" s="2"/>
+      <c r="AK93" s="2"/>
+      <c r="AL93" s="1"/>
+      <c r="AM93" s="1"/>
+    </row>
+    <row r="94" spans="2:39">
+      <c r="B94" s="20"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="18"/>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18"/>
+      <c r="N94" s="18"/>
+      <c r="O94" s="18"/>
+      <c r="P94" s="18"/>
+      <c r="Q94" s="18"/>
+      <c r="R94" s="18"/>
+      <c r="S94" s="18"/>
+      <c r="T94" s="18"/>
+      <c r="U94" s="18"/>
+      <c r="V94" s="18"/>
+      <c r="W94" s="18"/>
+      <c r="X94" s="18"/>
+      <c r="Y94" s="18"/>
+      <c r="Z94" s="19"/>
+      <c r="AA94" s="8" t="str">
+        <f t="shared" ca="1" si="28"/>
+        <v/>
+      </c>
+      <c r="AB94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC94" s="2"/>
+      <c r="AD94" s="2"/>
+      <c r="AE94" s="2"/>
+      <c r="AF94" s="2"/>
+      <c r="AG94" s="2"/>
+      <c r="AH94" s="2"/>
+      <c r="AI94" s="2"/>
+      <c r="AJ94" s="2"/>
+      <c r="AK94" s="2"/>
+      <c r="AL94" s="1"/>
+      <c r="AM94" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="95">
+    <mergeCell ref="D40:Z40"/>
+    <mergeCell ref="E41:Z41"/>
+    <mergeCell ref="E42:Z42"/>
+    <mergeCell ref="C38:Z38"/>
+    <mergeCell ref="D39:Z39"/>
     <mergeCell ref="C34:Z34"/>
     <mergeCell ref="D35:Z35"/>
     <mergeCell ref="C36:Z36"/>
@@ -5589,21 +6059,21 @@
     <mergeCell ref="C29:Z29"/>
     <mergeCell ref="D30:Z30"/>
     <mergeCell ref="D20:Z20"/>
-    <mergeCell ref="B52:Z52"/>
-    <mergeCell ref="C61:Z61"/>
-    <mergeCell ref="C60:Z60"/>
+    <mergeCell ref="B57:Z57"/>
+    <mergeCell ref="C66:Z66"/>
+    <mergeCell ref="C65:Z65"/>
+    <mergeCell ref="C50:Z50"/>
+    <mergeCell ref="C51:Z51"/>
+    <mergeCell ref="B53:Z53"/>
+    <mergeCell ref="C55:Z55"/>
+    <mergeCell ref="C49:Z49"/>
+    <mergeCell ref="B54:Z54"/>
+    <mergeCell ref="C56:Z56"/>
+    <mergeCell ref="D4:Z4"/>
+    <mergeCell ref="B44:Z44"/>
     <mergeCell ref="C45:Z45"/>
     <mergeCell ref="C46:Z46"/>
-    <mergeCell ref="B48:Z48"/>
-    <mergeCell ref="C50:Z50"/>
-    <mergeCell ref="C44:Z44"/>
-    <mergeCell ref="B49:Z49"/>
-    <mergeCell ref="C51:Z51"/>
-    <mergeCell ref="D4:Z4"/>
-    <mergeCell ref="B39:Z39"/>
-    <mergeCell ref="C40:Z40"/>
-    <mergeCell ref="C41:Z41"/>
-    <mergeCell ref="B42:Z42"/>
+    <mergeCell ref="B47:Z47"/>
     <mergeCell ref="C12:Z12"/>
     <mergeCell ref="D13:Z13"/>
     <mergeCell ref="C14:Z14"/>
@@ -5616,53 +6086,53 @@
     <mergeCell ref="C23:Z23"/>
     <mergeCell ref="D24:Z24"/>
     <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="H83:Z83"/>
-    <mergeCell ref="G84:Z84"/>
-    <mergeCell ref="F85:Z85"/>
-    <mergeCell ref="G77:Z77"/>
-    <mergeCell ref="G78:Z78"/>
-    <mergeCell ref="H79:Z79"/>
-    <mergeCell ref="H80:Z80"/>
-    <mergeCell ref="I81:Z81"/>
-    <mergeCell ref="F76:Z76"/>
-    <mergeCell ref="I82:Z82"/>
+    <mergeCell ref="H88:Z88"/>
+    <mergeCell ref="G89:Z89"/>
+    <mergeCell ref="F90:Z90"/>
+    <mergeCell ref="G82:Z82"/>
+    <mergeCell ref="G83:Z83"/>
+    <mergeCell ref="H84:Z84"/>
+    <mergeCell ref="H85:Z85"/>
+    <mergeCell ref="I86:Z86"/>
+    <mergeCell ref="F81:Z81"/>
+    <mergeCell ref="I87:Z87"/>
     <mergeCell ref="B1:Z1"/>
-    <mergeCell ref="D72:Z72"/>
+    <mergeCell ref="D77:Z77"/>
     <mergeCell ref="B2:Z2"/>
     <mergeCell ref="C3:Z3"/>
-    <mergeCell ref="B67:Z67"/>
-    <mergeCell ref="E73:Z73"/>
-    <mergeCell ref="B68:Z68"/>
+    <mergeCell ref="B72:Z72"/>
+    <mergeCell ref="E78:Z78"/>
+    <mergeCell ref="B73:Z73"/>
+    <mergeCell ref="C74:Z74"/>
+    <mergeCell ref="C75:Z75"/>
+    <mergeCell ref="D76:Z76"/>
+    <mergeCell ref="B94:Z94"/>
+    <mergeCell ref="E91:Z91"/>
+    <mergeCell ref="D92:Z92"/>
+    <mergeCell ref="C93:Z93"/>
+    <mergeCell ref="E79:Z79"/>
+    <mergeCell ref="F80:Z80"/>
+    <mergeCell ref="C67:Z67"/>
+    <mergeCell ref="C68:Z68"/>
     <mergeCell ref="C69:Z69"/>
     <mergeCell ref="C70:Z70"/>
-    <mergeCell ref="D71:Z71"/>
-    <mergeCell ref="B89:Z89"/>
-    <mergeCell ref="E86:Z86"/>
-    <mergeCell ref="D87:Z87"/>
-    <mergeCell ref="C88:Z88"/>
-    <mergeCell ref="E74:Z74"/>
-    <mergeCell ref="F75:Z75"/>
-    <mergeCell ref="C62:Z62"/>
-    <mergeCell ref="C63:Z63"/>
-    <mergeCell ref="C64:Z64"/>
-    <mergeCell ref="C65:Z65"/>
-    <mergeCell ref="C66:Z66"/>
+    <mergeCell ref="C71:Z71"/>
     <mergeCell ref="D5:Z5"/>
     <mergeCell ref="C10:Z10"/>
     <mergeCell ref="D11:Z11"/>
-    <mergeCell ref="C58:Z58"/>
-    <mergeCell ref="C59:Z59"/>
+    <mergeCell ref="C63:Z63"/>
+    <mergeCell ref="C64:Z64"/>
     <mergeCell ref="C7:Z7"/>
     <mergeCell ref="D9:Z9"/>
-    <mergeCell ref="C38:Z38"/>
+    <mergeCell ref="C43:Z43"/>
     <mergeCell ref="D8:Z8"/>
-    <mergeCell ref="C43:Z43"/>
-    <mergeCell ref="C47:Z47"/>
-    <mergeCell ref="B53:Z53"/>
-    <mergeCell ref="C54:Z54"/>
-    <mergeCell ref="C55:Z55"/>
-    <mergeCell ref="C56:Z56"/>
-    <mergeCell ref="C57:Z57"/>
+    <mergeCell ref="C48:Z48"/>
+    <mergeCell ref="C52:Z52"/>
+    <mergeCell ref="B58:Z58"/>
+    <mergeCell ref="C59:Z59"/>
+    <mergeCell ref="C60:Z60"/>
+    <mergeCell ref="C61:Z61"/>
+    <mergeCell ref="C62:Z62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more Kubernetes commands.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="330">
   <si>
     <t>Details</t>
   </si>
@@ -1175,30 +1175,6 @@
     <t>pods/monolith.yaml</t>
   </si>
   <si>
-    <t>kubectl label pods secure-monolith 'secure=enabled'</t>
-  </si>
-  <si>
-    <t>kubectl get pods secure-monolith --show-labels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kubectl describe services monolith </t>
-  </si>
-  <si>
-    <t>io</t>
-  </si>
-  <si>
-    <t>Opens a shell session inside the pod(?) container(?).</t>
-  </si>
-  <si>
-    <t>Creates a configmap(?).</t>
-  </si>
-  <si>
-    <t>Adds the label "secure=enabled" to the secure-monolith pod.</t>
-  </si>
-  <si>
-    <t>Displays the labels of the secure-monolith pod.</t>
-  </si>
-  <si>
     <t>Creates a resource out of a .yaml file.</t>
   </si>
   <si>
@@ -1274,7 +1250,92 @@
     <t>Labels:</t>
   </si>
   <si>
-    <t>app=monolith</t>
+    <t>bootcamp</t>
+  </si>
+  <si>
+    <t>Nodes:</t>
+  </si>
+  <si>
+    <t>Scopes(?):</t>
+  </si>
+  <si>
+    <t>"https://www.googleapis.com/auth/projecthosting,storage-rw"</t>
+  </si>
+  <si>
+    <t>Show labels:</t>
+  </si>
+  <si>
+    <t>Documentation about a particular field.</t>
+  </si>
+  <si>
+    <t>deployments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kubectl get pods -o jsonpath --template='{range .items[*]}{.metadata.name}{"\t"}{"\t"}{.spec.containers[0].image}{"\n"}{end}'
+</t>
+  </si>
+  <si>
+    <t>kubectl apply -f services/hello-blue.yaml</t>
+  </si>
+  <si>
+    <t>Updates labels on a resource (or resources).</t>
+  </si>
+  <si>
+    <t>secure-monolith</t>
+  </si>
+  <si>
+    <t>secure=enabled</t>
+  </si>
+  <si>
+    <t>services</t>
+  </si>
+  <si>
+    <t>Prints documentation about a Kubernete resource type and its .yaml definition.</t>
+  </si>
+  <si>
+    <t>Resource Type / field:</t>
+  </si>
+  <si>
+    <t>Recursive:</t>
+  </si>
+  <si>
+    <t>deployment.metadata.name</t>
+  </si>
+  <si>
+    <t>Set a new size for a Deployment, ReplicaSet, Replication Controller, or Job.</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>Target replicas:</t>
+  </si>
+  <si>
+    <t>Set a new size for a Deployment, ReplicaSet, Replication Controller, or Job identified by type and name.</t>
+  </si>
+  <si>
+    <t>Live edits the .yaml definition of a resource.</t>
+  </si>
+  <si>
+    <t>Manages rollout updates.</t>
+  </si>
+  <si>
+    <t>Lists rollout history of a resource.</t>
+  </si>
+  <si>
+    <t>Pause an in-progress rollout update.</t>
+  </si>
+  <si>
+    <t>Only deployments support this command.</t>
+  </si>
+  <si>
+    <t>Resumes a previously pauses rollout update.</t>
+  </si>
+  <si>
+    <t>Shows the status of the current/last rollout update.</t>
+  </si>
+  <si>
+    <t>Rolls back the last rollout update.</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1964,7 @@
   </sheetPr>
   <dimension ref="B1:AQ110"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="AA79" sqref="AA79"/>
     </sheetView>
   </sheetViews>
@@ -6416,12 +6477,12 @@
       </c>
       <c r="AQ78" s="1"/>
     </row>
-    <row r="79" spans="2:43" ht="30" outlineLevel="2">
+    <row r="79" spans="2:43" ht="51" customHeight="1" outlineLevel="2">
       <c r="B79" s="27"/>
       <c r="C79" s="26"/>
       <c r="D79" s="33" t="str">
-        <f>C$78&amp;" create "&amp;AC79</f>
-        <v>gcloud container clusters create io</v>
+        <f>C$78&amp;" create "&amp;AC79&amp;IF(ISBLANK(AE79),""," --num-nodes "&amp;AE79)&amp;IF(ISBLANK(AG79),""," --scopes "&amp;AG79)</f>
+        <v>gcloud container clusters create bootcamp --num-nodes 5 --scopes "https://www.googleapis.com/auth/projecthosting,storage-rw"</v>
       </c>
       <c r="E79" s="34"/>
       <c r="F79" s="34"/>
@@ -6447,18 +6508,26 @@
       <c r="Z79" s="35"/>
       <c r="AA79" s="8" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>gcloud container clusters create io</v>
+        <v>gcloud container clusters create bootcamp --num-nodes 5 --scopes "https://www.googleapis.com/auth/projecthosting,storage-rw"</v>
       </c>
       <c r="AB79" s="21" t="s">
         <v>250</v>
       </c>
       <c r="AC79" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AD79" s="2"/>
-      <c r="AE79" s="2"/>
-      <c r="AF79" s="2"/>
-      <c r="AG79" s="2"/>
+        <v>301</v>
+      </c>
+      <c r="AD79" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AE79" s="5">
+        <v>5</v>
+      </c>
+      <c r="AF79" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="AG79" s="5" t="s">
+        <v>304</v>
+      </c>
       <c r="AH79" s="2"/>
       <c r="AI79" s="2"/>
       <c r="AJ79" s="2"/>
@@ -10230,10 +10299,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AK55"/>
+  <dimension ref="B1:AK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -10243,7 +10312,7 @@
     <col min="28" max="28" width="18.140625" customWidth="1" outlineLevel="1"/>
     <col min="29" max="29" width="19.28515625" customWidth="1" outlineLevel="1"/>
     <col min="30" max="30" width="14.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="19.28515625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="19.28515625" customWidth="1" outlineLevel="1"/>
     <col min="32" max="32" width="12.7109375" customWidth="1" outlineLevel="1"/>
     <col min="33" max="33" width="21" customWidth="1" outlineLevel="1"/>
     <col min="34" max="34" width="15.5703125" customWidth="1" outlineLevel="1"/>
@@ -10331,7 +10400,7 @@
       <c r="Y2" s="37"/>
       <c r="Z2" s="38"/>
       <c r="AA2" s="8" t="str">
-        <f t="shared" ref="AA2:AA52" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
+        <f t="shared" ref="AA2:AA69" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
         <v>kubectl run nginx --image=nginx:1.10.0</v>
       </c>
       <c r="AB2" s="2" t="s">
@@ -10423,8 +10492,8 @@
     </row>
     <row r="4" spans="2:37">
       <c r="B4" s="36" t="str">
-        <f>"kubectl get "&amp;AC4&amp;IF(ISBLANK(AE4),""," "&amp;AE4)&amp;IF(ISBLANK(AG4),""," -l "&amp;CHAR(34)&amp;AG4&amp;CHAR(34))</f>
-        <v>kubectl get pods -l "app=monolith"</v>
+        <f>"kubectl get "&amp;AC4&amp;IF(ISBLANK(AE4),""," "&amp;AE4)&amp;IF(ISBLANK(AG4),""," -l "&amp;CHAR(34)&amp;AG4&amp;CHAR(34))&amp;IF(ISBLANK(AI4),""," --show-labels")</f>
+        <v>kubectl get deployments</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
@@ -10452,26 +10521,26 @@
       <c r="Z4" s="38"/>
       <c r="AA4" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>kubectl get pods -l "app=monolith"</v>
+        <v>kubectl get deployments</v>
       </c>
       <c r="AB4" s="21" t="s">
         <v>270</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="AD4" s="22" t="s">
         <v>269</v>
       </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
+        <v>300</v>
+      </c>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="AI4" s="5"/>
       <c r="AJ4" s="1" t="s">
         <v>272</v>
       </c>
@@ -10521,7 +10590,7 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="AK5" s="1"/>
     </row>
@@ -10559,7 +10628,7 @@
         <v>kubectl create -f pods/monolith.yaml</v>
       </c>
       <c r="AB6" s="21" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="AC6" s="5" t="s">
         <v>275</v>
@@ -10571,7 +10640,7 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="AK6" s="1"/>
     </row>
@@ -10655,23 +10724,23 @@
         <v>kubectl create secret generic tls-certs --from-file tls/</v>
       </c>
       <c r="AB8" s="21" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="AD8" s="21" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="AK8" s="1"/>
     </row>
@@ -10798,23 +10867,23 @@
         <v>kubectl create configmap nginx-proxy-conf --from-file nginx/proxy.conf</v>
       </c>
       <c r="AB11" s="21" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="AD11" s="21" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="AK11" s="1"/>
     </row>
@@ -10907,7 +10976,7 @@
     <row r="14" spans="2:37">
       <c r="B14" s="36" t="str">
         <f>"kubectl describe "&amp;AC14&amp;IF(ISBLANK(AE14),""," "&amp;AE14)</f>
-        <v>kubectl describe pods nginx</v>
+        <v>kubectl describe services monolith</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -10935,26 +11004,26 @@
       <c r="Z14" s="38"/>
       <c r="AA14" s="8" t="str">
         <f t="shared" ref="AA14" ca="1" si="3">IFERROR(OFFSET(A14,0,MATCH("",B14:Z14,-1)),"")</f>
-        <v>kubectl describe pods nginx</v>
+        <v>kubectl describe services monolith</v>
       </c>
       <c r="AB14" s="21" t="s">
         <v>270</v>
       </c>
       <c r="AC14" s="5" t="s">
-        <v>273</v>
+        <v>313</v>
       </c>
       <c r="AD14" s="22" t="s">
         <v>269</v>
       </c>
       <c r="AE14" s="5" t="s">
-        <v>99</v>
+        <v>281</v>
       </c>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="AK14" s="1"/>
     </row>
@@ -10992,19 +11061,19 @@
         <v>kubectl port-forward monolith 10080:80</v>
       </c>
       <c r="AB15" s="21" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AE15" s="5">
         <v>10080</v>
       </c>
       <c r="AF15" s="21" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="AG15" s="5">
         <v>80</v>
@@ -11012,7 +11081,7 @@
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="AK15" s="1"/>
     </row>
@@ -11050,13 +11119,13 @@
         <v>kubectl logs -f monolith</v>
       </c>
       <c r="AB16" s="21" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AE16" s="5" t="b">
         <v>1</v>
@@ -11066,7 +11135,7 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AK16" s="1"/>
     </row>
@@ -11114,7 +11183,7 @@
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="AK17" s="1"/>
     </row>
@@ -11152,25 +11221,25 @@
         <v>kubectl exec monolith -- ls</v>
       </c>
       <c r="AB18" s="21" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AD18" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="AE18" s="5"/>
       <c r="AF18" s="21" t="s">
         <v>21</v>
       </c>
       <c r="AG18" s="5" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="AK18" s="1"/>
     </row>
@@ -11208,13 +11277,13 @@
         <v>kubectl exec monolith --stdin --tty /bin/sh</v>
       </c>
       <c r="AB19" s="21" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="AE19" s="5"/>
       <c r="AF19" s="2"/>
@@ -11222,12 +11291,15 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="AK19" s="1"/>
     </row>
     <row r="20" spans="2:37">
-      <c r="B20" s="36"/>
+      <c r="B20" s="36" t="str">
+        <f>"kubectl label "&amp;AC20&amp;" "&amp;AE20&amp;" '"&amp;AG20&amp;"'"</f>
+        <v>kubectl label pods secure-monolith 'secure=enabled'</v>
+      </c>
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
@@ -11254,21 +11326,38 @@
       <c r="Z20" s="38"/>
       <c r="AA20" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
+        <v>kubectl label pods secure-monolith 'secure=enabled'</v>
+      </c>
+      <c r="AB20" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="AD20" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE20" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF20" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="AG20" s="5" t="s">
+        <v>312</v>
+      </c>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
-      <c r="AJ20" s="1"/>
+      <c r="AJ20" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="AK20" s="1"/>
     </row>
-    <row r="21" spans="2:37">
-      <c r="B21" s="36"/>
+    <row r="21" spans="2:37" ht="30">
+      <c r="B21" s="36" t="str">
+        <f>"kubectl explain "&amp;AC21&amp;IF(AE21," --recursive","")</f>
+        <v>kubectl explain deployment.metadata.name</v>
+      </c>
       <c r="C21" s="37"/>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
@@ -11295,21 +11384,32 @@
       <c r="Z21" s="38"/>
       <c r="AA21" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="2"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
+        <v>kubectl explain deployment.metadata.name</v>
+      </c>
+      <c r="AB21" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="AD21" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="AE21" s="5"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
-      <c r="AJ21" s="1"/>
+      <c r="AJ21" s="1" t="s">
+        <v>314</v>
+      </c>
       <c r="AK21" s="1"/>
     </row>
-    <row r="22" spans="2:37">
-      <c r="B22" s="36"/>
+    <row r="22" spans="2:37" ht="30">
+      <c r="B22" s="36" t="str">
+        <f>"kubectl scale"</f>
+        <v>kubectl scale</v>
+      </c>
       <c r="C22" s="37"/>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
@@ -11335,10 +11435,12 @@
       <c r="Y22" s="37"/>
       <c r="Z22" s="38"/>
       <c r="AA22" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB22" s="2"/>
+        <f ca="1">IFERROR(OFFSET(A22,0,MATCH("",B22:Z22,-1)),"")</f>
+        <v>kubectl scale</v>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
@@ -11347,13 +11449,16 @@
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="1" t="s">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="AK22" s="1"/>
     </row>
-    <row r="23" spans="2:37">
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+    <row r="23" spans="2:37" ht="30" outlineLevel="1">
+      <c r="B23" s="31"/>
+      <c r="C23" s="37" t="str">
+        <f>B$22&amp;" "&amp;AC23&amp;" "&amp;AE23&amp;" --replicas="&amp;AG23</f>
+        <v>kubectl scale deployment hello --replicas=5</v>
+      </c>
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
       <c r="F23" s="37"/>
@@ -11378,22 +11483,36 @@
       <c r="Y23" s="37"/>
       <c r="Z23" s="38"/>
       <c r="AA23" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB23" s="2"/>
-      <c r="AC23" s="2"/>
-      <c r="AD23" s="2"/>
-      <c r="AE23" s="2"/>
-      <c r="AF23" s="2"/>
-      <c r="AG23" s="2"/>
+        <f t="shared" ref="AA23:AA24" ca="1" si="6">IFERROR(OFFSET(A23,0,MATCH("",B23:Z23,-1)),"")</f>
+        <v>kubectl scale deployment hello --replicas=5</v>
+      </c>
+      <c r="AB23" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC23" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD23" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE23" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="AF23" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="AG23" s="5">
+        <v>5</v>
+      </c>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
-      <c r="AJ23" s="1"/>
+      <c r="AJ23" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" spans="2:37">
-      <c r="B24" s="36"/>
+    <row r="24" spans="2:37" outlineLevel="1">
+      <c r="B24" s="31"/>
       <c r="C24" s="37"/>
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
@@ -11419,10 +11538,12 @@
       <c r="Y24" s="37"/>
       <c r="Z24" s="38"/>
       <c r="AA24" s="8" t="str">
-        <f t="shared" ref="AA24:AA27" ca="1" si="6">IFERROR(OFFSET(A24,0,MATCH("",B24:Z24,-1)),"")</f>
+        <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="AB24" s="2"/>
+      <c r="AB24" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="AC24" s="2"/>
       <c r="AD24" s="2"/>
       <c r="AE24" s="2"/>
@@ -11430,13 +11551,14 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
-      <c r="AJ24" s="1" t="s">
-        <v>281</v>
-      </c>
+      <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
     </row>
     <row r="25" spans="2:37">
-      <c r="B25" s="36"/>
+      <c r="B25" s="36" t="str">
+        <f>"kubectl edit "&amp;AC25&amp;" "&amp;AE25</f>
+        <v>kubectl edit deployment hello</v>
+      </c>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -11462,23 +11584,34 @@
       <c r="Y25" s="37"/>
       <c r="Z25" s="38"/>
       <c r="AA25" s="8" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="2"/>
-      <c r="AD25" s="2"/>
-      <c r="AE25" s="2"/>
+        <f ca="1">IFERROR(OFFSET(A25,0,MATCH("",B25:Z25,-1)),"")</f>
+        <v>kubectl edit deployment hello</v>
+      </c>
+      <c r="AB25" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC25" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD25" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE25" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
-      <c r="AJ25" s="1"/>
+      <c r="AJ25" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="AK25" s="1"/>
     </row>
     <row r="26" spans="2:37">
-      <c r="B26" s="36" t="s">
-        <v>276</v>
+      <c r="B26" s="36" t="str">
+        <f>"kubectl rollout"</f>
+        <v>kubectl rollout</v>
       </c>
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
@@ -11505,10 +11638,12 @@
       <c r="Y26" s="37"/>
       <c r="Z26" s="38"/>
       <c r="AA26" s="8" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>kubectl label pods secure-monolith 'secure=enabled'</v>
-      </c>
-      <c r="AB26" s="2"/>
+        <f ca="1">IFERROR(OFFSET(A26,0,MATCH("",B26:Z26,-1)),"")</f>
+        <v>kubectl rollout</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
@@ -11517,15 +11652,16 @@
       <c r="AH26" s="2"/>
       <c r="AI26" s="2"/>
       <c r="AJ26" s="1" t="s">
-        <v>282</v>
+        <v>323</v>
       </c>
       <c r="AK26" s="1"/>
     </row>
-    <row r="27" spans="2:37">
-      <c r="B27" s="36" t="s">
-        <v>277</v>
-      </c>
-      <c r="C27" s="37"/>
+    <row r="27" spans="2:37" outlineLevel="1">
+      <c r="B27" s="31"/>
+      <c r="C27" s="37" t="str">
+        <f>B$26&amp;" history "&amp;AC27&amp;"/"&amp;AE27</f>
+        <v>kubectl rollout history deployment/hello</v>
+      </c>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
@@ -11550,27 +11686,36 @@
       <c r="Y27" s="37"/>
       <c r="Z27" s="38"/>
       <c r="AA27" s="8" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>kubectl get pods secure-monolith --show-labels</v>
-      </c>
-      <c r="AB27" s="2"/>
-      <c r="AC27" s="2"/>
-      <c r="AD27" s="2"/>
-      <c r="AE27" s="2"/>
+        <f t="shared" ref="AA27" ca="1" si="7">IFERROR(OFFSET(A27,0,MATCH("",B27:Z27,-1)),"")</f>
+        <v>kubectl rollout history deployment/hello</v>
+      </c>
+      <c r="AB27" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC27" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD27" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE27" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="1" t="s">
-        <v>283</v>
+        <v>324</v>
       </c>
       <c r="AK27" s="1"/>
     </row>
-    <row r="28" spans="2:37">
-      <c r="B28" s="36" t="s">
-        <v>278</v>
-      </c>
-      <c r="C28" s="37"/>
+    <row r="28" spans="2:37" outlineLevel="1">
+      <c r="B28" s="31"/>
+      <c r="C28" s="37" t="str">
+        <f>B$26&amp;" pause "&amp;AC28&amp;"/"&amp;AE28</f>
+        <v>kubectl rollout pause deployment/hello</v>
+      </c>
       <c r="D28" s="37"/>
       <c r="E28" s="37"/>
       <c r="F28" s="37"/>
@@ -11595,23 +11740,38 @@
       <c r="Y28" s="37"/>
       <c r="Z28" s="38"/>
       <c r="AA28" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">kubectl describe services monolith </v>
-      </c>
-      <c r="AB28" s="2"/>
-      <c r="AC28" s="2"/>
-      <c r="AD28" s="2"/>
-      <c r="AE28" s="2"/>
+        <f t="shared" ref="AA28" ca="1" si="8">IFERROR(OFFSET(A28,0,MATCH("",B28:Z28,-1)),"")</f>
+        <v>kubectl rollout pause deployment/hello</v>
+      </c>
+      <c r="AB28" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC28" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD28" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE28" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
-      <c r="AJ28" s="1"/>
-      <c r="AK28" s="1"/>
-    </row>
-    <row r="29" spans="2:37">
-      <c r="B29" s="36"/>
-      <c r="C29" s="37"/>
+      <c r="AJ28" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AK28" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="2:37" outlineLevel="1">
+      <c r="B29" s="31"/>
+      <c r="C29" s="37" t="str">
+        <f>B$26&amp;" resume "&amp;AC29&amp;"/"&amp;AE29</f>
+        <v>kubectl rollout resume deployment/hello</v>
+      </c>
       <c r="D29" s="37"/>
       <c r="E29" s="37"/>
       <c r="F29" s="37"/>
@@ -11636,23 +11796,38 @@
       <c r="Y29" s="37"/>
       <c r="Z29" s="38"/>
       <c r="AA29" s="8" t="str">
-        <f t="shared" ref="AA29" ca="1" si="7">IFERROR(OFFSET(A29,0,MATCH("",B29:Z29,-1)),"")</f>
-        <v/>
-      </c>
-      <c r="AB29" s="2"/>
-      <c r="AC29" s="2"/>
-      <c r="AD29" s="2"/>
-      <c r="AE29" s="2"/>
+        <f t="shared" ref="AA29" ca="1" si="9">IFERROR(OFFSET(A29,0,MATCH("",B29:Z29,-1)),"")</f>
+        <v>kubectl rollout resume deployment/hello</v>
+      </c>
+      <c r="AB29" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC29" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD29" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE29" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
-      <c r="AJ29" s="1"/>
-      <c r="AK29" s="1"/>
-    </row>
-    <row r="30" spans="2:37">
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
+      <c r="AJ29" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AK29" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="30" spans="2:37" outlineLevel="1">
+      <c r="B30" s="31"/>
+      <c r="C30" s="37" t="str">
+        <f>B$26&amp;" status "&amp;AC30&amp;"/"&amp;AE30</f>
+        <v>kubectl rollout status deployment/hello</v>
+      </c>
       <c r="D30" s="37"/>
       <c r="E30" s="37"/>
       <c r="F30" s="37"/>
@@ -11677,23 +11852,36 @@
       <c r="Y30" s="37"/>
       <c r="Z30" s="38"/>
       <c r="AA30" s="8" t="str">
-        <f t="shared" ref="AA30" ca="1" si="8">IFERROR(OFFSET(A30,0,MATCH("",B30:Z30,-1)),"")</f>
-        <v/>
-      </c>
-      <c r="AB30" s="2"/>
-      <c r="AC30" s="2"/>
-      <c r="AD30" s="2"/>
-      <c r="AE30" s="2"/>
+        <f t="shared" ref="AA30" ca="1" si="10">IFERROR(OFFSET(A30,0,MATCH("",B30:Z30,-1)),"")</f>
+        <v>kubectl rollout status deployment/hello</v>
+      </c>
+      <c r="AB30" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC30" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD30" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE30" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
-      <c r="AJ30" s="1"/>
+      <c r="AJ30" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="AK30" s="1"/>
     </row>
-    <row r="31" spans="2:37">
-      <c r="B31" s="36"/>
-      <c r="C31" s="37"/>
+    <row r="31" spans="2:37" outlineLevel="1">
+      <c r="B31" s="31"/>
+      <c r="C31" s="37" t="str">
+        <f>B$26&amp;" undo "&amp;AC31&amp;"/"&amp;AE31</f>
+        <v>kubectl rollout undo deployment/hello</v>
+      </c>
       <c r="D31" s="37"/>
       <c r="E31" s="37"/>
       <c r="F31" s="37"/>
@@ -11718,22 +11906,32 @@
       <c r="Y31" s="37"/>
       <c r="Z31" s="38"/>
       <c r="AA31" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB31" s="2"/>
-      <c r="AC31" s="2"/>
-      <c r="AD31" s="2"/>
-      <c r="AE31" s="2"/>
+        <f t="shared" ref="AA31" ca="1" si="11">IFERROR(OFFSET(A31,0,MATCH("",B31:Z31,-1)),"")</f>
+        <v>kubectl rollout undo deployment/hello</v>
+      </c>
+      <c r="AB31" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC31" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AD31" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE31" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
-      <c r="AJ31" s="1"/>
+      <c r="AJ31" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" spans="2:37" outlineLevel="1">
-      <c r="B32" s="27"/>
+    <row r="32" spans="2:37">
+      <c r="B32" s="36"/>
       <c r="C32" s="37"/>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
@@ -11759,12 +11957,10 @@
       <c r="Y32" s="37"/>
       <c r="Z32" s="38"/>
       <c r="AA32" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IFERROR(OFFSET(A32,0,MATCH("",B32:Z32,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB32" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
@@ -11775,8 +11971,8 @@
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
     </row>
-    <row r="33" spans="2:37" outlineLevel="1">
-      <c r="B33" s="27"/>
+    <row r="33" spans="2:37">
+      <c r="B33" s="36"/>
       <c r="C33" s="37"/>
       <c r="D33" s="37"/>
       <c r="E33" s="37"/>
@@ -11805,9 +12001,7 @@
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="AB33" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
       <c r="AE33" s="2"/>
@@ -11818,9 +12012,9 @@
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" spans="2:37" outlineLevel="2">
-      <c r="B34" s="27"/>
-      <c r="C34" s="26"/>
+    <row r="34" spans="2:37">
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
       <c r="F34" s="37"/>
@@ -11848,9 +12042,7 @@
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="AB34" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
       <c r="AE34" s="2"/>
@@ -11858,12 +12050,14 @@
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
-      <c r="AJ34" s="1"/>
+      <c r="AJ34" s="1" t="s">
+        <v>306</v>
+      </c>
       <c r="AK34" s="1"/>
     </row>
-    <row r="35" spans="2:37" outlineLevel="2">
-      <c r="B35" s="27"/>
-      <c r="C35" s="26"/>
+    <row r="35" spans="2:37">
+      <c r="B35" s="36"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
@@ -11888,12 +12082,10 @@
       <c r="Y35" s="37"/>
       <c r="Z35" s="38"/>
       <c r="AA35" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="AA35:AA36" ca="1" si="12">IFERROR(OFFSET(A35,0,MATCH("",B35:Z35,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB35" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
       <c r="AD35" s="2"/>
       <c r="AE35" s="2"/>
@@ -11904,10 +12096,10 @@
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
-    <row r="36" spans="2:37" outlineLevel="3">
-      <c r="B36" s="27"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+    <row r="36" spans="2:37">
+      <c r="B36" s="36"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="37"/>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
@@ -11931,12 +12123,10 @@
       <c r="Y36" s="37"/>
       <c r="Z36" s="38"/>
       <c r="AA36" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
-      <c r="AB36" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
       <c r="AD36" s="2"/>
       <c r="AE36" s="2"/>
@@ -11947,10 +12137,10 @@
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
-    <row r="37" spans="2:37" outlineLevel="3">
-      <c r="B37" s="27"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+    <row r="37" spans="2:37">
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="37"/>
       <c r="F37" s="37"/>
       <c r="G37" s="37"/>
@@ -11974,12 +12164,10 @@
       <c r="Y37" s="37"/>
       <c r="Z37" s="38"/>
       <c r="AA37" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="AA37:AA39" ca="1" si="13">IFERROR(OFFSET(A37,0,MATCH("",B37:Z37,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB37" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
       <c r="AE37" s="2"/>
@@ -11990,11 +12178,11 @@
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" spans="2:37" outlineLevel="4">
-      <c r="B38" s="27"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
+    <row r="38" spans="2:37">
+      <c r="B38" s="36"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
       <c r="H38" s="37"/>
@@ -12017,12 +12205,10 @@
       <c r="Y38" s="37"/>
       <c r="Z38" s="38"/>
       <c r="AA38" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="AB38" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
       <c r="AD38" s="2"/>
       <c r="AE38" s="2"/>
@@ -12033,11 +12219,13 @@
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" spans="2:37" outlineLevel="4">
-      <c r="B39" s="27"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
+    <row r="39" spans="2:37" ht="39" customHeight="1">
+      <c r="B39" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="37"/>
       <c r="G39" s="37"/>
       <c r="H39" s="37"/>
@@ -12060,12 +12248,11 @@
       <c r="Y39" s="37"/>
       <c r="Z39" s="38"/>
       <c r="AA39" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB39" s="2" t="s">
-        <v>6</v>
-      </c>
+        <f t="shared" ca="1" si="13"/>
+        <v xml:space="preserve">kubectl get pods -o jsonpath --template='{range .items[*]}{.metadata.name}{"\t"}{"\t"}{.spec.containers[0].image}{"\n"}{end}'
+</v>
+      </c>
+      <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
       <c r="AD39" s="2"/>
       <c r="AE39" s="2"/>
@@ -12076,12 +12263,14 @@
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" spans="2:37" outlineLevel="5">
-      <c r="B40" s="27"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
+    <row r="40" spans="2:37">
+      <c r="B40" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
       <c r="G40" s="37"/>
       <c r="H40" s="37"/>
       <c r="I40" s="37"/>
@@ -12104,11 +12293,9 @@
       <c r="Z40" s="38"/>
       <c r="AA40" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB40" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>kubectl apply -f services/hello-blue.yaml</v>
+      </c>
+      <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
       <c r="AD40" s="2"/>
       <c r="AE40" s="2"/>
@@ -12119,12 +12306,12 @@
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" spans="2:37" outlineLevel="5">
-      <c r="B41" s="27"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
+    <row r="41" spans="2:37">
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
       <c r="G41" s="37"/>
       <c r="H41" s="37"/>
       <c r="I41" s="37"/>
@@ -12146,12 +12333,10 @@
       <c r="Y41" s="37"/>
       <c r="Z41" s="38"/>
       <c r="AA41" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IFERROR(OFFSET(A41,0,MATCH("",B41:Z41,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB41" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
       <c r="AD41" s="2"/>
       <c r="AE41" s="2"/>
@@ -12162,13 +12347,13 @@
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
     </row>
-    <row r="42" spans="2:37" outlineLevel="6">
-      <c r="B42" s="27"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
+    <row r="42" spans="2:37">
+      <c r="B42" s="36"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
       <c r="H42" s="37"/>
       <c r="I42" s="37"/>
       <c r="J42" s="37"/>
@@ -12189,12 +12374,10 @@
       <c r="Y42" s="37"/>
       <c r="Z42" s="38"/>
       <c r="AA42" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IFERROR(OFFSET(A42,0,MATCH("",B42:Z42,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB42" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
       <c r="AD42" s="2"/>
       <c r="AE42" s="2"/>
@@ -12205,13 +12388,13 @@
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
     </row>
-    <row r="43" spans="2:37" outlineLevel="6">
-      <c r="B43" s="27"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
+    <row r="43" spans="2:37">
+      <c r="B43" s="36"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
       <c r="H43" s="37"/>
       <c r="I43" s="37"/>
       <c r="J43" s="37"/>
@@ -12232,12 +12415,10 @@
       <c r="Y43" s="37"/>
       <c r="Z43" s="38"/>
       <c r="AA43" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IFERROR(OFFSET(A43,0,MATCH("",B43:Z43,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB43" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
       <c r="AD43" s="2"/>
       <c r="AE43" s="2"/>
@@ -12248,14 +12429,14 @@
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
     </row>
-    <row r="44" spans="2:37" outlineLevel="7">
-      <c r="B44" s="27"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
+    <row r="44" spans="2:37">
+      <c r="B44" s="36"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
       <c r="K44" s="37"/>
@@ -12275,12 +12456,10 @@
       <c r="Y44" s="37"/>
       <c r="Z44" s="38"/>
       <c r="AA44" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IFERROR(OFFSET(A44,0,MATCH("",B44:Z44,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB44" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
       <c r="AD44" s="2"/>
       <c r="AE44" s="2"/>
@@ -12291,14 +12470,14 @@
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" spans="2:37" outlineLevel="7">
-      <c r="B45" s="27"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
+    <row r="45" spans="2:37">
+      <c r="B45" s="36"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
       <c r="I45" s="37"/>
       <c r="J45" s="37"/>
       <c r="K45" s="37"/>
@@ -12318,12 +12497,10 @@
       <c r="Y45" s="37"/>
       <c r="Z45" s="38"/>
       <c r="AA45" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="AA45" ca="1" si="14">IFERROR(OFFSET(A45,0,MATCH("",B45:Z45,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB45" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
@@ -12334,13 +12511,13 @@
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
     </row>
-    <row r="46" spans="2:37" outlineLevel="6">
-      <c r="B46" s="27"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
+    <row r="46" spans="2:37">
+      <c r="B46" s="36"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
       <c r="H46" s="37"/>
       <c r="I46" s="37"/>
       <c r="J46" s="37"/>
@@ -12361,12 +12538,10 @@
       <c r="Y46" s="37"/>
       <c r="Z46" s="38"/>
       <c r="AA46" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="AA46" ca="1" si="15">IFERROR(OFFSET(A46,0,MATCH("",B46:Z46,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB46" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
@@ -12377,12 +12552,12 @@
       <c r="AJ46" s="1"/>
       <c r="AK46" s="1"/>
     </row>
-    <row r="47" spans="2:37" outlineLevel="5">
-      <c r="B47" s="27"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
+    <row r="47" spans="2:37">
+      <c r="B47" s="36"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
       <c r="G47" s="37"/>
       <c r="H47" s="37"/>
       <c r="I47" s="37"/>
@@ -12404,12 +12579,10 @@
       <c r="Y47" s="37"/>
       <c r="Z47" s="38"/>
       <c r="AA47" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="AA47" ca="1" si="16">IFERROR(OFFSET(A47,0,MATCH("",B47:Z47,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB47" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
       <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
@@ -12420,11 +12593,11 @@
       <c r="AJ47" s="1"/>
       <c r="AK47" s="1"/>
     </row>
-    <row r="48" spans="2:37" outlineLevel="4">
-      <c r="B48" s="27"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
+    <row r="48" spans="2:37">
+      <c r="B48" s="36"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
       <c r="F48" s="37"/>
       <c r="G48" s="37"/>
       <c r="H48" s="37"/>
@@ -12450,9 +12623,7 @@
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="AB48" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
       <c r="AD48" s="2"/>
       <c r="AE48" s="2"/>
@@ -12463,10 +12634,10 @@
       <c r="AJ48" s="1"/>
       <c r="AK48" s="1"/>
     </row>
-    <row r="49" spans="2:37" outlineLevel="3">
+    <row r="49" spans="2:37" outlineLevel="1">
       <c r="B49" s="27"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="37"/>
       <c r="F49" s="37"/>
       <c r="G49" s="37"/>
@@ -12506,9 +12677,9 @@
       <c r="AJ49" s="1"/>
       <c r="AK49" s="1"/>
     </row>
-    <row r="50" spans="2:37" outlineLevel="3">
+    <row r="50" spans="2:37" outlineLevel="1">
       <c r="B50" s="27"/>
-      <c r="C50" s="26"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="37"/>
       <c r="E50" s="37"/>
       <c r="F50" s="37"/>
@@ -12551,7 +12722,7 @@
     </row>
     <row r="51" spans="2:37" outlineLevel="2">
       <c r="B51" s="27"/>
-      <c r="C51" s="37"/>
+      <c r="C51" s="26"/>
       <c r="D51" s="37"/>
       <c r="E51" s="37"/>
       <c r="F51" s="37"/>
@@ -12592,9 +12763,9 @@
       <c r="AJ51" s="1"/>
       <c r="AK51" s="1"/>
     </row>
-    <row r="52" spans="2:37">
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
+    <row r="52" spans="2:37" outlineLevel="2">
+      <c r="B52" s="27"/>
+      <c r="C52" s="26"/>
       <c r="D52" s="37"/>
       <c r="E52" s="37"/>
       <c r="F52" s="37"/>
@@ -12635,9 +12806,752 @@
       <c r="AJ52" s="1"/>
       <c r="AK52" s="1"/>
     </row>
-    <row r="55" spans="2:37" ht="15" customHeight="1"/>
+    <row r="53" spans="2:37" outlineLevel="3">
+      <c r="B53" s="27"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
+      <c r="S53" s="37"/>
+      <c r="T53" s="37"/>
+      <c r="U53" s="37"/>
+      <c r="V53" s="37"/>
+      <c r="W53" s="37"/>
+      <c r="X53" s="37"/>
+      <c r="Y53" s="37"/>
+      <c r="Z53" s="38"/>
+      <c r="AA53" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="2"/>
+      <c r="AE53" s="2"/>
+      <c r="AF53" s="2"/>
+      <c r="AG53" s="2"/>
+      <c r="AH53" s="2"/>
+      <c r="AI53" s="2"/>
+      <c r="AJ53" s="1"/>
+      <c r="AK53" s="1"/>
+    </row>
+    <row r="54" spans="2:37" outlineLevel="3">
+      <c r="B54" s="27"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="37"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
+      <c r="S54" s="37"/>
+      <c r="T54" s="37"/>
+      <c r="U54" s="37"/>
+      <c r="V54" s="37"/>
+      <c r="W54" s="37"/>
+      <c r="X54" s="37"/>
+      <c r="Y54" s="37"/>
+      <c r="Z54" s="38"/>
+      <c r="AA54" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="2"/>
+      <c r="AE54" s="2"/>
+      <c r="AF54" s="2"/>
+      <c r="AG54" s="2"/>
+      <c r="AH54" s="2"/>
+      <c r="AI54" s="2"/>
+      <c r="AJ54" s="1"/>
+      <c r="AK54" s="1"/>
+    </row>
+    <row r="55" spans="2:37" outlineLevel="4">
+      <c r="B55" s="27"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+      <c r="S55" s="37"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="37"/>
+      <c r="V55" s="37"/>
+      <c r="W55" s="37"/>
+      <c r="X55" s="37"/>
+      <c r="Y55" s="37"/>
+      <c r="Z55" s="38"/>
+      <c r="AA55" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="2"/>
+      <c r="AF55" s="2"/>
+      <c r="AG55" s="2"/>
+      <c r="AH55" s="2"/>
+      <c r="AI55" s="2"/>
+      <c r="AJ55" s="1"/>
+      <c r="AK55" s="1"/>
+    </row>
+    <row r="56" spans="2:37" outlineLevel="4">
+      <c r="B56" s="27"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
+      <c r="O56" s="37"/>
+      <c r="P56" s="37"/>
+      <c r="Q56" s="37"/>
+      <c r="R56" s="37"/>
+      <c r="S56" s="37"/>
+      <c r="T56" s="37"/>
+      <c r="U56" s="37"/>
+      <c r="V56" s="37"/>
+      <c r="W56" s="37"/>
+      <c r="X56" s="37"/>
+      <c r="Y56" s="37"/>
+      <c r="Z56" s="38"/>
+      <c r="AA56" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="2"/>
+      <c r="AE56" s="2"/>
+      <c r="AF56" s="2"/>
+      <c r="AG56" s="2"/>
+      <c r="AH56" s="2"/>
+      <c r="AI56" s="2"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+    </row>
+    <row r="57" spans="2:37" outlineLevel="5">
+      <c r="B57" s="27"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="37"/>
+      <c r="O57" s="37"/>
+      <c r="P57" s="37"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
+      <c r="S57" s="37"/>
+      <c r="T57" s="37"/>
+      <c r="U57" s="37"/>
+      <c r="V57" s="37"/>
+      <c r="W57" s="37"/>
+      <c r="X57" s="37"/>
+      <c r="Y57" s="37"/>
+      <c r="Z57" s="38"/>
+      <c r="AA57" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="2"/>
+      <c r="AE57" s="2"/>
+      <c r="AF57" s="2"/>
+      <c r="AG57" s="2"/>
+      <c r="AH57" s="2"/>
+      <c r="AI57" s="2"/>
+      <c r="AJ57" s="1"/>
+      <c r="AK57" s="1"/>
+    </row>
+    <row r="58" spans="2:37" outlineLevel="5">
+      <c r="B58" s="27"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="37"/>
+      <c r="O58" s="37"/>
+      <c r="P58" s="37"/>
+      <c r="Q58" s="37"/>
+      <c r="R58" s="37"/>
+      <c r="S58" s="37"/>
+      <c r="T58" s="37"/>
+      <c r="U58" s="37"/>
+      <c r="V58" s="37"/>
+      <c r="W58" s="37"/>
+      <c r="X58" s="37"/>
+      <c r="Y58" s="37"/>
+      <c r="Z58" s="38"/>
+      <c r="AA58" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="2"/>
+      <c r="AE58" s="2"/>
+      <c r="AF58" s="2"/>
+      <c r="AG58" s="2"/>
+      <c r="AH58" s="2"/>
+      <c r="AI58" s="2"/>
+      <c r="AJ58" s="1"/>
+      <c r="AK58" s="1"/>
+    </row>
+    <row r="59" spans="2:37" outlineLevel="6">
+      <c r="B59" s="27"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="37"/>
+      <c r="O59" s="37"/>
+      <c r="P59" s="37"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
+      <c r="S59" s="37"/>
+      <c r="T59" s="37"/>
+      <c r="U59" s="37"/>
+      <c r="V59" s="37"/>
+      <c r="W59" s="37"/>
+      <c r="X59" s="37"/>
+      <c r="Y59" s="37"/>
+      <c r="Z59" s="38"/>
+      <c r="AA59" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="2"/>
+      <c r="AF59" s="2"/>
+      <c r="AG59" s="2"/>
+      <c r="AH59" s="2"/>
+      <c r="AI59" s="2"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1"/>
+    </row>
+    <row r="60" spans="2:37" outlineLevel="6">
+      <c r="B60" s="27"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="37"/>
+      <c r="O60" s="37"/>
+      <c r="P60" s="37"/>
+      <c r="Q60" s="37"/>
+      <c r="R60" s="37"/>
+      <c r="S60" s="37"/>
+      <c r="T60" s="37"/>
+      <c r="U60" s="37"/>
+      <c r="V60" s="37"/>
+      <c r="W60" s="37"/>
+      <c r="X60" s="37"/>
+      <c r="Y60" s="37"/>
+      <c r="Z60" s="38"/>
+      <c r="AA60" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC60" s="2"/>
+      <c r="AD60" s="2"/>
+      <c r="AE60" s="2"/>
+      <c r="AF60" s="2"/>
+      <c r="AG60" s="2"/>
+      <c r="AH60" s="2"/>
+      <c r="AI60" s="2"/>
+      <c r="AJ60" s="1"/>
+      <c r="AK60" s="1"/>
+    </row>
+    <row r="61" spans="2:37" outlineLevel="7">
+      <c r="B61" s="27"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="37"/>
+      <c r="O61" s="37"/>
+      <c r="P61" s="37"/>
+      <c r="Q61" s="37"/>
+      <c r="R61" s="37"/>
+      <c r="S61" s="37"/>
+      <c r="T61" s="37"/>
+      <c r="U61" s="37"/>
+      <c r="V61" s="37"/>
+      <c r="W61" s="37"/>
+      <c r="X61" s="37"/>
+      <c r="Y61" s="37"/>
+      <c r="Z61" s="38"/>
+      <c r="AA61" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="2"/>
+      <c r="AE61" s="2"/>
+      <c r="AF61" s="2"/>
+      <c r="AG61" s="2"/>
+      <c r="AH61" s="2"/>
+      <c r="AI61" s="2"/>
+      <c r="AJ61" s="1"/>
+      <c r="AK61" s="1"/>
+    </row>
+    <row r="62" spans="2:37" outlineLevel="7">
+      <c r="B62" s="27"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="37"/>
+      <c r="O62" s="37"/>
+      <c r="P62" s="37"/>
+      <c r="Q62" s="37"/>
+      <c r="R62" s="37"/>
+      <c r="S62" s="37"/>
+      <c r="T62" s="37"/>
+      <c r="U62" s="37"/>
+      <c r="V62" s="37"/>
+      <c r="W62" s="37"/>
+      <c r="X62" s="37"/>
+      <c r="Y62" s="37"/>
+      <c r="Z62" s="38"/>
+      <c r="AA62" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC62" s="2"/>
+      <c r="AD62" s="2"/>
+      <c r="AE62" s="2"/>
+      <c r="AF62" s="2"/>
+      <c r="AG62" s="2"/>
+      <c r="AH62" s="2"/>
+      <c r="AI62" s="2"/>
+      <c r="AJ62" s="1"/>
+      <c r="AK62" s="1"/>
+    </row>
+    <row r="63" spans="2:37" outlineLevel="6">
+      <c r="B63" s="27"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" s="37"/>
+      <c r="P63" s="37"/>
+      <c r="Q63" s="37"/>
+      <c r="R63" s="37"/>
+      <c r="S63" s="37"/>
+      <c r="T63" s="37"/>
+      <c r="U63" s="37"/>
+      <c r="V63" s="37"/>
+      <c r="W63" s="37"/>
+      <c r="X63" s="37"/>
+      <c r="Y63" s="37"/>
+      <c r="Z63" s="38"/>
+      <c r="AA63" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="2"/>
+      <c r="AE63" s="2"/>
+      <c r="AF63" s="2"/>
+      <c r="AG63" s="2"/>
+      <c r="AH63" s="2"/>
+      <c r="AI63" s="2"/>
+      <c r="AJ63" s="1"/>
+      <c r="AK63" s="1"/>
+    </row>
+    <row r="64" spans="2:37" outlineLevel="5">
+      <c r="B64" s="27"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" s="37"/>
+      <c r="P64" s="37"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="37"/>
+      <c r="S64" s="37"/>
+      <c r="T64" s="37"/>
+      <c r="U64" s="37"/>
+      <c r="V64" s="37"/>
+      <c r="W64" s="37"/>
+      <c r="X64" s="37"/>
+      <c r="Y64" s="37"/>
+      <c r="Z64" s="38"/>
+      <c r="AA64" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC64" s="2"/>
+      <c r="AD64" s="2"/>
+      <c r="AE64" s="2"/>
+      <c r="AF64" s="2"/>
+      <c r="AG64" s="2"/>
+      <c r="AH64" s="2"/>
+      <c r="AI64" s="2"/>
+      <c r="AJ64" s="1"/>
+      <c r="AK64" s="1"/>
+    </row>
+    <row r="65" spans="2:37" outlineLevel="4">
+      <c r="B65" s="27"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="37"/>
+      <c r="P65" s="37"/>
+      <c r="Q65" s="37"/>
+      <c r="R65" s="37"/>
+      <c r="S65" s="37"/>
+      <c r="T65" s="37"/>
+      <c r="U65" s="37"/>
+      <c r="V65" s="37"/>
+      <c r="W65" s="37"/>
+      <c r="X65" s="37"/>
+      <c r="Y65" s="37"/>
+      <c r="Z65" s="38"/>
+      <c r="AA65" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC65" s="2"/>
+      <c r="AD65" s="2"/>
+      <c r="AE65" s="2"/>
+      <c r="AF65" s="2"/>
+      <c r="AG65" s="2"/>
+      <c r="AH65" s="2"/>
+      <c r="AI65" s="2"/>
+      <c r="AJ65" s="1"/>
+      <c r="AK65" s="1"/>
+    </row>
+    <row r="66" spans="2:37" outlineLevel="3">
+      <c r="B66" s="27"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+      <c r="L66" s="37"/>
+      <c r="M66" s="37"/>
+      <c r="N66" s="37"/>
+      <c r="O66" s="37"/>
+      <c r="P66" s="37"/>
+      <c r="Q66" s="37"/>
+      <c r="R66" s="37"/>
+      <c r="S66" s="37"/>
+      <c r="T66" s="37"/>
+      <c r="U66" s="37"/>
+      <c r="V66" s="37"/>
+      <c r="W66" s="37"/>
+      <c r="X66" s="37"/>
+      <c r="Y66" s="37"/>
+      <c r="Z66" s="38"/>
+      <c r="AA66" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC66" s="2"/>
+      <c r="AD66" s="2"/>
+      <c r="AE66" s="2"/>
+      <c r="AF66" s="2"/>
+      <c r="AG66" s="2"/>
+      <c r="AH66" s="2"/>
+      <c r="AI66" s="2"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+    </row>
+    <row r="67" spans="2:37" outlineLevel="3">
+      <c r="B67" s="27"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="37"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="37"/>
+      <c r="Q67" s="37"/>
+      <c r="R67" s="37"/>
+      <c r="S67" s="37"/>
+      <c r="T67" s="37"/>
+      <c r="U67" s="37"/>
+      <c r="V67" s="37"/>
+      <c r="W67" s="37"/>
+      <c r="X67" s="37"/>
+      <c r="Y67" s="37"/>
+      <c r="Z67" s="38"/>
+      <c r="AA67" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC67" s="2"/>
+      <c r="AD67" s="2"/>
+      <c r="AE67" s="2"/>
+      <c r="AF67" s="2"/>
+      <c r="AG67" s="2"/>
+      <c r="AH67" s="2"/>
+      <c r="AI67" s="2"/>
+      <c r="AJ67" s="1"/>
+      <c r="AK67" s="1"/>
+    </row>
+    <row r="68" spans="2:37" outlineLevel="2">
+      <c r="B68" s="27"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+      <c r="S68" s="37"/>
+      <c r="T68" s="37"/>
+      <c r="U68" s="37"/>
+      <c r="V68" s="37"/>
+      <c r="W68" s="37"/>
+      <c r="X68" s="37"/>
+      <c r="Y68" s="37"/>
+      <c r="Z68" s="38"/>
+      <c r="AA68" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="2"/>
+      <c r="AE68" s="2"/>
+      <c r="AF68" s="2"/>
+      <c r="AG68" s="2"/>
+      <c r="AH68" s="2"/>
+      <c r="AI68" s="2"/>
+      <c r="AJ68" s="1"/>
+      <c r="AK68" s="1"/>
+    </row>
+    <row r="69" spans="2:37">
+      <c r="B69" s="36"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="37"/>
+      <c r="O69" s="37"/>
+      <c r="P69" s="37"/>
+      <c r="Q69" s="37"/>
+      <c r="R69" s="37"/>
+      <c r="S69" s="37"/>
+      <c r="T69" s="37"/>
+      <c r="U69" s="37"/>
+      <c r="V69" s="37"/>
+      <c r="W69" s="37"/>
+      <c r="X69" s="37"/>
+      <c r="Y69" s="37"/>
+      <c r="Z69" s="38"/>
+      <c r="AA69" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC69" s="2"/>
+      <c r="AD69" s="2"/>
+      <c r="AE69" s="2"/>
+      <c r="AF69" s="2"/>
+      <c r="AG69" s="2"/>
+      <c r="AH69" s="2"/>
+      <c r="AI69" s="2"/>
+      <c r="AJ69" s="1"/>
+      <c r="AK69" s="1"/>
+    </row>
+    <row r="72" spans="2:37" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="70">
+    <mergeCell ref="B39:Z39"/>
+    <mergeCell ref="B41:Z41"/>
+    <mergeCell ref="B42:Z42"/>
+    <mergeCell ref="B43:Z43"/>
+    <mergeCell ref="C23:Z23"/>
+    <mergeCell ref="C24:Z24"/>
+    <mergeCell ref="B26:Z26"/>
+    <mergeCell ref="C27:Z27"/>
+    <mergeCell ref="C28:Z28"/>
+    <mergeCell ref="C29:Z29"/>
+    <mergeCell ref="C30:Z30"/>
+    <mergeCell ref="C31:Z31"/>
     <mergeCell ref="B5:Z5"/>
     <mergeCell ref="C7:Z7"/>
     <mergeCell ref="D8:Z8"/>
@@ -12647,41 +13561,46 @@
     <mergeCell ref="B2:Z2"/>
     <mergeCell ref="B3:Z3"/>
     <mergeCell ref="B4:Z4"/>
-    <mergeCell ref="G40:Z40"/>
+    <mergeCell ref="G57:Z57"/>
     <mergeCell ref="B15:Z15"/>
     <mergeCell ref="B16:Z16"/>
-    <mergeCell ref="B31:Z31"/>
-    <mergeCell ref="C32:Z32"/>
-    <mergeCell ref="C33:Z33"/>
-    <mergeCell ref="D34:Z34"/>
-    <mergeCell ref="B30:Z30"/>
-    <mergeCell ref="B28:Z28"/>
-    <mergeCell ref="B29:Z29"/>
-    <mergeCell ref="B24:Z24"/>
-    <mergeCell ref="D35:Z35"/>
-    <mergeCell ref="E36:Z36"/>
-    <mergeCell ref="E37:Z37"/>
-    <mergeCell ref="F38:Z38"/>
-    <mergeCell ref="F39:Z39"/>
-    <mergeCell ref="B52:Z52"/>
-    <mergeCell ref="G41:Z41"/>
-    <mergeCell ref="H42:Z42"/>
-    <mergeCell ref="H43:Z43"/>
-    <mergeCell ref="I44:Z44"/>
-    <mergeCell ref="I45:Z45"/>
-    <mergeCell ref="H46:Z46"/>
-    <mergeCell ref="G47:Z47"/>
-    <mergeCell ref="F48:Z48"/>
-    <mergeCell ref="E49:Z49"/>
-    <mergeCell ref="D50:Z50"/>
-    <mergeCell ref="C51:Z51"/>
+    <mergeCell ref="B48:Z48"/>
+    <mergeCell ref="C49:Z49"/>
+    <mergeCell ref="C50:Z50"/>
+    <mergeCell ref="D51:Z51"/>
+    <mergeCell ref="B47:Z47"/>
     <mergeCell ref="B25:Z25"/>
-    <mergeCell ref="B26:Z26"/>
-    <mergeCell ref="B27:Z27"/>
+    <mergeCell ref="B46:Z46"/>
+    <mergeCell ref="B35:Z35"/>
+    <mergeCell ref="B44:Z44"/>
+    <mergeCell ref="B40:Z40"/>
+    <mergeCell ref="B45:Z45"/>
+    <mergeCell ref="B37:Z37"/>
+    <mergeCell ref="B38:Z38"/>
+    <mergeCell ref="D52:Z52"/>
+    <mergeCell ref="E53:Z53"/>
+    <mergeCell ref="E54:Z54"/>
+    <mergeCell ref="F55:Z55"/>
+    <mergeCell ref="F56:Z56"/>
+    <mergeCell ref="B69:Z69"/>
+    <mergeCell ref="G58:Z58"/>
+    <mergeCell ref="H59:Z59"/>
+    <mergeCell ref="H60:Z60"/>
+    <mergeCell ref="I61:Z61"/>
+    <mergeCell ref="I62:Z62"/>
+    <mergeCell ref="H63:Z63"/>
+    <mergeCell ref="G64:Z64"/>
+    <mergeCell ref="F65:Z65"/>
+    <mergeCell ref="E66:Z66"/>
+    <mergeCell ref="D67:Z67"/>
+    <mergeCell ref="C68:Z68"/>
+    <mergeCell ref="B36:Z36"/>
+    <mergeCell ref="B22:Z22"/>
+    <mergeCell ref="B32:Z32"/>
     <mergeCell ref="B20:Z20"/>
     <mergeCell ref="B21:Z21"/>
-    <mergeCell ref="B22:Z22"/>
-    <mergeCell ref="B23:Z23"/>
+    <mergeCell ref="B33:Z33"/>
+    <mergeCell ref="B34:Z34"/>
     <mergeCell ref="B14:Z14"/>
     <mergeCell ref="B17:Z17"/>
     <mergeCell ref="C19:Z19"/>

</xml_diff>

<commit_message>
Added more gcloud functions commands.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
@@ -337,7 +337,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="445">
   <si>
     <t>Details</t>
   </si>
@@ -1641,6 +1641,58 @@
   </si>
   <si>
     <t>$REGION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcloud beta functions logs read helloWorld
+</t>
+  </si>
+  <si>
+    <t>gcloud functions</t>
+  </si>
+  <si>
+    <t>Manages  Google Cloud Functions.</t>
+  </si>
+  <si>
+    <t>Creates or updates a Google Cloud Function.</t>
+  </si>
+  <si>
+    <t>Function name:</t>
+  </si>
+  <si>
+    <t>helloWorld</t>
+  </si>
+  <si>
+    <t>Stage bucket:</t>
+  </si>
+  <si>
+    <t>ioso_bucket2</t>
+  </si>
+  <si>
+    <t>Creates a Google Cloud Function.</t>
+  </si>
+  <si>
+    <t>Trigger topic:</t>
+  </si>
+  <si>
+    <t>hello_world</t>
+  </si>
+  <si>
+    <t>Function:</t>
+  </si>
+  <si>
+    <t>Displays details of a Google Cloud Function.</t>
+  </si>
+  <si>
+    <t>Triggers the execution of a Google Cloud Function.</t>
+  </si>
+  <si>
+    <t>Data:</t>
+  </si>
+  <si>
+    <t>{"message":"Hello World!"}</t>
+  </si>
+  <si>
+    <t>Displays log entries produced by Google Cloud Functions.</t>
   </si>
 </sst>
 </file>
@@ -2288,30 +2340,30 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AQ143"/>
+  <dimension ref="B1:AQ150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121:Z121"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="26" width="2.85546875" customWidth="1"/>
-    <col min="27" max="27" width="20.5703125" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="24.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="14.140625" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="19.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="15.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="43" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="13.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="42.140625" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="10.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="14.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="8.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="16.140625" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="7.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="24.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="14.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="19.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="15.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="43" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="13.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="42.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="10.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="14.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="8.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="16.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="7.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="42" max="42" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="46" customWidth="1"/>
     <col min="44" max="44" width="68.140625" customWidth="1"/>
@@ -2400,7 +2452,7 @@
       <c r="Y2" s="43"/>
       <c r="Z2" s="44"/>
       <c r="AA2" s="8" t="str">
-        <f t="shared" ref="AA2:AA129" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
+        <f t="shared" ref="AA2:AA136" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
         <v>gcloud compute</v>
       </c>
       <c r="AB2" s="2" t="s">
@@ -8802,9 +8854,9 @@
       </c>
       <c r="AQ114" s="1"/>
     </row>
-    <row r="115" spans="2:43" ht="60" collapsed="1">
+    <row r="115" spans="2:43">
       <c r="B115" s="42" t="s">
-        <v>357</v>
+        <v>429</v>
       </c>
       <c r="C115" s="43"/>
       <c r="D115" s="43"/>
@@ -8831,8 +8883,8 @@
       <c r="Y115" s="43"/>
       <c r="Z115" s="44"/>
       <c r="AA115" s="8" t="str">
-        <f t="shared" ref="AA115:AA116" ca="1" si="41">IFERROR(OFFSET(A115,0,MATCH("",B115:Z115,-1)),"")</f>
-        <v>gcloud docker</v>
+        <f t="shared" ref="AA115:AA117" ca="1" si="41">IFERROR(OFFSET(A115,0,MATCH("",B115:Z115,-1)),"")</f>
+        <v>gcloud functions</v>
       </c>
       <c r="AB115" s="2" t="s">
         <v>6</v>
@@ -8851,17 +8903,15 @@
       <c r="AN115" s="2"/>
       <c r="AO115" s="2"/>
       <c r="AP115" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="AQ115" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="116" spans="2:43" ht="30" hidden="1" outlineLevel="1">
-      <c r="B116" s="33"/>
+        <v>430</v>
+      </c>
+      <c r="AQ115" s="1"/>
+    </row>
+    <row r="116" spans="2:43" outlineLevel="1">
+      <c r="B116" s="36"/>
       <c r="C116" s="39" t="str">
-        <f>B$115&amp;" -- push "&amp;AC116&amp;"/"&amp;AE116&amp;"/"&amp;AG116</f>
-        <v>gcloud docker -- push gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
+        <f>B$115&amp;" deploy"</f>
+        <v>gcloud functions deploy</v>
       </c>
       <c r="D116" s="40"/>
       <c r="E116" s="40"/>
@@ -8888,26 +8938,16 @@
       <c r="Z116" s="41"/>
       <c r="AA116" s="8" t="str">
         <f t="shared" ca="1" si="41"/>
-        <v>gcloud docker -- push gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
-      </c>
-      <c r="AB116" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="AC116" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="AD116" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE116" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="AF116" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="AG116" s="5" t="s">
-        <v>360</v>
-      </c>
+        <v>gcloud functions deploy</v>
+      </c>
+      <c r="AB116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC116" s="2"/>
+      <c r="AD116" s="2"/>
+      <c r="AE116" s="2"/>
+      <c r="AF116" s="2"/>
+      <c r="AG116" s="2"/>
       <c r="AH116" s="2"/>
       <c r="AI116" s="2"/>
       <c r="AJ116" s="2"/>
@@ -8917,17 +8957,17 @@
       <c r="AN116" s="2"/>
       <c r="AO116" s="2"/>
       <c r="AP116" s="1" t="s">
-        <v>367</v>
+        <v>431</v>
       </c>
       <c r="AQ116" s="1"/>
     </row>
-    <row r="117" spans="2:43" ht="30" hidden="1" outlineLevel="1">
-      <c r="B117" s="33"/>
-      <c r="C117" s="39" t="str">
-        <f>B$115&amp;" -- pull "&amp;AC117&amp;"/"&amp;AE117&amp;"/"&amp;AG117</f>
-        <v>gcloud docker -- pull gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
-      </c>
-      <c r="D117" s="40"/>
+    <row r="117" spans="2:43" ht="30" outlineLevel="2">
+      <c r="B117" s="36"/>
+      <c r="C117" s="37"/>
+      <c r="D117" s="39" t="str">
+        <f>C$116&amp;" "&amp;AC117&amp;" --stage-bucket "&amp;AE117&amp;IF(ISBLANK(AG117),""," --trigger-topic "&amp;AG117)</f>
+        <v>gcloud functions deploy helloWorld --stage-bucket ioso_bucket2 --trigger-topic hello_world</v>
+      </c>
       <c r="E117" s="40"/>
       <c r="F117" s="40"/>
       <c r="G117" s="40"/>
@@ -8951,26 +8991,26 @@
       <c r="Y117" s="40"/>
       <c r="Z117" s="41"/>
       <c r="AA117" s="8" t="str">
-        <f t="shared" ref="AA117:AA123" ca="1" si="42">IFERROR(OFFSET(A117,0,MATCH("",B117:Z117,-1)),"")</f>
-        <v>gcloud docker -- pull gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
-      </c>
-      <c r="AB117" s="22" t="s">
-        <v>358</v>
+        <f t="shared" ca="1" si="41"/>
+        <v>gcloud functions deploy helloWorld --stage-bucket ioso_bucket2 --trigger-topic hello_world</v>
+      </c>
+      <c r="AB117" s="21" t="s">
+        <v>432</v>
       </c>
       <c r="AC117" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="AD117" s="22" t="s">
-        <v>147</v>
+        <v>433</v>
+      </c>
+      <c r="AD117" s="21" t="s">
+        <v>434</v>
       </c>
       <c r="AE117" s="5" t="s">
-        <v>361</v>
+        <v>435</v>
       </c>
       <c r="AF117" s="2" t="s">
-        <v>261</v>
+        <v>437</v>
       </c>
       <c r="AG117" s="5" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="AH117" s="2"/>
       <c r="AI117" s="2"/>
@@ -8981,44 +9021,49 @@
       <c r="AN117" s="2"/>
       <c r="AO117" s="2"/>
       <c r="AP117" s="1" t="s">
-        <v>363</v>
+        <v>436</v>
       </c>
       <c r="AQ117" s="1"/>
     </row>
-    <row r="118" spans="2:43">
-      <c r="B118" s="42"/>
-      <c r="C118" s="43"/>
-      <c r="D118" s="43"/>
-      <c r="E118" s="43"/>
-      <c r="F118" s="43"/>
-      <c r="G118" s="43"/>
-      <c r="H118" s="43"/>
-      <c r="I118" s="43"/>
-      <c r="J118" s="43"/>
-      <c r="K118" s="43"/>
-      <c r="L118" s="43"/>
-      <c r="M118" s="43"/>
-      <c r="N118" s="43"/>
-      <c r="O118" s="43"/>
-      <c r="P118" s="43"/>
-      <c r="Q118" s="43"/>
-      <c r="R118" s="43"/>
-      <c r="S118" s="43"/>
-      <c r="T118" s="43"/>
-      <c r="U118" s="43"/>
-      <c r="V118" s="43"/>
-      <c r="W118" s="43"/>
-      <c r="X118" s="43"/>
-      <c r="Y118" s="43"/>
-      <c r="Z118" s="44"/>
+    <row r="118" spans="2:43" outlineLevel="1">
+      <c r="B118" s="36"/>
+      <c r="C118" s="39" t="str">
+        <f>B$115&amp;" describe "&amp;AC118</f>
+        <v>gcloud functions describe helloWorld</v>
+      </c>
+      <c r="D118" s="40"/>
+      <c r="E118" s="40"/>
+      <c r="F118" s="40"/>
+      <c r="G118" s="40"/>
+      <c r="H118" s="40"/>
+      <c r="I118" s="40"/>
+      <c r="J118" s="40"/>
+      <c r="K118" s="40"/>
+      <c r="L118" s="40"/>
+      <c r="M118" s="40"/>
+      <c r="N118" s="40"/>
+      <c r="O118" s="40"/>
+      <c r="P118" s="40"/>
+      <c r="Q118" s="40"/>
+      <c r="R118" s="40"/>
+      <c r="S118" s="40"/>
+      <c r="T118" s="40"/>
+      <c r="U118" s="40"/>
+      <c r="V118" s="40"/>
+      <c r="W118" s="40"/>
+      <c r="X118" s="40"/>
+      <c r="Y118" s="40"/>
+      <c r="Z118" s="41"/>
       <c r="AA118" s="8" t="str">
-        <f t="shared" ref="AA118" ca="1" si="43">IFERROR(OFFSET(A118,0,MATCH("",B118:Z118,-1)),"")</f>
-        <v/>
-      </c>
-      <c r="AB118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC118" s="2"/>
+        <f t="shared" ref="AA118" ca="1" si="42">IFERROR(OFFSET(A118,0,MATCH("",B118:Z118,-1)),"")</f>
+        <v>gcloud functions describe helloWorld</v>
+      </c>
+      <c r="AB118" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="AC118" s="5" t="s">
+        <v>433</v>
+      </c>
       <c r="AD118" s="2"/>
       <c r="AE118" s="2"/>
       <c r="AF118" s="2"/>
@@ -9031,13 +9076,18 @@
       <c r="AM118" s="2"/>
       <c r="AN118" s="2"/>
       <c r="AO118" s="2"/>
-      <c r="AP118" s="1"/>
+      <c r="AP118" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="AQ118" s="1"/>
     </row>
-    <row r="119" spans="2:43">
-      <c r="B119" s="42"/>
-      <c r="C119" s="43"/>
-      <c r="D119" s="39"/>
+    <row r="119" spans="2:43" ht="30" outlineLevel="1">
+      <c r="B119" s="36"/>
+      <c r="C119" s="39" t="str">
+        <f>B$115&amp;" call "&amp;AC119&amp;IF(ISBLANK(AE119),""," --data "&amp;"'"&amp;AE119&amp;"'")</f>
+        <v>gcloud functions call helloWorld --data '{"message":"Hello World!"}'</v>
+      </c>
+      <c r="D119" s="40"/>
       <c r="E119" s="40"/>
       <c r="F119" s="40"/>
       <c r="G119" s="40"/>
@@ -9060,13 +9110,22 @@
       <c r="X119" s="40"/>
       <c r="Y119" s="40"/>
       <c r="Z119" s="41"/>
-      <c r="AA119" s="8"/>
-      <c r="AB119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC119" s="2"/>
-      <c r="AD119" s="2"/>
-      <c r="AE119" s="2"/>
+      <c r="AA119" s="8" t="str">
+        <f t="shared" ref="AA119" ca="1" si="43">IFERROR(OFFSET(A119,0,MATCH("",B119:Z119,-1)),"")</f>
+        <v>gcloud functions call helloWorld --data '{"message":"Hello World!"}'</v>
+      </c>
+      <c r="AB119" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="AC119" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="AD119" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="AE119" s="5" t="s">
+        <v>443</v>
+      </c>
       <c r="AF119" s="2"/>
       <c r="AG119" s="2"/>
       <c r="AH119" s="2"/>
@@ -9077,38 +9136,43 @@
       <c r="AM119" s="2"/>
       <c r="AN119" s="2"/>
       <c r="AO119" s="2"/>
-      <c r="AP119" s="1"/>
+      <c r="AP119" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="AQ119" s="1"/>
     </row>
-    <row r="120" spans="2:43">
-      <c r="B120" s="42"/>
-      <c r="C120" s="43"/>
-      <c r="D120" s="43"/>
-      <c r="E120" s="43"/>
-      <c r="F120" s="43"/>
-      <c r="G120" s="43"/>
-      <c r="H120" s="43"/>
-      <c r="I120" s="43"/>
-      <c r="J120" s="43"/>
-      <c r="K120" s="43"/>
-      <c r="L120" s="43"/>
-      <c r="M120" s="43"/>
-      <c r="N120" s="43"/>
-      <c r="O120" s="43"/>
-      <c r="P120" s="43"/>
-      <c r="Q120" s="43"/>
-      <c r="R120" s="43"/>
-      <c r="S120" s="43"/>
-      <c r="T120" s="43"/>
-      <c r="U120" s="43"/>
-      <c r="V120" s="43"/>
-      <c r="W120" s="43"/>
-      <c r="X120" s="43"/>
-      <c r="Y120" s="43"/>
-      <c r="Z120" s="44"/>
+    <row r="120" spans="2:43" outlineLevel="1">
+      <c r="B120" s="36"/>
+      <c r="C120" s="39" t="str">
+        <f>B$115&amp;" logs"</f>
+        <v>gcloud functions logs</v>
+      </c>
+      <c r="D120" s="40"/>
+      <c r="E120" s="40"/>
+      <c r="F120" s="40"/>
+      <c r="G120" s="40"/>
+      <c r="H120" s="40"/>
+      <c r="I120" s="40"/>
+      <c r="J120" s="40"/>
+      <c r="K120" s="40"/>
+      <c r="L120" s="40"/>
+      <c r="M120" s="40"/>
+      <c r="N120" s="40"/>
+      <c r="O120" s="40"/>
+      <c r="P120" s="40"/>
+      <c r="Q120" s="40"/>
+      <c r="R120" s="40"/>
+      <c r="S120" s="40"/>
+      <c r="T120" s="40"/>
+      <c r="U120" s="40"/>
+      <c r="V120" s="40"/>
+      <c r="W120" s="40"/>
+      <c r="X120" s="40"/>
+      <c r="Y120" s="40"/>
+      <c r="Z120" s="41"/>
       <c r="AA120" s="8" t="str">
-        <f t="shared" ref="AA120" ca="1" si="44">IFERROR(OFFSET(A120,0,MATCH("",B120:Z120,-1)),"")</f>
-        <v/>
+        <f t="shared" ref="AA120:AA121" ca="1" si="44">IFERROR(OFFSET(A120,0,MATCH("",B120:Z120,-1)),"")</f>
+        <v>gcloud functions logs</v>
       </c>
       <c r="AB120" s="2" t="s">
         <v>6</v>
@@ -9126,13 +9190,18 @@
       <c r="AM120" s="2"/>
       <c r="AN120" s="2"/>
       <c r="AO120" s="2"/>
-      <c r="AP120" s="1"/>
+      <c r="AP120" s="1" t="s">
+        <v>444</v>
+      </c>
       <c r="AQ120" s="1"/>
     </row>
-    <row r="121" spans="2:43">
-      <c r="B121" s="42"/>
-      <c r="C121" s="43"/>
-      <c r="D121" s="39"/>
+    <row r="121" spans="2:43" outlineLevel="2">
+      <c r="B121" s="36"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="39" t="str">
+        <f>C$120&amp;" read "&amp;AC121</f>
+        <v>gcloud functions logs read helloWorld</v>
+      </c>
       <c r="E121" s="40"/>
       <c r="F121" s="40"/>
       <c r="G121" s="40"/>
@@ -9155,11 +9224,16 @@
       <c r="X121" s="40"/>
       <c r="Y121" s="40"/>
       <c r="Z121" s="41"/>
-      <c r="AA121" s="8"/>
-      <c r="AB121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC121" s="2"/>
+      <c r="AA121" s="8" t="str">
+        <f t="shared" ca="1" si="44"/>
+        <v>gcloud functions logs read helloWorld</v>
+      </c>
+      <c r="AB121" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="AC121" s="5" t="s">
+        <v>433</v>
+      </c>
       <c r="AD121" s="2"/>
       <c r="AE121" s="2"/>
       <c r="AF121" s="2"/>
@@ -9172,36 +9246,43 @@
       <c r="AM121" s="2"/>
       <c r="AN121" s="2"/>
       <c r="AO121" s="2"/>
-      <c r="AP121" s="1"/>
+      <c r="AP121" s="1" t="s">
+        <v>444</v>
+      </c>
       <c r="AQ121" s="1"/>
     </row>
-    <row r="122" spans="2:43">
-      <c r="B122" s="42"/>
+    <row r="122" spans="2:43" ht="60" collapsed="1">
+      <c r="B122" s="42" t="s">
+        <v>357</v>
+      </c>
       <c r="C122" s="43"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="40"/>
-      <c r="F122" s="40"/>
-      <c r="G122" s="40"/>
-      <c r="H122" s="40"/>
-      <c r="I122" s="40"/>
-      <c r="J122" s="40"/>
-      <c r="K122" s="40"/>
-      <c r="L122" s="40"/>
-      <c r="M122" s="40"/>
-      <c r="N122" s="40"/>
-      <c r="O122" s="40"/>
-      <c r="P122" s="40"/>
-      <c r="Q122" s="40"/>
-      <c r="R122" s="40"/>
-      <c r="S122" s="40"/>
-      <c r="T122" s="40"/>
-      <c r="U122" s="40"/>
-      <c r="V122" s="40"/>
-      <c r="W122" s="40"/>
-      <c r="X122" s="40"/>
-      <c r="Y122" s="40"/>
-      <c r="Z122" s="41"/>
-      <c r="AA122" s="8"/>
+      <c r="D122" s="43"/>
+      <c r="E122" s="43"/>
+      <c r="F122" s="43"/>
+      <c r="G122" s="43"/>
+      <c r="H122" s="43"/>
+      <c r="I122" s="43"/>
+      <c r="J122" s="43"/>
+      <c r="K122" s="43"/>
+      <c r="L122" s="43"/>
+      <c r="M122" s="43"/>
+      <c r="N122" s="43"/>
+      <c r="O122" s="43"/>
+      <c r="P122" s="43"/>
+      <c r="Q122" s="43"/>
+      <c r="R122" s="43"/>
+      <c r="S122" s="43"/>
+      <c r="T122" s="43"/>
+      <c r="U122" s="43"/>
+      <c r="V122" s="43"/>
+      <c r="W122" s="43"/>
+      <c r="X122" s="43"/>
+      <c r="Y122" s="43"/>
+      <c r="Z122" s="44"/>
+      <c r="AA122" s="8" t="str">
+        <f t="shared" ref="AA122:AA123" ca="1" si="45">IFERROR(OFFSET(A122,0,MATCH("",B122:Z122,-1)),"")</f>
+        <v>gcloud docker</v>
+      </c>
       <c r="AB122" s="2" t="s">
         <v>6</v>
       </c>
@@ -9218,47 +9299,64 @@
       <c r="AM122" s="2"/>
       <c r="AN122" s="2"/>
       <c r="AO122" s="2"/>
-      <c r="AP122" s="1"/>
-      <c r="AQ122" s="1"/>
-    </row>
-    <row r="123" spans="2:43">
-      <c r="B123" s="42"/>
-      <c r="C123" s="43"/>
-      <c r="D123" s="43"/>
-      <c r="E123" s="43"/>
-      <c r="F123" s="43"/>
-      <c r="G123" s="43"/>
-      <c r="H123" s="43"/>
-      <c r="I123" s="43"/>
-      <c r="J123" s="43"/>
-      <c r="K123" s="43"/>
-      <c r="L123" s="43"/>
-      <c r="M123" s="43"/>
-      <c r="N123" s="43"/>
-      <c r="O123" s="43"/>
-      <c r="P123" s="43"/>
-      <c r="Q123" s="43"/>
-      <c r="R123" s="43"/>
-      <c r="S123" s="43"/>
-      <c r="T123" s="43"/>
-      <c r="U123" s="43"/>
-      <c r="V123" s="43"/>
-      <c r="W123" s="43"/>
-      <c r="X123" s="43"/>
-      <c r="Y123" s="43"/>
-      <c r="Z123" s="44"/>
+      <c r="AP122" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AQ122" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="123" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+      <c r="B123" s="33"/>
+      <c r="C123" s="39" t="str">
+        <f>B$122&amp;" -- push "&amp;AC123&amp;"/"&amp;AE123&amp;"/"&amp;AG123</f>
+        <v>gcloud docker -- push gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
+      </c>
+      <c r="D123" s="40"/>
+      <c r="E123" s="40"/>
+      <c r="F123" s="40"/>
+      <c r="G123" s="40"/>
+      <c r="H123" s="40"/>
+      <c r="I123" s="40"/>
+      <c r="J123" s="40"/>
+      <c r="K123" s="40"/>
+      <c r="L123" s="40"/>
+      <c r="M123" s="40"/>
+      <c r="N123" s="40"/>
+      <c r="O123" s="40"/>
+      <c r="P123" s="40"/>
+      <c r="Q123" s="40"/>
+      <c r="R123" s="40"/>
+      <c r="S123" s="40"/>
+      <c r="T123" s="40"/>
+      <c r="U123" s="40"/>
+      <c r="V123" s="40"/>
+      <c r="W123" s="40"/>
+      <c r="X123" s="40"/>
+      <c r="Y123" s="40"/>
+      <c r="Z123" s="41"/>
       <c r="AA123" s="8" t="str">
-        <f t="shared" ca="1" si="42"/>
-        <v/>
-      </c>
-      <c r="AB123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC123" s="2"/>
-      <c r="AD123" s="2"/>
-      <c r="AE123" s="2"/>
-      <c r="AF123" s="2"/>
-      <c r="AG123" s="2"/>
+        <f t="shared" ca="1" si="45"/>
+        <v>gcloud docker -- push gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
+      </c>
+      <c r="AB123" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="AC123" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD123" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE123" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF123" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AG123" s="5" t="s">
+        <v>360</v>
+      </c>
       <c r="AH123" s="2"/>
       <c r="AI123" s="2"/>
       <c r="AJ123" s="2"/>
@@ -9267,13 +9365,18 @@
       <c r="AM123" s="2"/>
       <c r="AN123" s="2"/>
       <c r="AO123" s="2"/>
-      <c r="AP123" s="1"/>
+      <c r="AP123" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="AQ123" s="1"/>
     </row>
-    <row r="124" spans="2:43">
-      <c r="B124" s="42"/>
-      <c r="C124" s="43"/>
-      <c r="D124" s="39"/>
+    <row r="124" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+      <c r="B124" s="33"/>
+      <c r="C124" s="39" t="str">
+        <f>B$122&amp;" -- pull "&amp;AC124&amp;"/"&amp;AE124&amp;"/"&amp;AG124</f>
+        <v>gcloud docker -- pull gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
+      </c>
+      <c r="D124" s="40"/>
       <c r="E124" s="40"/>
       <c r="F124" s="40"/>
       <c r="G124" s="40"/>
@@ -9296,15 +9399,28 @@
       <c r="X124" s="40"/>
       <c r="Y124" s="40"/>
       <c r="Z124" s="41"/>
-      <c r="AA124" s="8"/>
-      <c r="AB124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC124" s="2"/>
-      <c r="AD124" s="2"/>
-      <c r="AE124" s="2"/>
-      <c r="AF124" s="2"/>
-      <c r="AG124" s="2"/>
+      <c r="AA124" s="8" t="str">
+        <f t="shared" ref="AA124:AA130" ca="1" si="46">IFERROR(OFFSET(A124,0,MATCH("",B124:Z124,-1)),"")</f>
+        <v>gcloud docker -- pull gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
+      </c>
+      <c r="AB124" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="AC124" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD124" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE124" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF124" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AG124" s="5" t="s">
+        <v>360</v>
+      </c>
       <c r="AH124" s="2"/>
       <c r="AI124" s="2"/>
       <c r="AJ124" s="2"/>
@@ -9313,36 +9429,41 @@
       <c r="AM124" s="2"/>
       <c r="AN124" s="2"/>
       <c r="AO124" s="2"/>
-      <c r="AP124" s="1"/>
+      <c r="AP124" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="AQ124" s="1"/>
     </row>
     <row r="125" spans="2:43">
       <c r="B125" s="42"/>
       <c r="C125" s="43"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="40"/>
-      <c r="F125" s="40"/>
-      <c r="G125" s="40"/>
-      <c r="H125" s="40"/>
-      <c r="I125" s="40"/>
-      <c r="J125" s="40"/>
-      <c r="K125" s="40"/>
-      <c r="L125" s="40"/>
-      <c r="M125" s="40"/>
-      <c r="N125" s="40"/>
-      <c r="O125" s="40"/>
-      <c r="P125" s="40"/>
-      <c r="Q125" s="40"/>
-      <c r="R125" s="40"/>
-      <c r="S125" s="40"/>
-      <c r="T125" s="40"/>
-      <c r="U125" s="40"/>
-      <c r="V125" s="40"/>
-      <c r="W125" s="40"/>
-      <c r="X125" s="40"/>
-      <c r="Y125" s="40"/>
-      <c r="Z125" s="41"/>
-      <c r="AA125" s="8"/>
+      <c r="D125" s="43"/>
+      <c r="E125" s="43"/>
+      <c r="F125" s="43"/>
+      <c r="G125" s="43"/>
+      <c r="H125" s="43"/>
+      <c r="I125" s="43"/>
+      <c r="J125" s="43"/>
+      <c r="K125" s="43"/>
+      <c r="L125" s="43"/>
+      <c r="M125" s="43"/>
+      <c r="N125" s="43"/>
+      <c r="O125" s="43"/>
+      <c r="P125" s="43"/>
+      <c r="Q125" s="43"/>
+      <c r="R125" s="43"/>
+      <c r="S125" s="43"/>
+      <c r="T125" s="43"/>
+      <c r="U125" s="43"/>
+      <c r="V125" s="43"/>
+      <c r="W125" s="43"/>
+      <c r="X125" s="43"/>
+      <c r="Y125" s="43"/>
+      <c r="Z125" s="44"/>
+      <c r="AA125" s="8" t="str">
+        <f t="shared" ref="AA125" ca="1" si="47">IFERROR(OFFSET(A125,0,MATCH("",B125:Z125,-1)),"")</f>
+        <v/>
+      </c>
       <c r="AB125" s="2" t="s">
         <v>6</v>
       </c>
@@ -9365,33 +9486,30 @@
     <row r="126" spans="2:43">
       <c r="B126" s="42"/>
       <c r="C126" s="43"/>
-      <c r="D126" s="43"/>
-      <c r="E126" s="43"/>
-      <c r="F126" s="43"/>
-      <c r="G126" s="43"/>
-      <c r="H126" s="43"/>
-      <c r="I126" s="43"/>
-      <c r="J126" s="43"/>
-      <c r="K126" s="43"/>
-      <c r="L126" s="43"/>
-      <c r="M126" s="43"/>
-      <c r="N126" s="43"/>
-      <c r="O126" s="43"/>
-      <c r="P126" s="43"/>
-      <c r="Q126" s="43"/>
-      <c r="R126" s="43"/>
-      <c r="S126" s="43"/>
-      <c r="T126" s="43"/>
-      <c r="U126" s="43"/>
-      <c r="V126" s="43"/>
-      <c r="W126" s="43"/>
-      <c r="X126" s="43"/>
-      <c r="Y126" s="43"/>
-      <c r="Z126" s="44"/>
-      <c r="AA126" s="8" t="str">
-        <f t="shared" ref="AA126" ca="1" si="45">IFERROR(OFFSET(A126,0,MATCH("",B126:Z126,-1)),"")</f>
-        <v/>
-      </c>
+      <c r="D126" s="39"/>
+      <c r="E126" s="40"/>
+      <c r="F126" s="40"/>
+      <c r="G126" s="40"/>
+      <c r="H126" s="40"/>
+      <c r="I126" s="40"/>
+      <c r="J126" s="40"/>
+      <c r="K126" s="40"/>
+      <c r="L126" s="40"/>
+      <c r="M126" s="40"/>
+      <c r="N126" s="40"/>
+      <c r="O126" s="40"/>
+      <c r="P126" s="40"/>
+      <c r="Q126" s="40"/>
+      <c r="R126" s="40"/>
+      <c r="S126" s="40"/>
+      <c r="T126" s="40"/>
+      <c r="U126" s="40"/>
+      <c r="V126" s="40"/>
+      <c r="W126" s="40"/>
+      <c r="X126" s="40"/>
+      <c r="Y126" s="40"/>
+      <c r="Z126" s="41"/>
+      <c r="AA126" s="8"/>
       <c r="AB126" s="2" t="s">
         <v>6</v>
       </c>
@@ -9411,33 +9529,36 @@
       <c r="AP126" s="1"/>
       <c r="AQ126" s="1"/>
     </row>
-    <row r="127" spans="2:43">
+    <row r="127" spans="2:43" ht="30" customHeight="1">
       <c r="B127" s="42"/>
       <c r="C127" s="43"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="40"/>
-      <c r="F127" s="40"/>
-      <c r="G127" s="40"/>
-      <c r="H127" s="40"/>
-      <c r="I127" s="40"/>
-      <c r="J127" s="40"/>
-      <c r="K127" s="40"/>
-      <c r="L127" s="40"/>
-      <c r="M127" s="40"/>
-      <c r="N127" s="40"/>
-      <c r="O127" s="40"/>
-      <c r="P127" s="40"/>
-      <c r="Q127" s="40"/>
-      <c r="R127" s="40"/>
-      <c r="S127" s="40"/>
-      <c r="T127" s="40"/>
-      <c r="U127" s="40"/>
-      <c r="V127" s="40"/>
-      <c r="W127" s="40"/>
-      <c r="X127" s="40"/>
-      <c r="Y127" s="40"/>
-      <c r="Z127" s="41"/>
-      <c r="AA127" s="8"/>
+      <c r="D127" s="43"/>
+      <c r="E127" s="43"/>
+      <c r="F127" s="43"/>
+      <c r="G127" s="43"/>
+      <c r="H127" s="43"/>
+      <c r="I127" s="43"/>
+      <c r="J127" s="43"/>
+      <c r="K127" s="43"/>
+      <c r="L127" s="43"/>
+      <c r="M127" s="43"/>
+      <c r="N127" s="43"/>
+      <c r="O127" s="43"/>
+      <c r="P127" s="43"/>
+      <c r="Q127" s="43"/>
+      <c r="R127" s="43"/>
+      <c r="S127" s="43"/>
+      <c r="T127" s="43"/>
+      <c r="U127" s="43"/>
+      <c r="V127" s="43"/>
+      <c r="W127" s="43"/>
+      <c r="X127" s="43"/>
+      <c r="Y127" s="43"/>
+      <c r="Z127" s="44"/>
+      <c r="AA127" s="8" t="str">
+        <f t="shared" ref="AA127:AA128" ca="1" si="48">IFERROR(OFFSET(A127,0,MATCH("",B127:Z127,-1)),"")</f>
+        <v/>
+      </c>
       <c r="AB127" s="2" t="s">
         <v>6</v>
       </c>
@@ -9483,7 +9604,10 @@
       <c r="X128" s="40"/>
       <c r="Y128" s="40"/>
       <c r="Z128" s="41"/>
-      <c r="AA128" s="8"/>
+      <c r="AA128" s="8" t="str">
+        <f t="shared" ca="1" si="48"/>
+        <v/>
+      </c>
       <c r="AB128" s="2" t="s">
         <v>6</v>
       </c>
@@ -9503,36 +9627,33 @@
       <c r="AP128" s="1"/>
       <c r="AQ128" s="1"/>
     </row>
-    <row r="129" spans="2:43" collapsed="1">
+    <row r="129" spans="2:43" ht="30.75" customHeight="1">
       <c r="B129" s="42"/>
       <c r="C129" s="43"/>
-      <c r="D129" s="43"/>
-      <c r="E129" s="43"/>
-      <c r="F129" s="43"/>
-      <c r="G129" s="43"/>
-      <c r="H129" s="43"/>
-      <c r="I129" s="43"/>
-      <c r="J129" s="43"/>
-      <c r="K129" s="43"/>
-      <c r="L129" s="43"/>
-      <c r="M129" s="43"/>
-      <c r="N129" s="43"/>
-      <c r="O129" s="43"/>
-      <c r="P129" s="43"/>
-      <c r="Q129" s="43"/>
-      <c r="R129" s="43"/>
-      <c r="S129" s="43"/>
-      <c r="T129" s="43"/>
-      <c r="U129" s="43"/>
-      <c r="V129" s="43"/>
-      <c r="W129" s="43"/>
-      <c r="X129" s="43"/>
-      <c r="Y129" s="43"/>
-      <c r="Z129" s="44"/>
-      <c r="AA129" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
+      <c r="D129" s="39"/>
+      <c r="E129" s="40"/>
+      <c r="F129" s="40"/>
+      <c r="G129" s="40"/>
+      <c r="H129" s="40"/>
+      <c r="I129" s="40"/>
+      <c r="J129" s="40"/>
+      <c r="K129" s="40"/>
+      <c r="L129" s="40"/>
+      <c r="M129" s="40"/>
+      <c r="N129" s="40"/>
+      <c r="O129" s="40"/>
+      <c r="P129" s="40"/>
+      <c r="Q129" s="40"/>
+      <c r="R129" s="40"/>
+      <c r="S129" s="40"/>
+      <c r="T129" s="40"/>
+      <c r="U129" s="40"/>
+      <c r="V129" s="40"/>
+      <c r="W129" s="40"/>
+      <c r="X129" s="40"/>
+      <c r="Y129" s="40"/>
+      <c r="Z129" s="41"/>
+      <c r="AA129" s="8"/>
       <c r="AB129" s="2" t="s">
         <v>6</v>
       </c>
@@ -9553,7 +9674,9 @@
       <c r="AQ129" s="1"/>
     </row>
     <row r="130" spans="2:43">
-      <c r="B130" s="42"/>
+      <c r="B130" s="42" t="s">
+        <v>428</v>
+      </c>
       <c r="C130" s="43"/>
       <c r="D130" s="43"/>
       <c r="E130" s="43"/>
@@ -9578,8 +9701,10 @@
       <c r="X130" s="43"/>
       <c r="Y130" s="43"/>
       <c r="Z130" s="44"/>
-      <c r="AA130" s="8" t="s">
-        <v>199</v>
+      <c r="AA130" s="8" t="str">
+        <f t="shared" ca="1" si="46"/>
+        <v xml:space="preserve">gcloud beta functions logs read helloWorld
+</v>
       </c>
       <c r="AB130" s="2" t="s">
         <v>6</v>
@@ -9600,35 +9725,33 @@
       <c r="AP130" s="1"/>
       <c r="AQ130" s="1"/>
     </row>
-    <row r="131" spans="2:43" outlineLevel="1">
-      <c r="B131" s="15"/>
+    <row r="131" spans="2:43">
+      <c r="B131" s="42"/>
       <c r="C131" s="43"/>
-      <c r="D131" s="43"/>
-      <c r="E131" s="43"/>
-      <c r="F131" s="43"/>
-      <c r="G131" s="43"/>
-      <c r="H131" s="43"/>
-      <c r="I131" s="43"/>
-      <c r="J131" s="43"/>
-      <c r="K131" s="43"/>
-      <c r="L131" s="43"/>
-      <c r="M131" s="43"/>
-      <c r="N131" s="43"/>
-      <c r="O131" s="43"/>
-      <c r="P131" s="43"/>
-      <c r="Q131" s="43"/>
-      <c r="R131" s="43"/>
-      <c r="S131" s="43"/>
-      <c r="T131" s="43"/>
-      <c r="U131" s="43"/>
-      <c r="V131" s="43"/>
-      <c r="W131" s="43"/>
-      <c r="X131" s="43"/>
-      <c r="Y131" s="43"/>
-      <c r="Z131" s="44"/>
-      <c r="AA131" s="8" t="s">
-        <v>199</v>
-      </c>
+      <c r="D131" s="39"/>
+      <c r="E131" s="40"/>
+      <c r="F131" s="40"/>
+      <c r="G131" s="40"/>
+      <c r="H131" s="40"/>
+      <c r="I131" s="40"/>
+      <c r="J131" s="40"/>
+      <c r="K131" s="40"/>
+      <c r="L131" s="40"/>
+      <c r="M131" s="40"/>
+      <c r="N131" s="40"/>
+      <c r="O131" s="40"/>
+      <c r="P131" s="40"/>
+      <c r="Q131" s="40"/>
+      <c r="R131" s="40"/>
+      <c r="S131" s="40"/>
+      <c r="T131" s="40"/>
+      <c r="U131" s="40"/>
+      <c r="V131" s="40"/>
+      <c r="W131" s="40"/>
+      <c r="X131" s="40"/>
+      <c r="Y131" s="40"/>
+      <c r="Z131" s="41"/>
+      <c r="AA131" s="8"/>
       <c r="AB131" s="2" t="s">
         <v>6</v>
       </c>
@@ -9648,35 +9771,33 @@
       <c r="AP131" s="1"/>
       <c r="AQ131" s="1"/>
     </row>
-    <row r="132" spans="2:43" outlineLevel="1">
-      <c r="B132" s="3"/>
+    <row r="132" spans="2:43">
+      <c r="B132" s="42"/>
       <c r="C132" s="43"/>
-      <c r="D132" s="43"/>
-      <c r="E132" s="43"/>
-      <c r="F132" s="43"/>
-      <c r="G132" s="43"/>
-      <c r="H132" s="43"/>
-      <c r="I132" s="43"/>
-      <c r="J132" s="43"/>
-      <c r="K132" s="43"/>
-      <c r="L132" s="43"/>
-      <c r="M132" s="43"/>
-      <c r="N132" s="43"/>
-      <c r="O132" s="43"/>
-      <c r="P132" s="43"/>
-      <c r="Q132" s="43"/>
-      <c r="R132" s="43"/>
-      <c r="S132" s="43"/>
-      <c r="T132" s="43"/>
-      <c r="U132" s="43"/>
-      <c r="V132" s="43"/>
-      <c r="W132" s="43"/>
-      <c r="X132" s="43"/>
-      <c r="Y132" s="43"/>
-      <c r="Z132" s="44"/>
-      <c r="AA132" s="8" t="s">
-        <v>199</v>
-      </c>
+      <c r="D132" s="39"/>
+      <c r="E132" s="40"/>
+      <c r="F132" s="40"/>
+      <c r="G132" s="40"/>
+      <c r="H132" s="40"/>
+      <c r="I132" s="40"/>
+      <c r="J132" s="40"/>
+      <c r="K132" s="40"/>
+      <c r="L132" s="40"/>
+      <c r="M132" s="40"/>
+      <c r="N132" s="40"/>
+      <c r="O132" s="40"/>
+      <c r="P132" s="40"/>
+      <c r="Q132" s="40"/>
+      <c r="R132" s="40"/>
+      <c r="S132" s="40"/>
+      <c r="T132" s="40"/>
+      <c r="U132" s="40"/>
+      <c r="V132" s="40"/>
+      <c r="W132" s="40"/>
+      <c r="X132" s="40"/>
+      <c r="Y132" s="40"/>
+      <c r="Z132" s="41"/>
+      <c r="AA132" s="8"/>
       <c r="AB132" s="2" t="s">
         <v>6</v>
       </c>
@@ -9696,9 +9817,9 @@
       <c r="AP132" s="1"/>
       <c r="AQ132" s="1"/>
     </row>
-    <row r="133" spans="2:43" outlineLevel="2">
-      <c r="B133" s="3"/>
-      <c r="C133" s="4"/>
+    <row r="133" spans="2:43">
+      <c r="B133" s="42"/>
+      <c r="C133" s="43"/>
       <c r="D133" s="43"/>
       <c r="E133" s="43"/>
       <c r="F133" s="43"/>
@@ -9722,8 +9843,9 @@
       <c r="X133" s="43"/>
       <c r="Y133" s="43"/>
       <c r="Z133" s="44"/>
-      <c r="AA133" s="8" t="s">
-        <v>199</v>
+      <c r="AA133" s="8" t="str">
+        <f t="shared" ref="AA133" ca="1" si="49">IFERROR(OFFSET(A133,0,MATCH("",B133:Z133,-1)),"")</f>
+        <v/>
       </c>
       <c r="AB133" s="2" t="s">
         <v>6</v>
@@ -9744,35 +9866,33 @@
       <c r="AP133" s="1"/>
       <c r="AQ133" s="1"/>
     </row>
-    <row r="134" spans="2:43" outlineLevel="2">
-      <c r="B134" s="3"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="43"/>
-      <c r="E134" s="43"/>
-      <c r="F134" s="43"/>
-      <c r="G134" s="43"/>
-      <c r="H134" s="43"/>
-      <c r="I134" s="43"/>
-      <c r="J134" s="43"/>
-      <c r="K134" s="43"/>
-      <c r="L134" s="43"/>
-      <c r="M134" s="43"/>
-      <c r="N134" s="43"/>
-      <c r="O134" s="43"/>
-      <c r="P134" s="43"/>
-      <c r="Q134" s="43"/>
-      <c r="R134" s="43"/>
-      <c r="S134" s="43"/>
-      <c r="T134" s="43"/>
-      <c r="U134" s="43"/>
-      <c r="V134" s="43"/>
-      <c r="W134" s="43"/>
-      <c r="X134" s="43"/>
-      <c r="Y134" s="43"/>
-      <c r="Z134" s="44"/>
-      <c r="AA134" s="8" t="s">
-        <v>199</v>
-      </c>
+    <row r="134" spans="2:43">
+      <c r="B134" s="42"/>
+      <c r="C134" s="43"/>
+      <c r="D134" s="39"/>
+      <c r="E134" s="40"/>
+      <c r="F134" s="40"/>
+      <c r="G134" s="40"/>
+      <c r="H134" s="40"/>
+      <c r="I134" s="40"/>
+      <c r="J134" s="40"/>
+      <c r="K134" s="40"/>
+      <c r="L134" s="40"/>
+      <c r="M134" s="40"/>
+      <c r="N134" s="40"/>
+      <c r="O134" s="40"/>
+      <c r="P134" s="40"/>
+      <c r="Q134" s="40"/>
+      <c r="R134" s="40"/>
+      <c r="S134" s="40"/>
+      <c r="T134" s="40"/>
+      <c r="U134" s="40"/>
+      <c r="V134" s="40"/>
+      <c r="W134" s="40"/>
+      <c r="X134" s="40"/>
+      <c r="Y134" s="40"/>
+      <c r="Z134" s="41"/>
+      <c r="AA134" s="8"/>
       <c r="AB134" s="2" t="s">
         <v>6</v>
       </c>
@@ -9792,35 +9912,33 @@
       <c r="AP134" s="1"/>
       <c r="AQ134" s="1"/>
     </row>
-    <row r="135" spans="2:43" outlineLevel="3">
-      <c r="B135" s="3"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="43"/>
-      <c r="F135" s="43"/>
-      <c r="G135" s="43"/>
-      <c r="H135" s="43"/>
-      <c r="I135" s="43"/>
-      <c r="J135" s="43"/>
-      <c r="K135" s="43"/>
-      <c r="L135" s="43"/>
-      <c r="M135" s="43"/>
-      <c r="N135" s="43"/>
-      <c r="O135" s="43"/>
-      <c r="P135" s="43"/>
-      <c r="Q135" s="43"/>
-      <c r="R135" s="43"/>
-      <c r="S135" s="43"/>
-      <c r="T135" s="43"/>
-      <c r="U135" s="43"/>
-      <c r="V135" s="43"/>
-      <c r="W135" s="43"/>
-      <c r="X135" s="43"/>
-      <c r="Y135" s="43"/>
-      <c r="Z135" s="44"/>
-      <c r="AA135" s="8" t="s">
-        <v>199</v>
-      </c>
+    <row r="135" spans="2:43">
+      <c r="B135" s="42"/>
+      <c r="C135" s="43"/>
+      <c r="D135" s="39"/>
+      <c r="E135" s="40"/>
+      <c r="F135" s="40"/>
+      <c r="G135" s="40"/>
+      <c r="H135" s="40"/>
+      <c r="I135" s="40"/>
+      <c r="J135" s="40"/>
+      <c r="K135" s="40"/>
+      <c r="L135" s="40"/>
+      <c r="M135" s="40"/>
+      <c r="N135" s="40"/>
+      <c r="O135" s="40"/>
+      <c r="P135" s="40"/>
+      <c r="Q135" s="40"/>
+      <c r="R135" s="40"/>
+      <c r="S135" s="40"/>
+      <c r="T135" s="40"/>
+      <c r="U135" s="40"/>
+      <c r="V135" s="40"/>
+      <c r="W135" s="40"/>
+      <c r="X135" s="40"/>
+      <c r="Y135" s="40"/>
+      <c r="Z135" s="41"/>
+      <c r="AA135" s="8"/>
       <c r="AB135" s="2" t="s">
         <v>6</v>
       </c>
@@ -9840,10 +9958,10 @@
       <c r="AP135" s="1"/>
       <c r="AQ135" s="1"/>
     </row>
-    <row r="136" spans="2:43" outlineLevel="3">
-      <c r="B136" s="3"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
+    <row r="136" spans="2:43" collapsed="1">
+      <c r="B136" s="42"/>
+      <c r="C136" s="43"/>
+      <c r="D136" s="43"/>
       <c r="E136" s="43"/>
       <c r="F136" s="43"/>
       <c r="G136" s="43"/>
@@ -9866,8 +9984,9 @@
       <c r="X136" s="43"/>
       <c r="Y136" s="43"/>
       <c r="Z136" s="44"/>
-      <c r="AA136" s="8" t="s">
-        <v>199</v>
+      <c r="AA136" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
       </c>
       <c r="AB136" s="2" t="s">
         <v>6</v>
@@ -9888,11 +10007,11 @@
       <c r="AP136" s="1"/>
       <c r="AQ136" s="1"/>
     </row>
-    <row r="137" spans="2:43" outlineLevel="4">
-      <c r="B137" s="3"/>
-      <c r="C137" s="4"/>
-      <c r="D137" s="4"/>
-      <c r="E137" s="4"/>
+    <row r="137" spans="2:43">
+      <c r="B137" s="42"/>
+      <c r="C137" s="43"/>
+      <c r="D137" s="43"/>
+      <c r="E137" s="43"/>
       <c r="F137" s="43"/>
       <c r="G137" s="43"/>
       <c r="H137" s="43"/>
@@ -9936,11 +10055,11 @@
       <c r="AP137" s="1"/>
       <c r="AQ137" s="1"/>
     </row>
-    <row r="138" spans="2:43" outlineLevel="4">
-      <c r="B138" s="3"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
-      <c r="E138" s="4"/>
+    <row r="138" spans="2:43" outlineLevel="1">
+      <c r="B138" s="15"/>
+      <c r="C138" s="43"/>
+      <c r="D138" s="43"/>
+      <c r="E138" s="43"/>
       <c r="F138" s="43"/>
       <c r="G138" s="43"/>
       <c r="H138" s="43"/>
@@ -9984,12 +10103,12 @@
       <c r="AP138" s="1"/>
       <c r="AQ138" s="1"/>
     </row>
-    <row r="139" spans="2:43" outlineLevel="5">
+    <row r="139" spans="2:43" outlineLevel="1">
       <c r="B139" s="3"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="4"/>
-      <c r="F139" s="4"/>
+      <c r="C139" s="43"/>
+      <c r="D139" s="43"/>
+      <c r="E139" s="43"/>
+      <c r="F139" s="43"/>
       <c r="G139" s="43"/>
       <c r="H139" s="43"/>
       <c r="I139" s="43"/>
@@ -10032,12 +10151,12 @@
       <c r="AP139" s="1"/>
       <c r="AQ139" s="1"/>
     </row>
-    <row r="140" spans="2:43" outlineLevel="5">
+    <row r="140" spans="2:43" outlineLevel="2">
       <c r="B140" s="3"/>
       <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-      <c r="F140" s="4"/>
+      <c r="D140" s="43"/>
+      <c r="E140" s="43"/>
+      <c r="F140" s="43"/>
       <c r="G140" s="43"/>
       <c r="H140" s="43"/>
       <c r="I140" s="43"/>
@@ -10080,13 +10199,13 @@
       <c r="AP140" s="1"/>
       <c r="AQ140" s="1"/>
     </row>
-    <row r="141" spans="2:43" outlineLevel="6">
+    <row r="141" spans="2:43" outlineLevel="2">
       <c r="B141" s="3"/>
       <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
-      <c r="E141" s="4"/>
-      <c r="F141" s="4"/>
-      <c r="G141" s="4"/>
+      <c r="D141" s="43"/>
+      <c r="E141" s="43"/>
+      <c r="F141" s="43"/>
+      <c r="G141" s="43"/>
       <c r="H141" s="43"/>
       <c r="I141" s="43"/>
       <c r="J141" s="43"/>
@@ -10128,13 +10247,13 @@
       <c r="AP141" s="1"/>
       <c r="AQ141" s="1"/>
     </row>
-    <row r="142" spans="2:43" outlineLevel="6">
+    <row r="142" spans="2:43" outlineLevel="3">
       <c r="B142" s="3"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
-      <c r="E142" s="4"/>
-      <c r="F142" s="4"/>
-      <c r="G142" s="4"/>
+      <c r="E142" s="43"/>
+      <c r="F142" s="43"/>
+      <c r="G142" s="43"/>
       <c r="H142" s="43"/>
       <c r="I142" s="43"/>
       <c r="J142" s="43"/>
@@ -10176,10 +10295,10 @@
       <c r="AP142" s="1"/>
       <c r="AQ142" s="1"/>
     </row>
-    <row r="143" spans="2:43">
-      <c r="B143" s="42"/>
-      <c r="C143" s="43"/>
-      <c r="D143" s="43"/>
+    <row r="143" spans="2:43" outlineLevel="3">
+      <c r="B143" s="3"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
       <c r="E143" s="43"/>
       <c r="F143" s="43"/>
       <c r="G143" s="43"/>
@@ -10224,12 +10343,355 @@
       <c r="AP143" s="1"/>
       <c r="AQ143" s="1"/>
     </row>
+    <row r="144" spans="2:43" outlineLevel="4">
+      <c r="B144" s="3"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="43"/>
+      <c r="G144" s="43"/>
+      <c r="H144" s="43"/>
+      <c r="I144" s="43"/>
+      <c r="J144" s="43"/>
+      <c r="K144" s="43"/>
+      <c r="L144" s="43"/>
+      <c r="M144" s="43"/>
+      <c r="N144" s="43"/>
+      <c r="O144" s="43"/>
+      <c r="P144" s="43"/>
+      <c r="Q144" s="43"/>
+      <c r="R144" s="43"/>
+      <c r="S144" s="43"/>
+      <c r="T144" s="43"/>
+      <c r="U144" s="43"/>
+      <c r="V144" s="43"/>
+      <c r="W144" s="43"/>
+      <c r="X144" s="43"/>
+      <c r="Y144" s="43"/>
+      <c r="Z144" s="44"/>
+      <c r="AA144" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB144" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC144" s="2"/>
+      <c r="AD144" s="2"/>
+      <c r="AE144" s="2"/>
+      <c r="AF144" s="2"/>
+      <c r="AG144" s="2"/>
+      <c r="AH144" s="2"/>
+      <c r="AI144" s="2"/>
+      <c r="AJ144" s="2"/>
+      <c r="AK144" s="2"/>
+      <c r="AL144" s="2"/>
+      <c r="AM144" s="2"/>
+      <c r="AN144" s="2"/>
+      <c r="AO144" s="2"/>
+      <c r="AP144" s="1"/>
+      <c r="AQ144" s="1"/>
+    </row>
+    <row r="145" spans="2:43" outlineLevel="4">
+      <c r="B145" s="3"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="43"/>
+      <c r="G145" s="43"/>
+      <c r="H145" s="43"/>
+      <c r="I145" s="43"/>
+      <c r="J145" s="43"/>
+      <c r="K145" s="43"/>
+      <c r="L145" s="43"/>
+      <c r="M145" s="43"/>
+      <c r="N145" s="43"/>
+      <c r="O145" s="43"/>
+      <c r="P145" s="43"/>
+      <c r="Q145" s="43"/>
+      <c r="R145" s="43"/>
+      <c r="S145" s="43"/>
+      <c r="T145" s="43"/>
+      <c r="U145" s="43"/>
+      <c r="V145" s="43"/>
+      <c r="W145" s="43"/>
+      <c r="X145" s="43"/>
+      <c r="Y145" s="43"/>
+      <c r="Z145" s="44"/>
+      <c r="AA145" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB145" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC145" s="2"/>
+      <c r="AD145" s="2"/>
+      <c r="AE145" s="2"/>
+      <c r="AF145" s="2"/>
+      <c r="AG145" s="2"/>
+      <c r="AH145" s="2"/>
+      <c r="AI145" s="2"/>
+      <c r="AJ145" s="2"/>
+      <c r="AK145" s="2"/>
+      <c r="AL145" s="2"/>
+      <c r="AM145" s="2"/>
+      <c r="AN145" s="2"/>
+      <c r="AO145" s="2"/>
+      <c r="AP145" s="1"/>
+      <c r="AQ145" s="1"/>
+    </row>
+    <row r="146" spans="2:43" outlineLevel="5">
+      <c r="B146" s="3"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="4"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="4"/>
+      <c r="G146" s="43"/>
+      <c r="H146" s="43"/>
+      <c r="I146" s="43"/>
+      <c r="J146" s="43"/>
+      <c r="K146" s="43"/>
+      <c r="L146" s="43"/>
+      <c r="M146" s="43"/>
+      <c r="N146" s="43"/>
+      <c r="O146" s="43"/>
+      <c r="P146" s="43"/>
+      <c r="Q146" s="43"/>
+      <c r="R146" s="43"/>
+      <c r="S146" s="43"/>
+      <c r="T146" s="43"/>
+      <c r="U146" s="43"/>
+      <c r="V146" s="43"/>
+      <c r="W146" s="43"/>
+      <c r="X146" s="43"/>
+      <c r="Y146" s="43"/>
+      <c r="Z146" s="44"/>
+      <c r="AA146" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB146" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC146" s="2"/>
+      <c r="AD146" s="2"/>
+      <c r="AE146" s="2"/>
+      <c r="AF146" s="2"/>
+      <c r="AG146" s="2"/>
+      <c r="AH146" s="2"/>
+      <c r="AI146" s="2"/>
+      <c r="AJ146" s="2"/>
+      <c r="AK146" s="2"/>
+      <c r="AL146" s="2"/>
+      <c r="AM146" s="2"/>
+      <c r="AN146" s="2"/>
+      <c r="AO146" s="2"/>
+      <c r="AP146" s="1"/>
+      <c r="AQ146" s="1"/>
+    </row>
+    <row r="147" spans="2:43" outlineLevel="5">
+      <c r="B147" s="3"/>
+      <c r="C147" s="4"/>
+      <c r="D147" s="4"/>
+      <c r="E147" s="4"/>
+      <c r="F147" s="4"/>
+      <c r="G147" s="43"/>
+      <c r="H147" s="43"/>
+      <c r="I147" s="43"/>
+      <c r="J147" s="43"/>
+      <c r="K147" s="43"/>
+      <c r="L147" s="43"/>
+      <c r="M147" s="43"/>
+      <c r="N147" s="43"/>
+      <c r="O147" s="43"/>
+      <c r="P147" s="43"/>
+      <c r="Q147" s="43"/>
+      <c r="R147" s="43"/>
+      <c r="S147" s="43"/>
+      <c r="T147" s="43"/>
+      <c r="U147" s="43"/>
+      <c r="V147" s="43"/>
+      <c r="W147" s="43"/>
+      <c r="X147" s="43"/>
+      <c r="Y147" s="43"/>
+      <c r="Z147" s="44"/>
+      <c r="AA147" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB147" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC147" s="2"/>
+      <c r="AD147" s="2"/>
+      <c r="AE147" s="2"/>
+      <c r="AF147" s="2"/>
+      <c r="AG147" s="2"/>
+      <c r="AH147" s="2"/>
+      <c r="AI147" s="2"/>
+      <c r="AJ147" s="2"/>
+      <c r="AK147" s="2"/>
+      <c r="AL147" s="2"/>
+      <c r="AM147" s="2"/>
+      <c r="AN147" s="2"/>
+      <c r="AO147" s="2"/>
+      <c r="AP147" s="1"/>
+      <c r="AQ147" s="1"/>
+    </row>
+    <row r="148" spans="2:43" outlineLevel="6">
+      <c r="B148" s="3"/>
+      <c r="C148" s="4"/>
+      <c r="D148" s="4"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
+      <c r="G148" s="4"/>
+      <c r="H148" s="43"/>
+      <c r="I148" s="43"/>
+      <c r="J148" s="43"/>
+      <c r="K148" s="43"/>
+      <c r="L148" s="43"/>
+      <c r="M148" s="43"/>
+      <c r="N148" s="43"/>
+      <c r="O148" s="43"/>
+      <c r="P148" s="43"/>
+      <c r="Q148" s="43"/>
+      <c r="R148" s="43"/>
+      <c r="S148" s="43"/>
+      <c r="T148" s="43"/>
+      <c r="U148" s="43"/>
+      <c r="V148" s="43"/>
+      <c r="W148" s="43"/>
+      <c r="X148" s="43"/>
+      <c r="Y148" s="43"/>
+      <c r="Z148" s="44"/>
+      <c r="AA148" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB148" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC148" s="2"/>
+      <c r="AD148" s="2"/>
+      <c r="AE148" s="2"/>
+      <c r="AF148" s="2"/>
+      <c r="AG148" s="2"/>
+      <c r="AH148" s="2"/>
+      <c r="AI148" s="2"/>
+      <c r="AJ148" s="2"/>
+      <c r="AK148" s="2"/>
+      <c r="AL148" s="2"/>
+      <c r="AM148" s="2"/>
+      <c r="AN148" s="2"/>
+      <c r="AO148" s="2"/>
+      <c r="AP148" s="1"/>
+      <c r="AQ148" s="1"/>
+    </row>
+    <row r="149" spans="2:43" outlineLevel="6">
+      <c r="B149" s="3"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="4"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+      <c r="H149" s="43"/>
+      <c r="I149" s="43"/>
+      <c r="J149" s="43"/>
+      <c r="K149" s="43"/>
+      <c r="L149" s="43"/>
+      <c r="M149" s="43"/>
+      <c r="N149" s="43"/>
+      <c r="O149" s="43"/>
+      <c r="P149" s="43"/>
+      <c r="Q149" s="43"/>
+      <c r="R149" s="43"/>
+      <c r="S149" s="43"/>
+      <c r="T149" s="43"/>
+      <c r="U149" s="43"/>
+      <c r="V149" s="43"/>
+      <c r="W149" s="43"/>
+      <c r="X149" s="43"/>
+      <c r="Y149" s="43"/>
+      <c r="Z149" s="44"/>
+      <c r="AA149" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB149" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC149" s="2"/>
+      <c r="AD149" s="2"/>
+      <c r="AE149" s="2"/>
+      <c r="AF149" s="2"/>
+      <c r="AG149" s="2"/>
+      <c r="AH149" s="2"/>
+      <c r="AI149" s="2"/>
+      <c r="AJ149" s="2"/>
+      <c r="AK149" s="2"/>
+      <c r="AL149" s="2"/>
+      <c r="AM149" s="2"/>
+      <c r="AN149" s="2"/>
+      <c r="AO149" s="2"/>
+      <c r="AP149" s="1"/>
+      <c r="AQ149" s="1"/>
+    </row>
+    <row r="150" spans="2:43">
+      <c r="B150" s="42"/>
+      <c r="C150" s="43"/>
+      <c r="D150" s="43"/>
+      <c r="E150" s="43"/>
+      <c r="F150" s="43"/>
+      <c r="G150" s="43"/>
+      <c r="H150" s="43"/>
+      <c r="I150" s="43"/>
+      <c r="J150" s="43"/>
+      <c r="K150" s="43"/>
+      <c r="L150" s="43"/>
+      <c r="M150" s="43"/>
+      <c r="N150" s="43"/>
+      <c r="O150" s="43"/>
+      <c r="P150" s="43"/>
+      <c r="Q150" s="43"/>
+      <c r="R150" s="43"/>
+      <c r="S150" s="43"/>
+      <c r="T150" s="43"/>
+      <c r="U150" s="43"/>
+      <c r="V150" s="43"/>
+      <c r="W150" s="43"/>
+      <c r="X150" s="43"/>
+      <c r="Y150" s="43"/>
+      <c r="Z150" s="44"/>
+      <c r="AA150" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB150" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC150" s="2"/>
+      <c r="AD150" s="2"/>
+      <c r="AE150" s="2"/>
+      <c r="AF150" s="2"/>
+      <c r="AG150" s="2"/>
+      <c r="AH150" s="2"/>
+      <c r="AI150" s="2"/>
+      <c r="AJ150" s="2"/>
+      <c r="AK150" s="2"/>
+      <c r="AL150" s="2"/>
+      <c r="AM150" s="2"/>
+      <c r="AN150" s="2"/>
+      <c r="AO150" s="2"/>
+      <c r="AP150" s="1"/>
+      <c r="AQ150" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="144">
+  <mergeCells count="151">
+    <mergeCell ref="C120:Z120"/>
+    <mergeCell ref="D121:Z121"/>
     <mergeCell ref="D29:Z29"/>
     <mergeCell ref="B112:Z112"/>
     <mergeCell ref="C113:Z113"/>
     <mergeCell ref="D114:Z114"/>
+    <mergeCell ref="B115:Z115"/>
+    <mergeCell ref="C116:Z116"/>
+    <mergeCell ref="D117:Z117"/>
+    <mergeCell ref="C118:Z118"/>
+    <mergeCell ref="C119:Z119"/>
     <mergeCell ref="D108:Z108"/>
     <mergeCell ref="E105:Z105"/>
     <mergeCell ref="E106:Z106"/>
@@ -10240,12 +10702,12 @@
     <mergeCell ref="D111:Z111"/>
     <mergeCell ref="D107:Z107"/>
     <mergeCell ref="D109:Z109"/>
-    <mergeCell ref="B143:Z143"/>
-    <mergeCell ref="E136:Z136"/>
-    <mergeCell ref="F137:Z137"/>
+    <mergeCell ref="B150:Z150"/>
+    <mergeCell ref="E143:Z143"/>
+    <mergeCell ref="F144:Z144"/>
     <mergeCell ref="C61:Z61"/>
     <mergeCell ref="C65:Z65"/>
-    <mergeCell ref="B128:Z128"/>
+    <mergeCell ref="B135:Z135"/>
     <mergeCell ref="B76:Z76"/>
     <mergeCell ref="C63:Z63"/>
     <mergeCell ref="C64:Z64"/>
@@ -10260,21 +10722,21 @@
     <mergeCell ref="C103:Z103"/>
     <mergeCell ref="D104:Z104"/>
     <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="G139:Z139"/>
-    <mergeCell ref="G140:Z140"/>
-    <mergeCell ref="H141:Z141"/>
-    <mergeCell ref="H142:Z142"/>
-    <mergeCell ref="F138:Z138"/>
+    <mergeCell ref="G146:Z146"/>
+    <mergeCell ref="G147:Z147"/>
+    <mergeCell ref="H148:Z148"/>
+    <mergeCell ref="H149:Z149"/>
+    <mergeCell ref="F145:Z145"/>
     <mergeCell ref="B1:Z1"/>
-    <mergeCell ref="D134:Z134"/>
+    <mergeCell ref="D141:Z141"/>
     <mergeCell ref="B2:Z2"/>
     <mergeCell ref="C3:Z3"/>
-    <mergeCell ref="B129:Z129"/>
-    <mergeCell ref="E135:Z135"/>
-    <mergeCell ref="B130:Z130"/>
-    <mergeCell ref="C131:Z131"/>
-    <mergeCell ref="C132:Z132"/>
-    <mergeCell ref="D133:Z133"/>
+    <mergeCell ref="B136:Z136"/>
+    <mergeCell ref="E142:Z142"/>
+    <mergeCell ref="B137:Z137"/>
+    <mergeCell ref="C138:Z138"/>
+    <mergeCell ref="C139:Z139"/>
+    <mergeCell ref="D140:Z140"/>
     <mergeCell ref="D5:Z5"/>
     <mergeCell ref="C11:Z11"/>
     <mergeCell ref="D12:Z12"/>
@@ -10323,7 +10785,7 @@
     <mergeCell ref="E24:Z24"/>
     <mergeCell ref="D46:Z46"/>
     <mergeCell ref="B77:Z77"/>
-    <mergeCell ref="B126:Z126"/>
+    <mergeCell ref="B133:Z133"/>
     <mergeCell ref="B70:Z70"/>
     <mergeCell ref="C71:Z71"/>
     <mergeCell ref="D72:Z72"/>
@@ -10347,20 +10809,20 @@
     <mergeCell ref="D82:Z82"/>
     <mergeCell ref="D83:Z83"/>
     <mergeCell ref="D89:Z89"/>
-    <mergeCell ref="B115:Z115"/>
-    <mergeCell ref="C116:Z116"/>
-    <mergeCell ref="C117:Z117"/>
+    <mergeCell ref="B122:Z122"/>
+    <mergeCell ref="C123:Z123"/>
+    <mergeCell ref="C124:Z124"/>
     <mergeCell ref="D86:Z86"/>
+    <mergeCell ref="B134:Z134"/>
+    <mergeCell ref="B130:Z130"/>
+    <mergeCell ref="B131:Z131"/>
+    <mergeCell ref="B132:Z132"/>
+    <mergeCell ref="B125:Z125"/>
+    <mergeCell ref="B126:Z126"/>
+    <mergeCell ref="B91:Z91"/>
     <mergeCell ref="B127:Z127"/>
-    <mergeCell ref="B123:Z123"/>
-    <mergeCell ref="B124:Z124"/>
-    <mergeCell ref="B125:Z125"/>
-    <mergeCell ref="B118:Z118"/>
-    <mergeCell ref="B119:Z119"/>
-    <mergeCell ref="B91:Z91"/>
-    <mergeCell ref="B120:Z120"/>
-    <mergeCell ref="B121:Z121"/>
-    <mergeCell ref="B122:Z122"/>
+    <mergeCell ref="B128:Z128"/>
+    <mergeCell ref="B129:Z129"/>
     <mergeCell ref="C92:Z92"/>
     <mergeCell ref="C93:Z93"/>
     <mergeCell ref="B94:Z94"/>

</xml_diff>

<commit_message>
Added bq (BigQuery) commands to gcloud cheatsheet.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7230" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7230" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="gcloud cheatsheet" sheetId="4" r:id="rId1"/>
     <sheet name="gsutil cheatsheet" sheetId="7" r:id="rId2"/>
     <sheet name="kubectl cheatsheet" sheetId="10" r:id="rId3"/>
     <sheet name="cbt cheatsheet" sheetId="11" r:id="rId4"/>
-    <sheet name="misc cheatsheet" sheetId="8" r:id="rId5"/>
-    <sheet name="template cheatsheet" sheetId="9" r:id="rId6"/>
+    <sheet name="bq cheatsheet" sheetId="12" r:id="rId5"/>
+    <sheet name="misc cheatsheet" sheetId="8" r:id="rId6"/>
+    <sheet name="template cheatsheet" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -298,6 +299,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="AK82" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This could be a drop-down since zones are a fixed set.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AC92" authorId="0">
       <text>
         <r>
@@ -339,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="498">
   <si>
     <t>Details</t>
   </si>
@@ -1173,9 +1187,6 @@
     <t>nginx:1.10.0</t>
   </si>
   <si>
-    <t>pods/monolith.yaml</t>
-  </si>
-  <si>
     <t>Creates a resource out of a .yaml file.</t>
   </si>
   <si>
@@ -1326,12 +1337,6 @@
     <t>Machine type:</t>
   </si>
   <si>
-    <t>n1-standard-2</t>
-  </si>
-  <si>
-    <t>"https://www.googleapis.com/auth/projecthosting,cloud-platform"</t>
-  </si>
-  <si>
     <t>Role binding(?) name:</t>
   </si>
   <si>
@@ -1417,9 +1422,6 @@
   </si>
   <si>
     <t>Creates some sort of proxy of the cluster in localhost(?).</t>
-  </si>
-  <si>
-    <t>app=gceme role=frontend</t>
   </si>
   <si>
     <t>Creates a ClusterRoleBinding for a particular ClusterRole(???!!!)</t>
@@ -1814,6 +1816,59 @@
   </si>
   <si>
     <t>Deletes a table.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kube-redis-bq/redis/redis-master.yaml
+</t>
+  </si>
+  <si>
+    <t>deployments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Dataset name:</t>
+  </si>
+  <si>
+    <t>rtda</t>
+  </si>
+  <si>
+    <t>Creates a BigQuery dataset.</t>
+  </si>
+  <si>
+    <t>Creates BigQuery objects.</t>
+  </si>
+  <si>
+    <t>Creates a BigQuery table.</t>
+  </si>
+  <si>
+    <t>Dataset:</t>
+  </si>
+  <si>
+    <t>tweets</t>
+  </si>
+  <si>
+    <t>Schema file:</t>
+  </si>
+  <si>
+    <t>kube-redis-bq/bigquery-setup/schema.json</t>
+  </si>
+  <si>
+    <t>Lists the objects contained in the named collection.</t>
+  </si>
+  <si>
+    <t>Apparently, GCE project id is also the name of your collection.</t>
+  </si>
+  <si>
+    <t>Collection:</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>compute-rw,monitoring,bigquery,logging-write,storage-ro</t>
   </si>
 </sst>
 </file>
@@ -2471,8 +2526,8 @@
   </sheetPr>
   <dimension ref="B1:AQ176"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150:Z150"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139:Z139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
@@ -2552,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:43" ht="30">
+    <row r="2" spans="2:43" ht="30" collapsed="1">
       <c r="B2" s="49" t="s">
         <v>7</v>
       </c>
@@ -2605,7 +2660,7 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="3" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B3" s="10"/>
       <c r="C3" s="50" t="str">
         <f>B$2&amp;" instances"</f>
@@ -2915,7 +2970,7 @@
       </c>
       <c r="AQ7" s="1"/>
     </row>
-    <row r="8" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="8" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B8" s="12"/>
       <c r="C8" s="50" t="str">
         <f>B$2&amp;" disks"</f>
@@ -3091,7 +3146,7 @@
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
     </row>
-    <row r="11" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="11" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B11" s="12"/>
       <c r="C11" s="50" t="str">
         <f>B$2&amp;" ssh"</f>
@@ -3205,7 +3260,7 @@
       </c>
       <c r="AQ12" s="1"/>
     </row>
-    <row r="13" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="13" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B13" s="15"/>
       <c r="C13" s="50" t="str">
         <f>B$2&amp;" instance-templates"</f>
@@ -3333,7 +3388,7 @@
       </c>
       <c r="AQ14" s="1"/>
     </row>
-    <row r="15" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="15" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B15" s="15"/>
       <c r="C15" s="50" t="str">
         <f>B$2&amp;" target-pools"</f>
@@ -3443,7 +3498,7 @@
       </c>
       <c r="AQ16" s="1"/>
     </row>
-    <row r="17" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="17" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B17" s="15"/>
       <c r="C17" s="50" t="str">
         <f>B$2&amp;" instance-groups"</f>
@@ -3985,7 +4040,7 @@
       </c>
       <c r="AQ25" s="1"/>
     </row>
-    <row r="26" spans="2:43" outlineLevel="1">
+    <row r="26" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B26" s="15"/>
       <c r="C26" s="50" t="str">
         <f>B$2&amp;" firewall-rules"</f>
@@ -4039,7 +4094,7 @@
       </c>
       <c r="AQ26" s="1"/>
     </row>
-    <row r="27" spans="2:43" ht="50.25" customHeight="1" outlineLevel="2">
+    <row r="27" spans="2:43" ht="50.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="46" t="str">
@@ -4109,7 +4164,7 @@
       </c>
       <c r="AQ27" s="1"/>
     </row>
-    <row r="28" spans="2:43" ht="50.25" customHeight="1" outlineLevel="2">
+    <row r="28" spans="2:43" ht="50.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B28" s="19"/>
       <c r="C28" s="18"/>
       <c r="D28" s="46" t="str">
@@ -4165,7 +4220,7 @@
       </c>
       <c r="AQ28" s="1"/>
     </row>
-    <row r="29" spans="2:43" ht="50.25" customHeight="1" outlineLevel="2">
+    <row r="29" spans="2:43" ht="50.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B29" s="36"/>
       <c r="C29" s="37"/>
       <c r="D29" s="46" t="str">
@@ -4215,11 +4270,11 @@
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
       <c r="AP29" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AQ29" s="1"/>
     </row>
-    <row r="30" spans="2:43" ht="30" outlineLevel="1" collapsed="1">
+    <row r="30" spans="2:43" ht="30" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B30" s="15"/>
       <c r="C30" s="50" t="str">
         <f>B$2&amp;" forwarding-rules"</f>
@@ -4515,7 +4570,7 @@
       </c>
       <c r="AQ34" s="1"/>
     </row>
-    <row r="35" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="35" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B35" s="15"/>
       <c r="C35" s="51" t="str">
         <f>B$2&amp;" health-checks"</f>
@@ -4622,7 +4677,7 @@
       </c>
       <c r="AQ36" s="1"/>
     </row>
-    <row r="37" spans="2:43" ht="135" outlineLevel="1" collapsed="1">
+    <row r="37" spans="2:43" ht="135" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B37" s="15"/>
       <c r="C37" s="50" t="str">
         <f>B$2&amp;" backend-services"</f>
@@ -4822,7 +4877,7 @@
       </c>
       <c r="AQ39" s="1"/>
     </row>
-    <row r="40" spans="2:43" outlineLevel="1">
+    <row r="40" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B40" s="15"/>
       <c r="C40" s="50" t="str">
         <f>B$2&amp;" url-maps"</f>
@@ -4876,7 +4931,7 @@
       </c>
       <c r="AQ40" s="1"/>
     </row>
-    <row r="41" spans="2:43" ht="30" outlineLevel="2">
+    <row r="41" spans="2:43" ht="30" hidden="1" outlineLevel="2">
       <c r="B41" s="15"/>
       <c r="C41" s="16"/>
       <c r="D41" s="46" t="str">
@@ -4936,7 +4991,7 @@
       </c>
       <c r="AQ41" s="1"/>
     </row>
-    <row r="42" spans="2:43" ht="105" outlineLevel="1" collapsed="1">
+    <row r="42" spans="2:43" ht="105" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B42" s="15"/>
       <c r="C42" s="50" t="str">
         <f>B$2&amp;" target-http-proxies"</f>
@@ -5052,7 +5107,7 @@
       </c>
       <c r="AQ43" s="1"/>
     </row>
-    <row r="44" spans="2:43" outlineLevel="1">
+    <row r="44" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B44" s="15"/>
       <c r="C44" s="50" t="str">
         <f>B$2&amp;" networks"</f>
@@ -5106,7 +5161,7 @@
       </c>
       <c r="AQ44" s="1"/>
     </row>
-    <row r="45" spans="2:43" ht="30" outlineLevel="2">
+    <row r="45" spans="2:43" ht="30" hidden="1" outlineLevel="2">
       <c r="B45" s="15"/>
       <c r="C45" s="16"/>
       <c r="D45" s="46" t="str">
@@ -5166,7 +5221,7 @@
       </c>
       <c r="AQ45" s="1"/>
     </row>
-    <row r="46" spans="2:43" outlineLevel="2">
+    <row r="46" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B46" s="27"/>
       <c r="C46" s="26"/>
       <c r="D46" s="46" t="str">
@@ -5220,7 +5275,7 @@
       </c>
       <c r="AQ46" s="1"/>
     </row>
-    <row r="47" spans="2:43" outlineLevel="2">
+    <row r="47" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B47" s="15"/>
       <c r="C47" s="16"/>
       <c r="D47" s="46" t="str">
@@ -5274,7 +5329,7 @@
       </c>
       <c r="AQ47" s="1"/>
     </row>
-    <row r="48" spans="2:43" ht="39.75" customHeight="1" outlineLevel="3">
+    <row r="48" spans="2:43" ht="39.75" hidden="1" customHeight="1" outlineLevel="3">
       <c r="B48" s="15"/>
       <c r="C48" s="16"/>
       <c r="D48" s="16"/>
@@ -5342,7 +5397,7 @@
       </c>
       <c r="AQ48" s="1"/>
     </row>
-    <row r="49" spans="2:43" ht="30" outlineLevel="3" collapsed="1">
+    <row r="49" spans="2:43" ht="30" hidden="1" outlineLevel="3" collapsed="1">
       <c r="B49" s="15"/>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
@@ -5396,7 +5451,7 @@
       </c>
       <c r="AQ49" s="1"/>
     </row>
-    <row r="50" spans="2:43" outlineLevel="1">
+    <row r="50" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B50" s="15"/>
       <c r="C50" s="50" t="str">
         <f>B$2&amp;" addresses"</f>
@@ -5450,7 +5505,7 @@
       </c>
       <c r="AQ50" s="1"/>
     </row>
-    <row r="51" spans="2:43" ht="31.5" customHeight="1" outlineLevel="2">
+    <row r="51" spans="2:43" ht="31.5" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B51" s="15"/>
       <c r="C51" s="16"/>
       <c r="D51" s="46" t="str">
@@ -5510,7 +5565,7 @@
       </c>
       <c r="AQ51" s="1"/>
     </row>
-    <row r="52" spans="2:43" ht="31.5" customHeight="1" outlineLevel="2">
+    <row r="52" spans="2:43" ht="31.5" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B52" s="15"/>
       <c r="C52" s="16"/>
       <c r="D52" s="46" t="str">
@@ -5564,7 +5619,7 @@
       </c>
       <c r="AQ52" s="1"/>
     </row>
-    <row r="53" spans="2:43" outlineLevel="1" collapsed="1">
+    <row r="53" spans="2:43" hidden="1" outlineLevel="1" collapsed="1">
       <c r="B53" s="36"/>
       <c r="C53" s="50" t="str">
         <f>B$2&amp;" zones"</f>
@@ -5614,7 +5669,7 @@
       <c r="AN53" s="2"/>
       <c r="AO53" s="2"/>
       <c r="AP53" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="AQ53" s="1"/>
     </row>
@@ -5668,7 +5723,7 @@
       <c r="AN54" s="2"/>
       <c r="AO54" s="2"/>
       <c r="AP54" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="AQ54" s="1"/>
     </row>
@@ -5724,11 +5779,11 @@
       <c r="AN55" s="2"/>
       <c r="AO55" s="2"/>
       <c r="AP55" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="AQ55" s="1"/>
     </row>
-    <row r="56" spans="2:43" outlineLevel="1">
+    <row r="56" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B56" s="10"/>
       <c r="C56" s="49"/>
       <c r="D56" s="50"/>
@@ -7048,7 +7103,7 @@
       </c>
       <c r="AQ79" s="1"/>
     </row>
-    <row r="80" spans="2:43" collapsed="1">
+    <row r="80" spans="2:43">
       <c r="B80" s="49" t="s">
         <v>250</v>
       </c>
@@ -7099,7 +7154,7 @@
       <c r="AP80" s="1"/>
       <c r="AQ80" s="1"/>
     </row>
-    <row r="81" spans="2:43" hidden="1" outlineLevel="1">
+    <row r="81" spans="2:43" outlineLevel="1">
       <c r="B81" s="27"/>
       <c r="C81" s="50" t="str">
         <f>B$80&amp;" clusters"</f>
@@ -7149,16 +7204,16 @@
       <c r="AN81" s="2"/>
       <c r="AO81" s="2"/>
       <c r="AP81" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="AQ81" s="1"/>
     </row>
-    <row r="82" spans="2:43" ht="51" hidden="1" customHeight="1" outlineLevel="2">
+    <row r="82" spans="2:43" ht="51" customHeight="1" outlineLevel="2">
       <c r="B82" s="27"/>
       <c r="C82" s="26"/>
       <c r="D82" s="46" t="str">
-        <f>C$81&amp;" create "&amp;AC82&amp;IF(ISBLANK(AE82),""," --num-nodes "&amp;AE82)&amp;IF(ISBLANK(AG82),""," --machine-type "&amp;AG82)&amp;IF(ISBLANK(AI82),""," --scopes "&amp;AI82)</f>
-        <v>gcloud container clusters create jenkins-cd --num-nodes 2 --machine-type n1-standard-2 --scopes "https://www.googleapis.com/auth/projecthosting,cloud-platform"</v>
+        <f>C$81&amp;" create "&amp;AC82&amp;IF(ISBLANK(AE82),""," --num-nodes "&amp;AE82)&amp;IF(ISBLANK(AG82),""," --machine-type "&amp;AG82)&amp;IF(ISBLANK(AI82),""," --scopes "&amp;AI82)&amp;IF(ISBLANK(AK82),""," --zone "&amp;AK82)</f>
+        <v>gcloud container clusters create test --scopes compute-rw,monitoring,bigquery,logging-write,storage-ro --zone us-central1-a</v>
       </c>
       <c r="E82" s="47"/>
       <c r="F82" s="47"/>
@@ -7184,34 +7239,34 @@
       <c r="Z82" s="48"/>
       <c r="AA82" s="8" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>gcloud container clusters create jenkins-cd --num-nodes 2 --machine-type n1-standard-2 --scopes "https://www.googleapis.com/auth/projecthosting,cloud-platform"</v>
+        <v>gcloud container clusters create test --scopes compute-rw,monitoring,bigquery,logging-write,storage-ro --zone us-central1-a</v>
       </c>
       <c r="AB82" s="21" t="s">
         <v>248</v>
       </c>
       <c r="AC82" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="AD82" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AE82" s="5"/>
+      <c r="AF82" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="AD82" s="2" t="s">
+      <c r="AG82" s="5"/>
+      <c r="AH82" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="AE82" s="5">
-        <v>2</v>
-      </c>
-      <c r="AF82" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="AG82" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="AH82" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="AI82" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="AJ82" s="2"/>
-      <c r="AK82" s="2"/>
+        <v>497</v>
+      </c>
+      <c r="AJ82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK82" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="AL82" s="2"/>
       <c r="AM82" s="2"/>
       <c r="AN82" s="2"/>
@@ -7220,10 +7275,10 @@
         <v>249</v>
       </c>
       <c r="AQ82" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="83" spans="2:43" ht="30" hidden="1" outlineLevel="2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="83" spans="2:43" ht="30" outlineLevel="2">
       <c r="B83" s="27"/>
       <c r="C83" s="26"/>
       <c r="D83" s="46" t="str">
@@ -7260,7 +7315,7 @@
         <v>252</v>
       </c>
       <c r="AC83" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD83" s="2"/>
       <c r="AE83" s="2"/>
@@ -7279,7 +7334,7 @@
       </c>
       <c r="AQ83" s="1"/>
     </row>
-    <row r="84" spans="2:43" hidden="1" outlineLevel="2">
+    <row r="84" spans="2:43" outlineLevel="2">
       <c r="B84" s="33"/>
       <c r="C84" s="34"/>
       <c r="D84" s="46" t="str">
@@ -7329,11 +7384,11 @@
       <c r="AN84" s="2"/>
       <c r="AO84" s="2"/>
       <c r="AP84" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="AQ84" s="1"/>
     </row>
-    <row r="85" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+    <row r="85" spans="2:43" ht="30" outlineLevel="1" collapsed="1">
       <c r="B85" s="27"/>
       <c r="C85" s="50" t="str">
         <f>B$80&amp;" images"</f>
@@ -7383,7 +7438,7 @@
       <c r="AN85" s="2"/>
       <c r="AO85" s="2"/>
       <c r="AP85" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AQ85" s="1"/>
     </row>
@@ -7437,13 +7492,13 @@
       <c r="AN86" s="2"/>
       <c r="AO86" s="2"/>
       <c r="AP86" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="AQ86" s="1"/>
     </row>
     <row r="87" spans="2:43" collapsed="1">
       <c r="B87" s="49" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
@@ -7490,7 +7545,7 @@
       <c r="AN87" s="2"/>
       <c r="AO87" s="2"/>
       <c r="AP87" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AQ87" s="1"/>
     </row>
@@ -7544,7 +7599,7 @@
       <c r="AN88" s="2"/>
       <c r="AO88" s="2"/>
       <c r="AP88" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="AQ88" s="1"/>
     </row>
@@ -7582,10 +7637,10 @@
         <v>gcloud source repos create other</v>
       </c>
       <c r="AB89" s="21" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AC89" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="AD89" s="2"/>
       <c r="AE89" s="2"/>
@@ -7600,7 +7655,7 @@
       <c r="AN89" s="2"/>
       <c r="AO89" s="2"/>
       <c r="AP89" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AQ89" s="1"/>
     </row>
@@ -7638,10 +7693,10 @@
         <v>gcloud source repos clone DEFAULT</v>
       </c>
       <c r="AB90" s="21" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AC90" s="5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AD90" s="2"/>
       <c r="AE90" s="2"/>
@@ -7656,15 +7711,15 @@
       <c r="AN90" s="2"/>
       <c r="AO90" s="2"/>
       <c r="AP90" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="AQ90" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="91" spans="2:43">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="91" spans="2:43" collapsed="1">
       <c r="B91" s="49" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C91" s="50"/>
       <c r="D91" s="46"/>
@@ -7711,11 +7766,11 @@
       <c r="AN91" s="2"/>
       <c r="AO91" s="2"/>
       <c r="AP91" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="AQ91" s="1"/>
     </row>
-    <row r="92" spans="2:43" outlineLevel="1">
+    <row r="92" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B92" s="33"/>
       <c r="C92" s="49" t="str">
         <f>B$91&amp;" create"&amp;IF(ISBLANK(AC92),""," --region="&amp;AC92)</f>
@@ -7752,7 +7807,7 @@
         <v>82</v>
       </c>
       <c r="AC92" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="AD92" s="2"/>
       <c r="AE92" s="2"/>
@@ -7767,11 +7822,11 @@
       <c r="AN92" s="2"/>
       <c r="AO92" s="2"/>
       <c r="AP92" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="AQ92" s="1"/>
     </row>
-    <row r="93" spans="2:43" ht="90" outlineLevel="1">
+    <row r="93" spans="2:43" ht="90" hidden="1" outlineLevel="1">
       <c r="B93" s="33"/>
       <c r="C93" s="49" t="str">
         <f>B$91&amp;" deploy"&amp;IF(ISBLANK(AC93),""," "&amp;AC93)&amp;IF(ISBLANK(AE93),""," --version "&amp;AE93)</f>
@@ -7805,11 +7860,11 @@
         <v>gcloud app deploy --version 1</v>
       </c>
       <c r="AB93" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="AC93" s="5"/>
       <c r="AD93" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="AE93" s="5">
         <v>1</v>
@@ -7825,15 +7880,15 @@
       <c r="AN93" s="2"/>
       <c r="AO93" s="2"/>
       <c r="AP93" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="AQ93" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="94" spans="2:43" collapsed="1">
       <c r="B94" s="49" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C94" s="50"/>
       <c r="D94" s="46"/>
@@ -7880,7 +7935,7 @@
       <c r="AN94" s="2"/>
       <c r="AO94" s="2"/>
       <c r="AP94" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AQ94" s="1"/>
     </row>
@@ -7918,10 +7973,10 @@
         <v>gcloud datastore create-indexes index.yaml</v>
       </c>
       <c r="AB95" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AC95" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="AD95" s="2"/>
       <c r="AE95" s="2"/>
@@ -7936,13 +7991,13 @@
       <c r="AN95" s="2"/>
       <c r="AO95" s="2"/>
       <c r="AP95" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="AQ95" s="1"/>
     </row>
     <row r="96" spans="2:43" collapsed="1">
       <c r="B96" s="49" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C96" s="50"/>
       <c r="D96" s="50"/>
@@ -7989,7 +8044,7 @@
       <c r="AN96" s="2"/>
       <c r="AO96" s="2"/>
       <c r="AP96" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="AQ96" s="1"/>
     </row>
@@ -8043,7 +8098,7 @@
       <c r="AN97" s="2"/>
       <c r="AO97" s="2"/>
       <c r="AP97" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AQ97" s="1"/>
     </row>
@@ -8097,7 +8152,7 @@
       <c r="AN98" s="2"/>
       <c r="AO98" s="2"/>
       <c r="AP98" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="AQ98" s="1"/>
     </row>
@@ -8138,13 +8193,13 @@
         <v>213</v>
       </c>
       <c r="AC99" s="5" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="AD99" s="21" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="AE99" s="5" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="AF99" s="2"/>
       <c r="AG99" s="2"/>
@@ -8157,13 +8212,13 @@
       <c r="AN99" s="2"/>
       <c r="AO99" s="2"/>
       <c r="AP99" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="AQ99" s="1"/>
     </row>
     <row r="100" spans="2:43" collapsed="1">
       <c r="B100" s="49" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
@@ -8210,7 +8265,7 @@
       <c r="AN100" s="2"/>
       <c r="AO100" s="2"/>
       <c r="AP100" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="AQ100" s="1"/>
     </row>
@@ -8248,16 +8303,16 @@
         <v>gcloud sql connect myinstance --user=root</v>
       </c>
       <c r="AB101" s="21" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="AC101" s="5" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AD101" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="AE101" s="5" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AF101" s="2"/>
       <c r="AG101" s="2"/>
@@ -8270,13 +8325,13 @@
       <c r="AN101" s="2"/>
       <c r="AO101" s="2"/>
       <c r="AP101" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="AQ101" s="1"/>
     </row>
     <row r="102" spans="2:43" ht="30" collapsed="1">
       <c r="B102" s="49" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C102" s="50"/>
       <c r="D102" s="50"/>
@@ -8323,10 +8378,10 @@
       <c r="AN102" s="2"/>
       <c r="AO102" s="2"/>
       <c r="AP102" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="AQ102" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="2:43" hidden="1" outlineLevel="1">
@@ -8379,7 +8434,7 @@
       <c r="AN103" s="2"/>
       <c r="AO103" s="2"/>
       <c r="AP103" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="AQ103" s="1"/>
     </row>
@@ -8433,7 +8488,7 @@
       <c r="AN104" s="2"/>
       <c r="AO104" s="2"/>
       <c r="AP104" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="AQ104" s="1"/>
     </row>
@@ -8474,13 +8529,13 @@
         <v>260</v>
       </c>
       <c r="AC105" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="AD105" s="21" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="AE105" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="AF105" s="2"/>
       <c r="AG105" s="2"/>
@@ -8493,7 +8548,7 @@
       <c r="AN105" s="2"/>
       <c r="AO105" s="2"/>
       <c r="AP105" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AQ105" s="1"/>
     </row>
@@ -8580,10 +8635,10 @@
         <v>gcloud deployment-manager deployments delete custom-net-deployment</v>
       </c>
       <c r="AB107" s="21" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AC107" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AD107" s="2"/>
       <c r="AE107" s="2"/>
@@ -8598,7 +8653,7 @@
       <c r="AN107" s="2"/>
       <c r="AO107" s="2"/>
       <c r="AP107" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="AQ107" s="1"/>
     </row>
@@ -8652,7 +8707,7 @@
       <c r="AN108" s="2"/>
       <c r="AO108" s="2"/>
       <c r="AP108" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="AQ108" s="1"/>
     </row>
@@ -8690,10 +8745,10 @@
         <v>gcloud deployment-manager deployments describe custom-net-deployment</v>
       </c>
       <c r="AB109" s="21" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="AC109" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="AD109" s="2"/>
       <c r="AE109" s="2"/>
@@ -8708,7 +8763,7 @@
       <c r="AN109" s="2"/>
       <c r="AO109" s="2"/>
       <c r="AP109" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="AQ109" s="1"/>
     </row>
@@ -8762,7 +8817,7 @@
       <c r="AN110" s="2"/>
       <c r="AO110" s="2"/>
       <c r="AP110" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="AQ110" s="1"/>
     </row>
@@ -8816,13 +8871,13 @@
       <c r="AN111" s="2"/>
       <c r="AO111" s="2"/>
       <c r="AP111" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="AQ111" s="1"/>
     </row>
-    <row r="112" spans="2:43">
+    <row r="112" spans="2:43" collapsed="1">
       <c r="B112" s="49" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C112" s="50"/>
       <c r="D112" s="50"/>
@@ -8869,11 +8924,11 @@
       <c r="AN112" s="2"/>
       <c r="AO112" s="2"/>
       <c r="AP112" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="AQ112" s="1"/>
     </row>
-    <row r="113" spans="2:43" outlineLevel="1">
+    <row r="113" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B113" s="36"/>
       <c r="C113" s="50" t="str">
         <f>B$112&amp;" services"</f>
@@ -8923,11 +8978,11 @@
       <c r="AN113" s="2"/>
       <c r="AO113" s="2"/>
       <c r="AP113" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="AQ113" s="1"/>
     </row>
-    <row r="114" spans="2:43" outlineLevel="2">
+    <row r="114" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B114" s="36"/>
       <c r="C114" s="37"/>
       <c r="D114" s="50" t="str">
@@ -8961,10 +9016,10 @@
         <v>gcloud endpoints services deploy openapi.yaml</v>
       </c>
       <c r="AB114" s="21" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="AC114" s="5" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="AD114" s="2"/>
       <c r="AE114" s="2"/>
@@ -8979,13 +9034,13 @@
       <c r="AN114" s="2"/>
       <c r="AO114" s="2"/>
       <c r="AP114" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="AQ114" s="1"/>
     </row>
-    <row r="115" spans="2:43">
+    <row r="115" spans="2:43" collapsed="1">
       <c r="B115" s="49" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
@@ -9032,11 +9087,11 @@
       <c r="AN115" s="2"/>
       <c r="AO115" s="2"/>
       <c r="AP115" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="AQ115" s="1"/>
     </row>
-    <row r="116" spans="2:43" outlineLevel="1">
+    <row r="116" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B116" s="36"/>
       <c r="C116" s="46" t="str">
         <f>B$115&amp;" deploy"</f>
@@ -9086,11 +9141,11 @@
       <c r="AN116" s="2"/>
       <c r="AO116" s="2"/>
       <c r="AP116" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="AQ116" s="1"/>
     </row>
-    <row r="117" spans="2:43" ht="30" outlineLevel="2">
+    <row r="117" spans="2:43" ht="30" hidden="1" outlineLevel="2">
       <c r="B117" s="36"/>
       <c r="C117" s="37"/>
       <c r="D117" s="46" t="str">
@@ -9124,22 +9179,22 @@
         <v>gcloud functions deploy helloWorld --stage-bucket ioso_bucket2 --trigger-topic hello_world</v>
       </c>
       <c r="AB117" s="21" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="AC117" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="AD117" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="AE117" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF117" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="AD117" s="21" t="s">
+      <c r="AG117" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="AE117" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="AF117" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="AG117" s="5" t="s">
-        <v>437</v>
       </c>
       <c r="AH117" s="2"/>
       <c r="AI117" s="2"/>
@@ -9150,11 +9205,11 @@
       <c r="AN117" s="2"/>
       <c r="AO117" s="2"/>
       <c r="AP117" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="AQ117" s="1"/>
     </row>
-    <row r="118" spans="2:43" outlineLevel="1">
+    <row r="118" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B118" s="36"/>
       <c r="C118" s="46" t="str">
         <f>B$115&amp;" describe "&amp;AC118</f>
@@ -9188,10 +9243,10 @@
         <v>gcloud functions describe helloWorld</v>
       </c>
       <c r="AB118" s="21" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="AC118" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="AD118" s="2"/>
       <c r="AE118" s="2"/>
@@ -9206,11 +9261,11 @@
       <c r="AN118" s="2"/>
       <c r="AO118" s="2"/>
       <c r="AP118" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="AQ118" s="1"/>
     </row>
-    <row r="119" spans="2:43" ht="30" outlineLevel="1">
+    <row r="119" spans="2:43" ht="30" hidden="1" outlineLevel="1">
       <c r="B119" s="36"/>
       <c r="C119" s="46" t="str">
         <f>B$115&amp;" call "&amp;AC119&amp;IF(ISBLANK(AE119),""," --data "&amp;"'"&amp;AE119&amp;"'")</f>
@@ -9244,16 +9299,16 @@
         <v>gcloud functions call helloWorld --data '{"message":"Hello World!"}'</v>
       </c>
       <c r="AB119" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="AC119" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="AD119" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="AE119" s="5" t="s">
         <v>438</v>
-      </c>
-      <c r="AC119" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="AD119" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="AE119" s="5" t="s">
-        <v>442</v>
       </c>
       <c r="AF119" s="2"/>
       <c r="AG119" s="2"/>
@@ -9266,11 +9321,11 @@
       <c r="AN119" s="2"/>
       <c r="AO119" s="2"/>
       <c r="AP119" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="AQ119" s="1"/>
     </row>
-    <row r="120" spans="2:43" outlineLevel="1">
+    <row r="120" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B120" s="36"/>
       <c r="C120" s="46" t="str">
         <f>B$115&amp;" logs"</f>
@@ -9320,11 +9375,11 @@
       <c r="AN120" s="2"/>
       <c r="AO120" s="2"/>
       <c r="AP120" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="AQ120" s="1"/>
     </row>
-    <row r="121" spans="2:43" outlineLevel="2">
+    <row r="121" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B121" s="36"/>
       <c r="C121" s="37"/>
       <c r="D121" s="46" t="str">
@@ -9358,10 +9413,10 @@
         <v>gcloud functions logs read helloWorld</v>
       </c>
       <c r="AB121" s="21" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="AC121" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="AD121" s="2"/>
       <c r="AE121" s="2"/>
@@ -9376,13 +9431,13 @@
       <c r="AN121" s="2"/>
       <c r="AO121" s="2"/>
       <c r="AP121" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="AQ121" s="1"/>
     </row>
-    <row r="122" spans="2:43">
+    <row r="122" spans="2:43" collapsed="1">
       <c r="B122" s="49" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C122" s="50"/>
       <c r="D122" s="50"/>
@@ -9429,11 +9484,11 @@
       <c r="AN122" s="2"/>
       <c r="AO122" s="2"/>
       <c r="AP122" s="1" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="AQ122" s="1"/>
     </row>
-    <row r="123" spans="2:43" outlineLevel="1">
+    <row r="123" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B123" s="36"/>
       <c r="C123" s="50" t="str">
         <f>B$122&amp;" topics"</f>
@@ -9483,11 +9538,11 @@
       <c r="AN123" s="2"/>
       <c r="AO123" s="2"/>
       <c r="AP123" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="AQ123" s="1"/>
     </row>
-    <row r="124" spans="2:43" outlineLevel="2">
+    <row r="124" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B124" s="36"/>
       <c r="C124" s="37"/>
       <c r="D124" s="50" t="str">
@@ -9521,10 +9576,10 @@
         <v>gcloud pubsub topics create myTopic</v>
       </c>
       <c r="AB124" s="21" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="AC124" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AD124" s="2"/>
       <c r="AE124" s="2"/>
@@ -9539,11 +9594,11 @@
       <c r="AN124" s="2"/>
       <c r="AO124" s="2"/>
       <c r="AP124" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="AQ124" s="1"/>
     </row>
-    <row r="125" spans="2:43" outlineLevel="2">
+    <row r="125" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B125" s="36"/>
       <c r="C125" s="37"/>
       <c r="D125" s="50" t="str">
@@ -9593,11 +9648,11 @@
       <c r="AN125" s="2"/>
       <c r="AO125" s="2"/>
       <c r="AP125" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="AQ125" s="1"/>
     </row>
-    <row r="126" spans="2:43" outlineLevel="2">
+    <row r="126" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B126" s="36"/>
       <c r="C126" s="37"/>
       <c r="D126" s="50" t="str">
@@ -9631,10 +9686,10 @@
         <v>gcloud pubsub topics list-subscriptions myTopic</v>
       </c>
       <c r="AB126" s="21" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="AC126" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AD126" s="2"/>
       <c r="AE126" s="2"/>
@@ -9649,11 +9704,11 @@
       <c r="AN126" s="2"/>
       <c r="AO126" s="2"/>
       <c r="AP126" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="AQ126" s="1"/>
     </row>
-    <row r="127" spans="2:43" outlineLevel="2">
+    <row r="127" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B127" s="39"/>
       <c r="C127" s="40"/>
       <c r="D127" s="46" t="str">
@@ -9687,16 +9742,16 @@
         <v>gcloud pubsub topics publish myTopic --message "Hello"</v>
       </c>
       <c r="AB127" s="21" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="AC127" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AD127" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="AE127" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="AF127" s="2"/>
       <c r="AG127" s="2"/>
@@ -9709,11 +9764,11 @@
       <c r="AN127" s="2"/>
       <c r="AO127" s="2"/>
       <c r="AP127" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="AQ127" s="1"/>
     </row>
-    <row r="128" spans="2:43" outlineLevel="2">
+    <row r="128" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B128" s="36"/>
       <c r="C128" s="37"/>
       <c r="D128" s="50" t="str">
@@ -9747,10 +9802,10 @@
         <v>gcloud pubsub topics delete myTopic</v>
       </c>
       <c r="AB128" s="21" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="AC128" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AD128" s="2"/>
       <c r="AE128" s="2"/>
@@ -9765,11 +9820,11 @@
       <c r="AN128" s="2"/>
       <c r="AO128" s="2"/>
       <c r="AP128" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="AQ128" s="1"/>
     </row>
-    <row r="129" spans="2:43" outlineLevel="1">
+    <row r="129" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B129" s="36"/>
       <c r="C129" s="50" t="str">
         <f>B$122&amp;" subscriptions"</f>
@@ -9819,11 +9874,11 @@
       <c r="AN129" s="2"/>
       <c r="AO129" s="2"/>
       <c r="AP129" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="AQ129" s="1"/>
     </row>
-    <row r="130" spans="2:43" ht="30" outlineLevel="2">
+    <row r="130" spans="2:43" ht="30" hidden="1" outlineLevel="2">
       <c r="B130" s="36"/>
       <c r="C130" s="37"/>
       <c r="D130" s="46" t="str">
@@ -9857,16 +9912,16 @@
         <v>gcloud pubsub subscriptions create --topic myTopic mySubscription</v>
       </c>
       <c r="AB130" s="21" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="AC130" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="AD130" s="21" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="AE130" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="AF130" s="2"/>
       <c r="AG130" s="2"/>
@@ -9879,11 +9934,11 @@
       <c r="AN130" s="2"/>
       <c r="AO130" s="2"/>
       <c r="AP130" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="AQ130" s="1"/>
     </row>
-    <row r="131" spans="2:43" ht="30.75" customHeight="1" outlineLevel="2">
+    <row r="131" spans="2:43" ht="30.75" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B131" s="39"/>
       <c r="C131" s="40"/>
       <c r="D131" s="46" t="str">
@@ -9917,19 +9972,19 @@
         <v>gcloud pubsub subscriptions pull mySubscription --auto-ack --limit=3</v>
       </c>
       <c r="AB131" s="21" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="AC131" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="AD131" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="AE131" s="5" t="b">
         <v>1</v>
       </c>
       <c r="AF131" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="AG131" s="5">
         <v>3</v>
@@ -9943,11 +9998,11 @@
       <c r="AN131" s="2"/>
       <c r="AO131" s="2"/>
       <c r="AP131" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="AQ131" s="1"/>
     </row>
-    <row r="132" spans="2:43" outlineLevel="2">
+    <row r="132" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B132" s="36"/>
       <c r="C132" s="37"/>
       <c r="D132" s="46" t="str">
@@ -9981,10 +10036,10 @@
         <v>gcloud pubsub subscriptions delete Test1</v>
       </c>
       <c r="AB132" s="21" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="AC132" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="AD132" s="2"/>
       <c r="AE132" s="2"/>
@@ -9999,13 +10054,13 @@
       <c r="AN132" s="2"/>
       <c r="AO132" s="2"/>
       <c r="AP132" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="AQ132" s="1"/>
     </row>
     <row r="133" spans="2:43" ht="60" collapsed="1">
       <c r="B133" s="49" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C133" s="50"/>
       <c r="D133" s="50"/>
@@ -10052,10 +10107,10 @@
       <c r="AN133" s="2"/>
       <c r="AO133" s="2"/>
       <c r="AP133" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="AQ133" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="134" spans="2:43" ht="30" hidden="1" outlineLevel="1">
@@ -10092,22 +10147,22 @@
         <v>gcloud docker -- push gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
       </c>
       <c r="AB134" s="22" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AC134" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AD134" s="22" t="s">
         <v>147</v>
       </c>
       <c r="AE134" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AF134" s="2" t="s">
         <v>261</v>
       </c>
       <c r="AG134" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="AH134" s="2"/>
       <c r="AI134" s="2"/>
@@ -10118,7 +10173,7 @@
       <c r="AN134" s="2"/>
       <c r="AO134" s="2"/>
       <c r="AP134" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="AQ134" s="1"/>
     </row>
@@ -10156,22 +10211,22 @@
         <v>gcloud docker -- pull gcr.io/qwiklabs-gcp-a02f70a41a3fba35/quickstart-image</v>
       </c>
       <c r="AB135" s="22" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AC135" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AD135" s="22" t="s">
         <v>147</v>
       </c>
       <c r="AE135" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="AF135" s="2" t="s">
         <v>261</v>
       </c>
       <c r="AG135" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="AH135" s="2"/>
       <c r="AI135" s="2"/>
@@ -10182,7 +10237,7 @@
       <c r="AN135" s="2"/>
       <c r="AO135" s="2"/>
       <c r="AP135" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="AQ135" s="1"/>
     </row>
@@ -10426,7 +10481,9 @@
       <c r="AQ140" s="1"/>
     </row>
     <row r="141" spans="2:43" ht="27" customHeight="1">
-      <c r="B141" s="46"/>
+      <c r="B141" s="46" t="s">
+        <v>483</v>
+      </c>
       <c r="C141" s="47"/>
       <c r="D141" s="47"/>
       <c r="E141" s="47"/>
@@ -10453,7 +10510,8 @@
       <c r="Z141" s="48"/>
       <c r="AA141" s="8" t="str">
         <f t="shared" ca="1" si="51"/>
-        <v/>
+        <v xml:space="preserve">
+</v>
       </c>
       <c r="AB141" s="2" t="s">
         <v>6</v>
@@ -10475,7 +10533,9 @@
       <c r="AQ141" s="1"/>
     </row>
     <row r="142" spans="2:43" ht="30.75" customHeight="1">
-      <c r="B142" s="46"/>
+      <c r="B142" s="46" t="s">
+        <v>483</v>
+      </c>
       <c r="C142" s="47"/>
       <c r="D142" s="47"/>
       <c r="E142" s="47"/>
@@ -10502,7 +10562,8 @@
       <c r="Z142" s="48"/>
       <c r="AA142" s="8" t="str">
         <f t="shared" ca="1" si="51"/>
-        <v/>
+        <v xml:space="preserve">
+</v>
       </c>
       <c r="AB142" s="2" t="s">
         <v>6</v>
@@ -11490,7 +11551,7 @@
       <c r="AP162" s="1"/>
       <c r="AQ162" s="1"/>
     </row>
-    <row r="163" spans="2:43">
+    <row r="163" spans="2:43" collapsed="1">
       <c r="B163" s="49"/>
       <c r="C163" s="50"/>
       <c r="D163" s="50"/>
@@ -11538,7 +11599,7 @@
       <c r="AP163" s="1"/>
       <c r="AQ163" s="1"/>
     </row>
-    <row r="164" spans="2:43" outlineLevel="1">
+    <row r="164" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B164" s="15"/>
       <c r="C164" s="50"/>
       <c r="D164" s="50"/>
@@ -11586,7 +11647,7 @@
       <c r="AP164" s="1"/>
       <c r="AQ164" s="1"/>
     </row>
-    <row r="165" spans="2:43" outlineLevel="1">
+    <row r="165" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B165" s="3"/>
       <c r="C165" s="50"/>
       <c r="D165" s="50"/>
@@ -11634,7 +11695,7 @@
       <c r="AP165" s="1"/>
       <c r="AQ165" s="1"/>
     </row>
-    <row r="166" spans="2:43" outlineLevel="2">
+    <row r="166" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B166" s="3"/>
       <c r="C166" s="4"/>
       <c r="D166" s="50"/>
@@ -11682,7 +11743,7 @@
       <c r="AP166" s="1"/>
       <c r="AQ166" s="1"/>
     </row>
-    <row r="167" spans="2:43" outlineLevel="2">
+    <row r="167" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B167" s="3"/>
       <c r="C167" s="4"/>
       <c r="D167" s="50"/>
@@ -11730,7 +11791,7 @@
       <c r="AP167" s="1"/>
       <c r="AQ167" s="1"/>
     </row>
-    <row r="168" spans="2:43" outlineLevel="3">
+    <row r="168" spans="2:43" hidden="1" outlineLevel="3">
       <c r="B168" s="3"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
@@ -11778,7 +11839,7 @@
       <c r="AP168" s="1"/>
       <c r="AQ168" s="1"/>
     </row>
-    <row r="169" spans="2:43" outlineLevel="3">
+    <row r="169" spans="2:43" hidden="1" outlineLevel="3">
       <c r="B169" s="3"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -11826,7 +11887,7 @@
       <c r="AP169" s="1"/>
       <c r="AQ169" s="1"/>
     </row>
-    <row r="170" spans="2:43" outlineLevel="4">
+    <row r="170" spans="2:43" hidden="1" outlineLevel="4">
       <c r="B170" s="3"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
@@ -11874,7 +11935,7 @@
       <c r="AP170" s="1"/>
       <c r="AQ170" s="1"/>
     </row>
-    <row r="171" spans="2:43" outlineLevel="4">
+    <row r="171" spans="2:43" hidden="1" outlineLevel="4">
       <c r="B171" s="3"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
@@ -11922,7 +11983,7 @@
       <c r="AP171" s="1"/>
       <c r="AQ171" s="1"/>
     </row>
-    <row r="172" spans="2:43" outlineLevel="5">
+    <row r="172" spans="2:43" hidden="1" outlineLevel="5">
       <c r="B172" s="3"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -11970,7 +12031,7 @@
       <c r="AP172" s="1"/>
       <c r="AQ172" s="1"/>
     </row>
-    <row r="173" spans="2:43" outlineLevel="5">
+    <row r="173" spans="2:43" hidden="1" outlineLevel="5">
       <c r="B173" s="3"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
@@ -12018,7 +12079,7 @@
       <c r="AP173" s="1"/>
       <c r="AQ173" s="1"/>
     </row>
-    <row r="174" spans="2:43" outlineLevel="6">
+    <row r="174" spans="2:43" hidden="1" outlineLevel="6">
       <c r="B174" s="3"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
@@ -12066,7 +12127,7 @@
       <c r="AP174" s="1"/>
       <c r="AQ174" s="1"/>
     </row>
-    <row r="175" spans="2:43" outlineLevel="6">
+    <row r="175" spans="2:43" hidden="1" outlineLevel="6">
       <c r="B175" s="3"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
@@ -12789,7 +12850,7 @@
         <v>57</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="2:41" ht="30" outlineLevel="1">
@@ -12833,24 +12894,24 @@
         <v>59</v>
       </c>
       <c r="AE9" s="5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AG9" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AH9" s="22" t="s">
         <v>61</v>
       </c>
       <c r="AI9" s="5"/>
       <c r="AJ9" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="AK9" s="5"/>
       <c r="AL9" s="2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="AM9" s="5"/>
       <c r="AN9" s="1" t="s">
@@ -15091,8 +15152,8 @@
   </sheetPr>
   <dimension ref="B1:AM78"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:Z46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -15288,10 +15349,10 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="2:39" ht="30">
+    <row r="4" spans="2:39">
       <c r="B4" s="49" t="str">
         <f>"kubectl get "&amp;AC4&amp;IF(ISBLANK(AE4),""," "&amp;AE4)&amp;IF(ISBLANK(AG4),""," -l "&amp;SUBSTITUTE(AG4," "," -l "))&amp;IF(ISBLANK(AI4),""," --show-labels")&amp;IF(ISBLANK(AK4),""," -n "&amp;AK4)</f>
-        <v>kubectl get pods -l app=gceme -l role=frontend -n production</v>
+        <v>kubectl get deployments</v>
       </c>
       <c r="C4" s="50"/>
       <c r="D4" s="50"/>
@@ -15319,34 +15380,30 @@
       <c r="Z4" s="51"/>
       <c r="AA4" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>kubectl get pods -l app=gceme -l role=frontend -n production</v>
+        <v>kubectl get deployments</v>
       </c>
       <c r="AB4" s="21" t="s">
         <v>266</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>269</v>
+        <v>482</v>
       </c>
       <c r="AD4" s="22" t="s">
         <v>265</v>
       </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>353</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="AG4" s="5"/>
       <c r="AH4" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="AK4" s="5" t="s">
-        <v>337</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="AK4" s="5"/>
       <c r="AL4" s="1" t="s">
         <v>268</v>
       </c>
@@ -15398,15 +15455,16 @@
       <c r="AJ5" s="2"/>
       <c r="AK5" s="2"/>
       <c r="AL5" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AM5" s="1"/>
     </row>
-    <row r="6" spans="2:39" ht="30" outlineLevel="1">
+    <row r="6" spans="2:39" ht="60" outlineLevel="1">
       <c r="B6" s="27"/>
       <c r="C6" s="50" t="str">
         <f>B$5&amp;" -f "&amp;AC6</f>
-        <v>kubectl create -f pods/monolith.yaml</v>
+        <v xml:space="preserve">kubectl create -f kube-redis-bq/redis/redis-master.yaml
+</v>
       </c>
       <c r="D6" s="50"/>
       <c r="E6" s="50"/>
@@ -15433,13 +15491,14 @@
       <c r="Z6" s="51"/>
       <c r="AA6" s="8" t="str">
         <f t="shared" ref="AA6:AA18" ca="1" si="1">IFERROR(OFFSET(A6,0,MATCH("",B6:Z6,-1)),"")</f>
-        <v>kubectl create -f pods/monolith.yaml</v>
+        <v xml:space="preserve">kubectl create -f kube-redis-bq/redis/redis-master.yaml
+</v>
       </c>
       <c r="AB6" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>271</v>
+        <v>481</v>
       </c>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -15450,11 +15509,11 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AM6" s="1"/>
     </row>
-    <row r="7" spans="2:39" outlineLevel="1">
+    <row r="7" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B7" s="31"/>
       <c r="C7" s="50" t="str">
         <f>B$5&amp;" secret"</f>
@@ -15502,7 +15561,7 @@
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
     </row>
-    <row r="8" spans="2:39" outlineLevel="2">
+    <row r="8" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B8" s="31"/>
       <c r="C8" s="30"/>
       <c r="D8" s="50" t="str">
@@ -15536,16 +15595,16 @@
         <v>kubectl create secret generic tls-certs --from-file tls/</v>
       </c>
       <c r="AB8" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="AC8" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="AC8" s="5" t="s">
+      <c r="AD8" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="AD8" s="21" t="s">
-        <v>289</v>
-      </c>
       <c r="AE8" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
@@ -15554,11 +15613,11 @@
       <c r="AJ8" s="2"/>
       <c r="AK8" s="2"/>
       <c r="AL8" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AM8" s="1"/>
     </row>
-    <row r="9" spans="2:39" outlineLevel="2">
+    <row r="9" spans="2:39" hidden="1" outlineLevel="2">
       <c r="B9" s="31"/>
       <c r="C9" s="30"/>
       <c r="D9" s="50"/>
@@ -15603,7 +15662,7 @@
       <c r="AL9" s="1"/>
       <c r="AM9" s="1"/>
     </row>
-    <row r="10" spans="2:39" outlineLevel="1">
+    <row r="10" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B10" s="31"/>
       <c r="C10" s="50" t="str">
         <f>B$5&amp;" configmap"</f>
@@ -15651,7 +15710,7 @@
       <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
     </row>
-    <row r="11" spans="2:39" ht="30" customHeight="1" outlineLevel="2">
+    <row r="11" spans="2:39" ht="30" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B11" s="31"/>
       <c r="C11" s="30"/>
       <c r="D11" s="46" t="str">
@@ -15685,16 +15744,16 @@
         <v>kubectl create configmap nginx-proxy-conf --from-file nginx/proxy.conf</v>
       </c>
       <c r="AB11" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="AC11" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="AC11" s="5" t="s">
+      <c r="AD11" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="AE11" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="AD11" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="AE11" s="5" t="s">
-        <v>294</v>
       </c>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
@@ -15703,11 +15762,11 @@
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AM11" s="1"/>
     </row>
-    <row r="12" spans="2:39" outlineLevel="1">
+    <row r="12" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B12" s="33"/>
       <c r="C12" s="50" t="str">
         <f>B$5&amp;" clusterrolebinding"</f>
@@ -15753,11 +15812,11 @@
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
       <c r="AL12" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="AM12" s="1"/>
     </row>
-    <row r="13" spans="2:39" ht="41.25" customHeight="1" outlineLevel="2">
+    <row r="13" spans="2:39" ht="41.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B13" s="33"/>
       <c r="C13" s="34"/>
       <c r="D13" s="46" t="str">
@@ -15791,35 +15850,35 @@
         <v>kubectl create clusterrolebinding tiller-admin-binding --clusterrole=cluster-admin --serviceaccount=kube-system:tiller</v>
       </c>
       <c r="AB13" s="21" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="AD13" s="22" t="s">
         <v>217</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="AG13" s="5"/>
       <c r="AH13" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="AI13" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
       <c r="AL13" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="AM13" s="1"/>
     </row>
-    <row r="14" spans="2:39" outlineLevel="1">
+    <row r="14" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B14" s="33"/>
       <c r="C14" s="50" t="str">
         <f>B$5&amp;" serviceaccount"</f>
@@ -15865,11 +15924,11 @@
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
       <c r="AL14" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AM14" s="1"/>
     </row>
-    <row r="15" spans="2:39" ht="41.25" customHeight="1" outlineLevel="2">
+    <row r="15" spans="2:39" ht="41.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B15" s="33"/>
       <c r="C15" s="34"/>
       <c r="D15" s="46" t="str">
@@ -15903,16 +15962,16 @@
         <v>kubectl create serviceaccount tiller --namespace kube-system</v>
       </c>
       <c r="AB15" s="21" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="AC15" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="AE15" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
@@ -15925,7 +15984,7 @@
       </c>
       <c r="AM15" s="1"/>
     </row>
-    <row r="16" spans="2:39" outlineLevel="1">
+    <row r="16" spans="2:39" outlineLevel="1" collapsed="1">
       <c r="B16" s="33"/>
       <c r="C16" s="50" t="str">
         <f>B$5&amp;" ns"</f>
@@ -15971,11 +16030,11 @@
       <c r="AJ16" s="2"/>
       <c r="AK16" s="2"/>
       <c r="AL16" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AM16" s="1"/>
     </row>
-    <row r="17" spans="2:39" ht="41.25" customHeight="1" outlineLevel="2">
+    <row r="17" spans="2:39" ht="41.25" hidden="1" customHeight="1" outlineLevel="2">
       <c r="B17" s="33"/>
       <c r="C17" s="34"/>
       <c r="D17" s="46" t="str">
@@ -16009,10 +16068,10 @@
         <v>kubectl create ns production</v>
       </c>
       <c r="AB17" s="21" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
@@ -16109,13 +16168,13 @@
         <v>266</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AD19" s="22" t="s">
         <v>265</v>
       </c>
       <c r="AE19" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
@@ -16124,7 +16183,7 @@
       <c r="AJ19" s="2"/>
       <c r="AK19" s="2"/>
       <c r="AL19" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AM19" s="1"/>
     </row>
@@ -16162,19 +16221,19 @@
         <v>kubectl port-forward monolith 10080:80</v>
       </c>
       <c r="AB20" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC20" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AC20" s="5" t="s">
+      <c r="AD20" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="AD20" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="AE20" s="5">
         <v>10080</v>
       </c>
       <c r="AF20" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AG20" s="5">
         <v>80</v>
@@ -16184,7 +16243,7 @@
       <c r="AJ20" s="2"/>
       <c r="AK20" s="2"/>
       <c r="AL20" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AM20" s="1"/>
     </row>
@@ -16222,13 +16281,13 @@
         <v>kubectl logs -f monolith</v>
       </c>
       <c r="AB21" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC21" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AC21" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="AD21" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AE21" s="5" t="b">
         <v>1</v>
@@ -16240,11 +16299,11 @@
       <c r="AJ21" s="2"/>
       <c r="AK21" s="2"/>
       <c r="AL21" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AM21" s="1"/>
     </row>
-    <row r="22" spans="2:39">
+    <row r="22" spans="2:39" collapsed="1">
       <c r="B22" s="49" t="str">
         <f>"kubectl exec"</f>
         <v>kubectl exec</v>
@@ -16290,11 +16349,11 @@
       <c r="AJ22" s="2"/>
       <c r="AK22" s="2"/>
       <c r="AL22" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AM22" s="1"/>
     </row>
-    <row r="23" spans="2:39" outlineLevel="1">
+    <row r="23" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B23" s="27"/>
       <c r="C23" s="50" t="str">
         <f>B$22&amp;" "&amp;AC23&amp;IF(ISBLANK(AE23),""," -c "&amp;AE23)&amp;" -- "&amp;AG23</f>
@@ -16328,31 +16387,31 @@
         <v>kubectl exec monolith -- ls</v>
       </c>
       <c r="AB23" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC23" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AC23" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="AD23" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AE23" s="5"/>
       <c r="AF23" s="21" t="s">
         <v>21</v>
       </c>
       <c r="AG23" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2"/>
       <c r="AL23" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AM23" s="1"/>
     </row>
-    <row r="24" spans="2:39" outlineLevel="1">
+    <row r="24" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B24" s="27"/>
       <c r="C24" s="50" t="str">
         <f>B$22&amp;" "&amp;AC24&amp;" --stdin --tty "&amp;IF(ISBLANK(AE24),""," -c "&amp;AE24)&amp;"/bin/sh"</f>
@@ -16386,13 +16445,13 @@
         <v>kubectl exec monolith --stdin --tty /bin/sh</v>
       </c>
       <c r="AB24" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC24" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AC24" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="AD24" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AE24" s="5"/>
       <c r="AF24" s="2"/>
@@ -16402,7 +16461,7 @@
       <c r="AJ24" s="2"/>
       <c r="AK24" s="2"/>
       <c r="AL24" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AM24" s="1"/>
     </row>
@@ -16449,20 +16508,20 @@
         <v>265</v>
       </c>
       <c r="AE25" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="AF25" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="AG25" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="AF25" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="AG25" s="5" t="s">
-        <v>302</v>
       </c>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
       <c r="AL25" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AM25" s="1"/>
     </row>
@@ -16500,13 +16559,13 @@
         <v>kubectl explain deployment.metadata.name</v>
       </c>
       <c r="AB26" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="AC26" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="AD26" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="AC26" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="AD26" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="AE26" s="5"/>
       <c r="AF26" s="2"/>
@@ -16516,11 +16575,11 @@
       <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
       <c r="AL26" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AM26" s="1"/>
     </row>
-    <row r="27" spans="2:39" ht="30">
+    <row r="27" spans="2:39" ht="30" collapsed="1">
       <c r="B27" s="49" t="str">
         <f>"kubectl scale"</f>
         <v>kubectl scale</v>
@@ -16566,11 +16625,11 @@
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2"/>
       <c r="AL27" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AM27" s="1"/>
     </row>
-    <row r="28" spans="2:39" ht="30" outlineLevel="1">
+    <row r="28" spans="2:39" ht="30" hidden="1" outlineLevel="1">
       <c r="B28" s="31"/>
       <c r="C28" s="46" t="str">
         <f>B$27&amp;" "&amp;AC28&amp;" "&amp;AE28&amp;" --replicas="&amp;AG28&amp;IF(ISBLANK(AI28),""," -n "&amp;AI28)</f>
@@ -16613,28 +16672,28 @@
         <v>265</v>
       </c>
       <c r="AE28" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AF28" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AG28" s="5">
         <v>4</v>
       </c>
       <c r="AH28" s="22" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="AI28" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AJ28" s="2"/>
       <c r="AK28" s="2"/>
       <c r="AL28" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AM28" s="1"/>
     </row>
-    <row r="29" spans="2:39" outlineLevel="1">
+    <row r="29" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B29" s="31"/>
       <c r="C29" s="50"/>
       <c r="D29" s="50"/>
@@ -16722,7 +16781,7 @@
         <v>265</v>
       </c>
       <c r="AE30" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
@@ -16731,11 +16790,11 @@
       <c r="AJ30" s="2"/>
       <c r="AK30" s="2"/>
       <c r="AL30" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AM30" s="1"/>
     </row>
-    <row r="31" spans="2:39">
+    <row r="31" spans="2:39" collapsed="1">
       <c r="B31" s="49" t="str">
         <f>"kubectl rollout"</f>
         <v>kubectl rollout</v>
@@ -16781,11 +16840,11 @@
       <c r="AJ31" s="2"/>
       <c r="AK31" s="2"/>
       <c r="AL31" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AM31" s="1"/>
     </row>
-    <row r="32" spans="2:39" outlineLevel="1">
+    <row r="32" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B32" s="31"/>
       <c r="C32" s="50" t="str">
         <f>B$31&amp;" history "&amp;AC32&amp;"/"&amp;AE32</f>
@@ -16828,7 +16887,7 @@
         <v>265</v>
       </c>
       <c r="AE32" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
@@ -16837,11 +16896,11 @@
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AM32" s="1"/>
     </row>
-    <row r="33" spans="2:39" outlineLevel="1">
+    <row r="33" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B33" s="31"/>
       <c r="C33" s="50" t="str">
         <f>B$31&amp;" pause "&amp;AC33&amp;"/"&amp;AE33</f>
@@ -16884,7 +16943,7 @@
         <v>265</v>
       </c>
       <c r="AE33" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
@@ -16893,13 +16952,13 @@
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
       <c r="AL33" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="AM33" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="AM33" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="34" spans="2:39" outlineLevel="1">
+    </row>
+    <row r="34" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B34" s="31"/>
       <c r="C34" s="50" t="str">
         <f>B$31&amp;" resume "&amp;AC34&amp;"/"&amp;AE34</f>
@@ -16942,7 +17001,7 @@
         <v>265</v>
       </c>
       <c r="AE34" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
@@ -16951,13 +17010,13 @@
       <c r="AJ34" s="2"/>
       <c r="AK34" s="2"/>
       <c r="AL34" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AM34" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="35" spans="2:39" outlineLevel="1">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="35" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B35" s="31"/>
       <c r="C35" s="50" t="str">
         <f>B$31&amp;" status "&amp;AC35&amp;"/"&amp;AE35</f>
@@ -17000,7 +17059,7 @@
         <v>265</v>
       </c>
       <c r="AE35" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
@@ -17009,11 +17068,11 @@
       <c r="AJ35" s="2"/>
       <c r="AK35" s="2"/>
       <c r="AL35" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AM35" s="1"/>
     </row>
-    <row r="36" spans="2:39" outlineLevel="1">
+    <row r="36" spans="2:39" hidden="1" outlineLevel="1">
       <c r="B36" s="31"/>
       <c r="C36" s="50" t="str">
         <f>B$31&amp;" undo "&amp;AC36&amp;"/"&amp;AE36</f>
@@ -17056,7 +17115,7 @@
         <v>265</v>
       </c>
       <c r="AE36" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
@@ -17065,7 +17124,7 @@
       <c r="AJ36" s="2"/>
       <c r="AK36" s="2"/>
       <c r="AL36" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AM36" s="1"/>
     </row>
@@ -17151,16 +17210,16 @@
         <v>kubectl apply -f k8s/production -n production</v>
       </c>
       <c r="AB38" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AC38" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="AD38" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="AE38" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
@@ -17169,13 +17228,13 @@
       <c r="AJ38" s="2"/>
       <c r="AK38" s="2"/>
       <c r="AL38" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AM38" s="1"/>
     </row>
     <row r="39" spans="2:39">
       <c r="B39" s="49" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C39" s="50"/>
       <c r="D39" s="50"/>
@@ -17216,7 +17275,7 @@
       <c r="AJ39" s="2"/>
       <c r="AK39" s="2"/>
       <c r="AL39" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="AM39" s="1"/>
     </row>
@@ -17263,7 +17322,7 @@
       <c r="AL40" s="1"/>
       <c r="AM40" s="1"/>
     </row>
-    <row r="41" spans="2:39" ht="39" customHeight="1">
+    <row r="41" spans="2:39">
       <c r="B41" s="49"/>
       <c r="C41" s="50"/>
       <c r="D41" s="50"/>
@@ -17306,7 +17365,7 @@
       <c r="AL41" s="1"/>
       <c r="AM41" s="1"/>
     </row>
-    <row r="42" spans="2:39">
+    <row r="42" spans="2:39" ht="27.75" customHeight="1">
       <c r="B42" s="49"/>
       <c r="C42" s="50"/>
       <c r="D42" s="50"/>
@@ -17392,7 +17451,7 @@
       <c r="AL43" s="1"/>
       <c r="AM43" s="1"/>
     </row>
-    <row r="44" spans="2:39">
+    <row r="44" spans="2:39" ht="27" customHeight="1">
       <c r="B44" s="49"/>
       <c r="C44" s="50"/>
       <c r="D44" s="50"/>
@@ -18903,7 +18962,7 @@
   </sheetPr>
   <dimension ref="B1:AM45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:Z8"/>
     </sheetView>
   </sheetViews>
@@ -19010,10 +19069,10 @@
         <v>cbt createtable my-table</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
@@ -19024,7 +19083,7 @@
       <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="AM2" s="1"/>
     </row>
@@ -19062,10 +19121,10 @@
         <v>cbt ls my-table</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -19076,7 +19135,7 @@
       <c r="AJ3" s="2"/>
       <c r="AK3" s="2"/>
       <c r="AL3" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="AM3" s="1"/>
     </row>
@@ -19114,16 +19173,16 @@
         <v>cbt createfamily my-table cf1</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AD4" s="21" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
@@ -19132,7 +19191,7 @@
       <c r="AJ4" s="2"/>
       <c r="AK4" s="2"/>
       <c r="AL4" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="AM4" s="1"/>
     </row>
@@ -19170,37 +19229,37 @@
         <v>cbt set my-table r1 cf1:c1=test-value</v>
       </c>
       <c r="AB5" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="AD5" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="AE5" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="AC5" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="AD5" s="21" t="s">
+      <c r="AF5" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="AH5" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="AI5" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="AE5" s="5" t="s">
+      <c r="AJ5" s="21" t="s">
         <v>476</v>
       </c>
-      <c r="AF5" s="21" t="s">
+      <c r="AK5" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="AG5" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="AH5" s="21" t="s">
+      <c r="AL5" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="AI5" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="AJ5" s="21" t="s">
-        <v>480</v>
-      </c>
-      <c r="AK5" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="AL5" s="1" t="s">
-        <v>482</v>
       </c>
       <c r="AM5" s="1"/>
     </row>
@@ -19238,10 +19297,10 @@
         <v>cbt read my-table</v>
       </c>
       <c r="AB6" s="21" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -19252,7 +19311,7 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="AM6" s="1"/>
     </row>
@@ -19290,10 +19349,10 @@
         <v>cbt deletetable my-table</v>
       </c>
       <c r="AB7" s="21" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
@@ -19304,7 +19363,7 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="1" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="AM7" s="1"/>
     </row>
@@ -20940,6 +20999,1405 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B1:AK33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="26" width="2.85546875" customWidth="1"/>
+    <col min="27" max="27" width="21.28515625" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="22.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="7.140625" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="40.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="15.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="26.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="46" customWidth="1"/>
+    <col min="38" max="38" width="68.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:37">
+      <c r="B1" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK1" s="42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:37">
+      <c r="B2" s="49" t="str">
+        <f>"bq mk"</f>
+        <v>bq mk</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="8" t="str">
+        <f t="shared" ref="AA2:AA30" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
+        <v>bq mk</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AK2" s="1"/>
+    </row>
+    <row r="3" spans="2:37" outlineLevel="1">
+      <c r="B3" s="39"/>
+      <c r="C3" s="50" t="str">
+        <f>B$2&amp;" "&amp;AC3</f>
+        <v>bq mk rtda</v>
+      </c>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="51"/>
+      <c r="AA3" s="8" t="str">
+        <f t="shared" ref="AA3:AA4" ca="1" si="1">IFERROR(OFFSET(A3,0,MATCH("",B3:Z3,-1)),"")</f>
+        <v>bq mk rtda</v>
+      </c>
+      <c r="AB3" s="21" t="s">
+        <v>484</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AK3" s="1"/>
+    </row>
+    <row r="4" spans="2:37" ht="30" customHeight="1" outlineLevel="1">
+      <c r="B4" s="39"/>
+      <c r="C4" s="46" t="str">
+        <f>B$2&amp;" -t "&amp;AC4&amp;"."&amp;AE4&amp;" "&amp;AG4</f>
+        <v>bq mk -t rtda.tweets kube-redis-bq/bigquery-setup/schema.json</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>bq mk -t rtda.tweets kube-redis-bq/bigquery-setup/schema.json</v>
+      </c>
+      <c r="AB4" s="21" t="s">
+        <v>489</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="AF4" s="21" t="s">
+        <v>491</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>492</v>
+      </c>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AK4" s="1"/>
+    </row>
+    <row r="5" spans="2:37" ht="30">
+      <c r="B5" s="49" t="str">
+        <f>"bq ls"&amp;IF(ISBLANK(AC5),""," "&amp;AC5&amp;":")</f>
+        <v>bq ls $DEVSHELL_PROJECT_ID:</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="50"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="50"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="51"/>
+      <c r="AA5" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>bq ls $DEVSHELL_PROJECT_ID:</v>
+      </c>
+      <c r="AB5" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="2:37">
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+      <c r="T6" s="50"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="50"/>
+      <c r="X6" s="50"/>
+      <c r="Y6" s="50"/>
+      <c r="Z6" s="51"/>
+      <c r="AA6" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+    </row>
+    <row r="7" spans="2:37">
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="R7" s="50"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="50"/>
+      <c r="Y7" s="50"/>
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+    </row>
+    <row r="8" spans="2:37">
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="51"/>
+      <c r="AA8" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+    </row>
+    <row r="9" spans="2:37" collapsed="1">
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+    </row>
+    <row r="10" spans="2:37" hidden="1" outlineLevel="1">
+      <c r="B10" s="39"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="51"/>
+      <c r="AA10" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+    </row>
+    <row r="11" spans="2:37" hidden="1" outlineLevel="1">
+      <c r="B11" s="39"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="51"/>
+      <c r="AA11" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+    </row>
+    <row r="12" spans="2:37" hidden="1" outlineLevel="2">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="51"/>
+      <c r="AA12" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+    </row>
+    <row r="13" spans="2:37" hidden="1" outlineLevel="2">
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="51"/>
+      <c r="AA13" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+    </row>
+    <row r="14" spans="2:37" hidden="1" outlineLevel="3">
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+    </row>
+    <row r="15" spans="2:37" hidden="1" outlineLevel="3">
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="50"/>
+      <c r="Y15" s="50"/>
+      <c r="Z15" s="51"/>
+      <c r="AA15" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+    </row>
+    <row r="16" spans="2:37" hidden="1" outlineLevel="4">
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="50"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="50"/>
+      <c r="X16" s="50"/>
+      <c r="Y16" s="50"/>
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+    </row>
+    <row r="17" spans="2:37" hidden="1" outlineLevel="4">
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+    </row>
+    <row r="18" spans="2:37" hidden="1" outlineLevel="5">
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+    </row>
+    <row r="19" spans="2:37" hidden="1" outlineLevel="5">
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+    </row>
+    <row r="20" spans="2:37" hidden="1" outlineLevel="6">
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+    </row>
+    <row r="21" spans="2:37" hidden="1" outlineLevel="6">
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+    </row>
+    <row r="22" spans="2:37" hidden="1" outlineLevel="7">
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="50"/>
+      <c r="T22" s="50"/>
+      <c r="U22" s="50"/>
+      <c r="V22" s="50"/>
+      <c r="W22" s="50"/>
+      <c r="X22" s="50"/>
+      <c r="Y22" s="50"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+    </row>
+    <row r="23" spans="2:37" hidden="1" outlineLevel="7">
+      <c r="B23" s="39"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+    </row>
+    <row r="24" spans="2:37" hidden="1" outlineLevel="6">
+      <c r="B24" s="39"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="50"/>
+      <c r="Z24" s="51"/>
+      <c r="AA24" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+    </row>
+    <row r="25" spans="2:37" hidden="1" outlineLevel="5">
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+    </row>
+    <row r="26" spans="2:37" hidden="1" outlineLevel="4">
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+    </row>
+    <row r="27" spans="2:37" hidden="1" outlineLevel="3">
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="50"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+    </row>
+    <row r="28" spans="2:37" hidden="1" outlineLevel="3">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="51"/>
+      <c r="AA28" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+    </row>
+    <row r="29" spans="2:37" hidden="1" outlineLevel="2">
+      <c r="B29" s="39"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="51"/>
+      <c r="AA29" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+    </row>
+    <row r="30" spans="2:37">
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="AB30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="1"/>
+      <c r="AK30" s="1"/>
+    </row>
+    <row r="33" ht="15" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="G25:Z25"/>
+    <mergeCell ref="F26:Z26"/>
+    <mergeCell ref="E27:Z27"/>
+    <mergeCell ref="D28:Z28"/>
+    <mergeCell ref="C29:Z29"/>
+    <mergeCell ref="B30:Z30"/>
+    <mergeCell ref="G19:Z19"/>
+    <mergeCell ref="H20:Z20"/>
+    <mergeCell ref="H21:Z21"/>
+    <mergeCell ref="I22:Z22"/>
+    <mergeCell ref="I23:Z23"/>
+    <mergeCell ref="H24:Z24"/>
+    <mergeCell ref="D13:Z13"/>
+    <mergeCell ref="E14:Z14"/>
+    <mergeCell ref="E15:Z15"/>
+    <mergeCell ref="F16:Z16"/>
+    <mergeCell ref="F17:Z17"/>
+    <mergeCell ref="G18:Z18"/>
+    <mergeCell ref="B7:Z7"/>
+    <mergeCell ref="B8:Z8"/>
+    <mergeCell ref="B9:Z9"/>
+    <mergeCell ref="C10:Z10"/>
+    <mergeCell ref="C11:Z11"/>
+    <mergeCell ref="D12:Z12"/>
+    <mergeCell ref="B1:Z1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="B2:Z2"/>
+    <mergeCell ref="B5:Z5"/>
+    <mergeCell ref="B6:Z6"/>
+    <mergeCell ref="C3:Z3"/>
+    <mergeCell ref="C4:Z4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <dimension ref="B1:AK49"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -21440,7 +22898,7 @@
     </row>
     <row r="10" spans="2:37">
       <c r="B10" s="49" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C10" s="50"/>
       <c r="D10" s="50"/>
@@ -21483,7 +22941,7 @@
     </row>
     <row r="11" spans="2:37">
       <c r="B11" s="49" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
@@ -21526,7 +22984,7 @@
     </row>
     <row r="12" spans="2:37">
       <c r="B12" s="49" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="50"/>
@@ -21569,7 +23027,7 @@
     </row>
     <row r="13" spans="2:37" ht="32.25" customHeight="1">
       <c r="B13" s="49" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
@@ -23061,7 +24519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
Added deployment-manager configuration examples to GCP cheatsheet.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Google Cloud Platform Cheatsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7230"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7230" tabRatio="653"/>
   </bookViews>
   <sheets>
     <sheet name="gcloud cheatsheet" sheetId="4" r:id="rId1"/>
@@ -14,6 +14,9 @@
     <sheet name="bq cheatsheet" sheetId="12" r:id="rId5"/>
     <sheet name="misc cheatsheet" sheetId="8" r:id="rId6"/>
     <sheet name="template cheatsheet" sheetId="9" r:id="rId7"/>
+    <sheet name="deployment-manager.yaml" sheetId="13" r:id="rId8"/>
+    <sheet name="deployment-manager.jinja" sheetId="14" r:id="rId9"/>
+    <sheet name="deployment-manager.jinja.schema" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -568,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="743">
   <si>
     <t>Details</t>
   </si>
@@ -1977,9 +1980,6 @@
     <t>default</t>
   </si>
   <si>
-    <t>$LOCATION</t>
-  </si>
-  <si>
     <t>$MY_ZONE</t>
   </si>
   <si>
@@ -2088,9 +2088,6 @@
     <t>Print version URL?</t>
   </si>
   <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
     <t>Lists all versions of files in Google Cloud Storage buckets.</t>
   </si>
   <si>
@@ -2394,12 +2391,6 @@
     <t>As user:</t>
   </si>
   <si>
-    <t>cloud-training</t>
-  </si>
-  <si>
-    <t>archinfra/dm*</t>
-  </si>
-  <si>
     <t>ingress</t>
   </si>
   <si>
@@ -2448,9 +2439,6 @@
     <t>f1-micro</t>
   </si>
   <si>
-    <t>appserver.yaml</t>
-  </si>
-  <si>
     <t>Read Google Compute Engine virtual machine types.</t>
   </si>
   <si>
@@ -2473,6 +2461,366 @@
   </si>
   <si>
     <t>Print URI only?</t>
+  </si>
+  <si>
+    <t>qwiklabs-gcp-5b57f7da0359cd75</t>
+  </si>
+  <si>
+    <t>echo-service</t>
+  </si>
+  <si>
+    <t>config.yaml</t>
+  </si>
+  <si>
+    <t>imports:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - path: instance.jinja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - path: install-echo.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    name: startup-script</t>
+  </si>
+  <si>
+    <t>resources:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - name: instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    type: instance.jinja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    properties:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      zone: europe-west1-c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      tags: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      metadata:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - key: echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          value: https://storage.googleapis.com/qwiklabs-gcp-5b57f7da0359cd75/echo-0.0.1.tar.gz</t>
+  </si>
+  <si>
+    <t>{#</t>
+  </si>
+  <si>
+    <t>Copyright 2017 Google Inc.</t>
+  </si>
+  <si>
+    <t>Licensed under the Apache License, Version 2.0 (the "License");</t>
+  </si>
+  <si>
+    <t>you may not use this file except in compliance with the License.</t>
+  </si>
+  <si>
+    <t>You may obtain a copy of the License at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    http://www.apache.org/licenses/LICENSE-2.0</t>
+  </si>
+  <si>
+    <t>Unless required by applicable law or agreed to in writing, software</t>
+  </si>
+  <si>
+    <t>distributed under the License is distributed on an "AS IS" BASIS,</t>
+  </si>
+  <si>
+    <t>WITHOUT WARRANTIES OR CONDITIONS OF ANY KIND, either express or implied.</t>
+  </si>
+  <si>
+    <t>See the License for the specific language governing permissions and</t>
+  </si>
+  <si>
+    <t>limitations under the License.</t>
+  </si>
+  <si>
+    <t>#}</t>
+  </si>
+  <si>
+    <t>- name: {{ env['deployment'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  type: compute.v1.instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  properties:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    zone: {{ properties['zone'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    machineType: zones/{{ properties['zone'] }}/machineTypes/{{ properties['machineType'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    metadata:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      items:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - key: deployment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">          value: {{ env['deployment'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {% if imports['startup-script'] %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - key: startup-script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          value: |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            {{ imports['startup-script']|indent(12) }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {% endif %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {% for i in properties["metadata"] %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - {{ i }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {% endfor %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    disks:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - deviceName: boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        boot: true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        autoDelete: true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        initializeParams:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          diskSizeGb: 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          sourceImage: {{ properties['sourceImage'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    networkInterfaces:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - name: {{ ID }}-eth0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        network: {{ properties['network'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {% if properties['subnet'] %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        subnetwork: {{ properties['subnet'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        accessConfigs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          - name: eth0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            type: ONE_TO_ONE_NAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    serviceAccounts: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      - email: {{ properties['serviceAccount'] }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        scopes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          - 'https://www.googleapis.com/auth/cloud-platform'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {% if properties['tags'] %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    tags:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {% for i in properties["tags"] %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - {{ i }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {% endif %}</t>
+  </si>
+  <si>
+    <t>outputs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - name: url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    value: http://$(ref.{{ env['deployment'] }}.networkInterfaces[0].accessConfigs[0].natIP)</t>
+  </si>
+  <si>
+    <t>info:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  title: Test instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  author: cloud-training@google.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  description: |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Creates a test instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  version: 0.1</t>
+  </si>
+  <si>
+    <t>required:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - zone</t>
+  </si>
+  <si>
+    <t>properties:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  zone:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    type: string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: i.e. us-east1-d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  network:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: Network URL i.e. projects/project/global/networks/network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    default: global/networks/default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  subnet:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: Subnet URL i.e regions/region/subnetworks/subnetwork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sourceImage: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: Image uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    default: projects/ubuntu-os-cloud/global/images/family/ubuntu-1404-lts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  machineType:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    default: n1-standard-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  serviceAccount:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: Service account with permissions to label resources i.e. Project editor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    default: default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  tags:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    type: array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: Array of tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    items:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      type: string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  metadata:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    type: array </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    description: Array of metadata key pairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      type: object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      required:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        - value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      properties:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        key:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          type: string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        value: </t>
+  </si>
+  <si>
+    <t>echo-0.0.1.tar.gz</t>
+  </si>
+  <si>
+    <t>$MY_BUCKET</t>
+  </si>
+  <si>
+    <t>public-read</t>
+  </si>
+  <si>
+    <t>Content-Type:application/gzip Cache-Control:private</t>
+  </si>
+  <si>
+    <t>Lists even more details of files and directories in Google Cloud Storage buckets.</t>
   </si>
 </sst>
 </file>
@@ -3160,32 +3508,30 @@
   </sheetPr>
   <dimension ref="B1:AU203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Z2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="26" width="2.85546875" customWidth="1"/>
-    <col min="27" max="27" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="13.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="24.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="14.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="19.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="15.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="43" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="13.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="42.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="10.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="14.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="9.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="16.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="10.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="12.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="10.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="12.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="8.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="13.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="20.5703125" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="24.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="14.140625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="19.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="15.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="43" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="13.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="42.140625" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="10.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="14.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="38" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="16.140625" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="10.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="41" width="12.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="42" max="42" width="10.140625" customWidth="1" outlineLevel="1"/>
+    <col min="43" max="43" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="8.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="13.28515625" customWidth="1" outlineLevel="1"/>
     <col min="46" max="46" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="46" customWidth="1"/>
     <col min="48" max="48" width="68.140625" customWidth="1"/>
@@ -3251,7 +3597,7 @@
     </row>
     <row r="2" spans="2:47">
       <c r="B2" s="61" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C2" s="62"/>
       <c r="D2" s="62"/>
@@ -3302,7 +3648,7 @@
       <c r="AR2" s="2"/>
       <c r="AS2" s="2"/>
       <c r="AT2" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="AU2" s="1"/>
     </row>
@@ -3417,7 +3763,7 @@
       <c r="AR4" s="2"/>
       <c r="AS4" s="2"/>
       <c r="AT4" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="AU4" s="1"/>
     </row>
@@ -3475,7 +3821,7 @@
       <c r="AR5" s="2"/>
       <c r="AS5" s="2"/>
       <c r="AT5" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="AU5" s="1"/>
     </row>
@@ -3516,7 +3862,7 @@
         <v>160</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AD6" s="22" t="s">
         <v>161</v>
@@ -3541,7 +3887,7 @@
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
       <c r="AT6" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AU6" s="1"/>
     </row>
@@ -3582,19 +3928,19 @@
         <v>160</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AD7" s="21" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AF7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AG7" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
@@ -3609,7 +3955,7 @@
       <c r="AR7" s="2"/>
       <c r="AS7" s="2"/>
       <c r="AT7" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="AU7" s="1"/>
     </row>
@@ -3710,35 +4056,35 @@
         <v>101</v>
       </c>
       <c r="AC9" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AD9" s="21" t="s">
         <v>130</v>
       </c>
       <c r="AE9" s="5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="AH9" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AL9" s="2" t="s">
         <v>173</v>
       </c>
       <c r="AM9" s="5"/>
       <c r="AN9" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AO9" s="5" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="AP9" s="2"/>
       <c r="AQ9" s="2"/>
@@ -3786,25 +4132,25 @@
         <v>101</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AD10" s="21" t="s">
         <v>168</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="AF10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AG10" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="AH10" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AI10" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AJ10" s="2" t="s">
         <v>165</v>
@@ -4127,7 +4473,7 @@
       <c r="AR15" s="2"/>
       <c r="AS15" s="2"/>
       <c r="AT15" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="AU15" s="1"/>
     </row>
@@ -4168,13 +4514,13 @@
         <v>112</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="AD16" s="21" t="s">
         <v>124</v>
       </c>
       <c r="AE16" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="AF16" s="2" t="s">
         <v>141</v>
@@ -4187,10 +4533,10 @@
       </c>
       <c r="AI16" s="5"/>
       <c r="AJ16" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="AL16" s="2"/>
       <c r="AM16" s="2"/>
@@ -4201,7 +4547,7 @@
       <c r="AR16" s="2"/>
       <c r="AS16" s="2"/>
       <c r="AT16" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="AU16" s="1"/>
     </row>
@@ -4377,7 +4723,7 @@
       <c r="AR19" s="2"/>
       <c r="AS19" s="2"/>
       <c r="AT19" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AU19" s="1"/>
     </row>
@@ -4435,7 +4781,7 @@
       <c r="AR20" s="2"/>
       <c r="AS20" s="2"/>
       <c r="AT20" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AU20" s="1"/>
     </row>
@@ -4476,13 +4822,13 @@
         <v>112</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="AD21" s="21" t="s">
         <v>89</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AF21" s="2" t="s">
         <v>97</v>
@@ -4494,13 +4840,13 @@
         <v>79</v>
       </c>
       <c r="AI21" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AJ21" s="2" t="s">
         <v>175</v>
       </c>
       <c r="AK21" s="57" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="AL21" s="2"/>
       <c r="AM21" s="2"/>
@@ -4626,13 +4972,13 @@
         <v>112</v>
       </c>
       <c r="AC23" s="5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AD23" s="21" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AE23" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AF23" s="2" t="s">
         <v>97</v>
@@ -4650,13 +4996,13 @@
         <v>175</v>
       </c>
       <c r="AK23" s="57" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AL23" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AM23" s="5" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
@@ -4665,7 +5011,7 @@
       <c r="AR23" s="2"/>
       <c r="AS23" s="2"/>
       <c r="AT23" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="AU23" s="1"/>
     </row>
@@ -4706,13 +5052,13 @@
         <v>112</v>
       </c>
       <c r="AC24" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AD24" s="21" t="s">
         <v>152</v>
       </c>
       <c r="AE24" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AF24" s="2" t="s">
         <v>97</v>
@@ -4724,13 +5070,13 @@
         <v>79</v>
       </c>
       <c r="AI24" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AJ24" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AK24" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AL24" s="2" t="s">
         <v>141</v>
@@ -4739,7 +5085,7 @@
         <v>461</v>
       </c>
       <c r="AN24" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="AO24" s="57" t="s">
         <v>461</v>
@@ -4749,7 +5095,7 @@
       <c r="AR24" s="2"/>
       <c r="AS24" s="2"/>
       <c r="AT24" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="AU24" s="1"/>
     </row>
@@ -4899,13 +5245,13 @@
         <v>129</v>
       </c>
       <c r="AC27" s="5" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="AD27" s="21" t="s">
         <v>172</v>
       </c>
       <c r="AE27" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AF27" s="2" t="s">
         <v>236</v>
@@ -4984,7 +5330,7 @@
       <c r="AR28" s="2"/>
       <c r="AS28" s="2"/>
       <c r="AT28" s="1" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="AU28" s="1"/>
     </row>
@@ -5022,7 +5368,7 @@
         <v>gcloud compute images list --uri</v>
       </c>
       <c r="AB29" s="21" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AC29" s="5" t="b">
         <v>1</v>
@@ -5044,7 +5390,7 @@
       <c r="AR29" s="2"/>
       <c r="AS29" s="2"/>
       <c r="AT29" s="1" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="AU29" s="1"/>
     </row>
@@ -5399,13 +5745,13 @@
         <v>92</v>
       </c>
       <c r="AC35" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="AD35" s="22" t="s">
         <v>11</v>
       </c>
       <c r="AE35" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
@@ -5463,19 +5809,19 @@
         <v>92</v>
       </c>
       <c r="AC36" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="AD36" s="2" t="s">
         <v>163</v>
       </c>
       <c r="AE36" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="AF36" s="22" t="s">
         <v>11</v>
       </c>
       <c r="AG36" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
@@ -5857,7 +6203,7 @@
         <v>9</v>
       </c>
       <c r="AC42" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="AD42" s="2" t="s">
         <v>291</v>
@@ -5867,7 +6213,7 @@
         <v>11</v>
       </c>
       <c r="AG42" s="5" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="AH42" s="2" t="s">
         <v>139</v>
@@ -5883,13 +6229,13 @@
         <v>126</v>
       </c>
       <c r="AM42" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="AN42" s="2" t="s">
         <v>158</v>
       </c>
       <c r="AO42" s="5" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="AP42" s="2" t="s">
         <v>159</v>
@@ -6156,7 +6502,7 @@
       <c r="AR46" s="2"/>
       <c r="AS46" s="2"/>
       <c r="AT46" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="AU46" s="1"/>
     </row>
@@ -6214,7 +6560,7 @@
       <c r="AR47" s="2"/>
       <c r="AS47" s="2"/>
       <c r="AT47" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="AU47" s="1"/>
     </row>
@@ -6252,10 +6598,10 @@
         <v>gcloud compute machine-types describe f1-micro --zone europe-west1-b</v>
       </c>
       <c r="AB48" s="21" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="AC48" s="5" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="AD48" s="22" t="s">
         <v>11</v>
@@ -6278,7 +6624,7 @@
       <c r="AR48" s="2"/>
       <c r="AS48" s="2"/>
       <c r="AT48" s="1" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="AU48" s="1"/>
     </row>
@@ -6460,7 +6806,7 @@
       <c r="AR51" s="2"/>
       <c r="AS51" s="2"/>
       <c r="AT51" s="1" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="AU51" s="1"/>
     </row>
@@ -6634,7 +6980,7 @@
       <c r="AR54" s="2"/>
       <c r="AS54" s="2"/>
       <c r="AT54" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="AU54" s="1"/>
     </row>
@@ -6692,7 +7038,7 @@
       <c r="AR55" s="2"/>
       <c r="AS55" s="2"/>
       <c r="AT55" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AU55" s="1"/>
     </row>
@@ -6750,7 +7096,7 @@
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
       <c r="AT56" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="AU56" s="1"/>
     </row>
@@ -6808,7 +7154,7 @@
       <c r="AR57" s="2"/>
       <c r="AS57" s="2"/>
       <c r="AT57" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AU57" s="1"/>
     </row>
@@ -6846,25 +7192,25 @@
         <v>gcloud compute routes create route2to1 --destination-range 10.5.4.0/24 --next-hop-vpn-tunnel tunnel2to1 --next-hop-vpn-tunnel-region europe-west1 --network vpn-network-2</v>
       </c>
       <c r="AB58" s="21" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="AC58" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AD58" s="21" t="s">
+        <v>551</v>
+      </c>
+      <c r="AE58" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="AF58" s="21" t="s">
         <v>553</v>
       </c>
-      <c r="AE58" s="5" t="s">
-        <v>558</v>
-      </c>
-      <c r="AF58" s="21" t="s">
-        <v>555</v>
-      </c>
       <c r="AG58" s="5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AH58" s="21" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="AI58" s="5" t="s">
         <v>143</v>
@@ -6873,7 +7219,7 @@
         <v>141</v>
       </c>
       <c r="AK58" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AL58" s="2"/>
       <c r="AM58" s="2"/>
@@ -6884,7 +7230,7 @@
       <c r="AR58" s="2"/>
       <c r="AS58" s="2"/>
       <c r="AT58" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="AU58" s="1"/>
     </row>
@@ -6983,16 +7329,16 @@
         <v>9</v>
       </c>
       <c r="AC60" s="5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="AD60" s="21" t="s">
         <v>11</v>
       </c>
       <c r="AE60" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="AF60" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="AG60" s="5"/>
       <c r="AH60" s="2"/>
@@ -7231,19 +7577,19 @@
         <v>89</v>
       </c>
       <c r="AC64" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AD64" s="21" t="s">
         <v>79</v>
       </c>
       <c r="AE64" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AF64" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="AG64" s="5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="AH64" s="2"/>
       <c r="AI64" s="2"/>
@@ -7296,22 +7642,22 @@
         <v>gcloud compute target-pools add-instances extloadbalancer --instances webserver1,webserver2,webserver3 --instances-zone=$MY_ZONE1</v>
       </c>
       <c r="AB65" s="21" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="AC65" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AD65" s="21" t="s">
         <v>163</v>
       </c>
       <c r="AE65" s="5" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="AF65" s="21" t="s">
         <v>11</v>
       </c>
       <c r="AG65" s="5" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="AH65" s="2"/>
       <c r="AI65" s="2"/>
@@ -7384,7 +7730,7 @@
       <c r="AR66" s="2"/>
       <c r="AS66" s="2"/>
       <c r="AT66" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AU66" s="1"/>
     </row>
@@ -7442,7 +7788,7 @@
       <c r="AR67" s="2"/>
       <c r="AS67" s="2"/>
       <c r="AT67" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="AU67" s="1"/>
     </row>
@@ -7480,16 +7826,16 @@
         <v>gcloud compute target-vpn-gateways create vpn-2 --network vpn-network-2 --region us-central1</v>
       </c>
       <c r="AB68" s="21" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AC68" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AD68" s="21" t="s">
         <v>141</v>
       </c>
       <c r="AE68" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AF68" s="21" t="s">
         <v>79</v>
@@ -7510,7 +7856,7 @@
       <c r="AR68" s="2"/>
       <c r="AS68" s="2"/>
       <c r="AT68" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="AU68" s="1"/>
     </row>
@@ -7803,10 +8149,10 @@
         <v>121</v>
       </c>
       <c r="AC73" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="AD73" s="21" t="s">
         <v>472</v>
-      </c>
-      <c r="AD73" s="21" t="s">
-        <v>473</v>
       </c>
       <c r="AE73" s="5">
         <v>23</v>
@@ -7815,7 +8161,7 @@
         <v>79</v>
       </c>
       <c r="AG73" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AH73" s="2"/>
       <c r="AI73" s="2"/>
@@ -7830,7 +8176,7 @@
       <c r="AR73" s="2"/>
       <c r="AS73" s="2"/>
       <c r="AT73" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AU73" s="1"/>
     </row>
@@ -7888,7 +8234,7 @@
       <c r="AR74" s="2"/>
       <c r="AS74" s="2"/>
       <c r="AT74" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AU74" s="1"/>
     </row>
@@ -7946,7 +8292,7 @@
       <c r="AR75" s="2"/>
       <c r="AS75" s="2"/>
       <c r="AT75" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AU75" s="1"/>
     </row>
@@ -7984,28 +8330,28 @@
         <v>gcloud compute vpn-tunnels create tunnel2to1 --peer-address $STATIC_IP_VPN_1 --shared-secret gcprocks --target-vpn-gateway vpn-2 --region europe-west1 --ike-version 2 --local-traffic-selector 0.0.0.0/0 --remote-traffic-selector 0.0.0.0/0</v>
       </c>
       <c r="AB76" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="AC76" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="AD76" s="21" t="s">
+        <v>540</v>
+      </c>
+      <c r="AE76" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="AF76" s="21" t="s">
         <v>541</v>
       </c>
-      <c r="AC76" s="5" t="s">
-        <v>548</v>
-      </c>
-      <c r="AD76" s="21" t="s">
+      <c r="AG76" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="AH76" s="21" t="s">
         <v>542</v>
       </c>
-      <c r="AE76" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="AF76" s="21" t="s">
-        <v>543</v>
-      </c>
-      <c r="AG76" s="5" t="s">
+      <c r="AI76" s="5" t="s">
         <v>519</v>
-      </c>
-      <c r="AH76" s="21" t="s">
-        <v>544</v>
-      </c>
-      <c r="AI76" s="5" t="s">
-        <v>521</v>
       </c>
       <c r="AJ76" s="21" t="s">
         <v>79</v>
@@ -8014,31 +8360,31 @@
         <v>143</v>
       </c>
       <c r="AL76" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AM76" s="5">
         <v>2</v>
       </c>
       <c r="AN76" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AO76" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AP76" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="AQ76" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AR76" s="2"/>
       <c r="AS76" s="2"/>
       <c r="AT76" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="AU76" s="1"/>
     </row>
-    <row r="77" spans="2:47" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="77" spans="2:47" hidden="1" outlineLevel="1">
       <c r="B77" s="36"/>
       <c r="C77" s="62" t="str">
         <f>B$3&amp;" zones"</f>
@@ -8092,7 +8438,7 @@
       <c r="AR77" s="2"/>
       <c r="AS77" s="2"/>
       <c r="AT77" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="AU77" s="1"/>
     </row>
@@ -8100,8 +8446,8 @@
       <c r="B78" s="36"/>
       <c r="C78" s="37"/>
       <c r="D78" s="58" t="str">
-        <f>C$77&amp;" list"</f>
-        <v>gcloud compute zones list</v>
+        <f>C$77&amp;" describe "&amp;AC78</f>
+        <v>gcloud compute zones describe europe-west1-b</v>
       </c>
       <c r="E78" s="59"/>
       <c r="F78" s="59"/>
@@ -8126,13 +8472,15 @@
       <c r="Y78" s="59"/>
       <c r="Z78" s="60"/>
       <c r="AA78" s="8" t="str">
-        <f t="shared" ref="AA78:AA79" ca="1" si="35">IFERROR(OFFSET(A78,0,MATCH("",B78:Z78,-1)),"")</f>
-        <v>gcloud compute zones list</v>
-      </c>
-      <c r="AB78" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC78" s="2"/>
+        <f ca="1">IFERROR(OFFSET(A78,0,MATCH("",B78:Z78,-1)),"")</f>
+        <v>gcloud compute zones describe europe-west1-b</v>
+      </c>
+      <c r="AB78" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC78" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="AD78" s="2"/>
       <c r="AE78" s="2"/>
       <c r="AF78" s="2"/>
@@ -8150,7 +8498,7 @@
       <c r="AR78" s="2"/>
       <c r="AS78" s="2"/>
       <c r="AT78" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AU78" s="1"/>
     </row>
@@ -8158,8 +8506,8 @@
       <c r="B79" s="36"/>
       <c r="C79" s="37"/>
       <c r="D79" s="58" t="str">
-        <f>C$77&amp;" describe "&amp;AC79</f>
-        <v>gcloud compute zones describe europe-west1-b</v>
+        <f>C$77&amp;" list"</f>
+        <v>gcloud compute zones list</v>
       </c>
       <c r="E79" s="59"/>
       <c r="F79" s="59"/>
@@ -8184,15 +8532,13 @@
       <c r="Y79" s="59"/>
       <c r="Z79" s="60"/>
       <c r="AA79" s="8" t="str">
-        <f t="shared" ca="1" si="35"/>
-        <v>gcloud compute zones describe europe-west1-b</v>
-      </c>
-      <c r="AB79" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC79" s="5" t="s">
-        <v>171</v>
-      </c>
+        <f t="shared" ref="AA79" ca="1" si="35">IFERROR(OFFSET(A79,0,MATCH("",B79:Z79,-1)),"")</f>
+        <v>gcloud compute zones list</v>
+      </c>
+      <c r="AB79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC79" s="2"/>
       <c r="AD79" s="2"/>
       <c r="AE79" s="2"/>
       <c r="AF79" s="2"/>
@@ -8210,7 +8556,7 @@
       <c r="AR79" s="2"/>
       <c r="AS79" s="2"/>
       <c r="AT79" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AU79" s="1"/>
     </row>
@@ -8415,10 +8761,10 @@
         <v>gcloud auth activate-service-account --key-file credentials.json</v>
       </c>
       <c r="AB83" s="21" t="s">
+        <v>475</v>
+      </c>
+      <c r="AC83" s="5" t="s">
         <v>476</v>
-      </c>
-      <c r="AC83" s="5" t="s">
-        <v>477</v>
       </c>
       <c r="AD83" s="2"/>
       <c r="AE83" s="2"/>
@@ -8437,10 +8783,10 @@
       <c r="AR83" s="2"/>
       <c r="AS83" s="2"/>
       <c r="AT83" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="AU83" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="84" spans="2:47" collapsed="1">
@@ -8653,7 +8999,7 @@
         <v>11</v>
       </c>
       <c r="AC87" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AD87" s="2"/>
       <c r="AE87" s="2"/>
@@ -8713,7 +9059,7 @@
         <v>79</v>
       </c>
       <c r="AC88" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AD88" s="2"/>
       <c r="AE88" s="2"/>
@@ -9847,7 +10193,7 @@
         <v>223</v>
       </c>
       <c r="AC107" s="5" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="AD107" s="2" t="s">
         <v>268</v>
@@ -9865,7 +10211,7 @@
         <v>11</v>
       </c>
       <c r="AK107" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AL107" s="2"/>
       <c r="AM107" s="2"/>
@@ -9979,13 +10325,13 @@
         <v>227</v>
       </c>
       <c r="AC109" s="5" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="AD109" s="21" t="s">
         <v>11</v>
       </c>
       <c r="AE109" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AF109" s="2"/>
       <c r="AG109" s="2"/>
@@ -10002,7 +10348,7 @@
       <c r="AR109" s="2"/>
       <c r="AS109" s="2"/>
       <c r="AT109" s="1" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="AU109" s="1"/>
     </row>
@@ -10513,14 +10859,14 @@
         <v>344</v>
       </c>
       <c r="AC118" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="AD118" s="2" t="s">
         <v>338</v>
       </c>
       <c r="AE118" s="5"/>
       <c r="AF118" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="AG118" s="5" t="b">
         <v>1</v>
@@ -10598,7 +10944,7 @@
       <c r="AR119" s="2"/>
       <c r="AS119" s="2"/>
       <c r="AT119" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="AU119" s="1"/>
     </row>
@@ -11258,7 +11604,7 @@
       <c r="D131" s="37"/>
       <c r="E131" s="58" t="str">
         <f>D$130&amp;" "&amp;AC131&amp;" --config "&amp;AE131</f>
-        <v>gcloud deployment-manager deployments create production --config appserver.yaml</v>
+        <v>gcloud deployment-manager deployments create echo-service --config config.yaml</v>
       </c>
       <c r="F131" s="59"/>
       <c r="G131" s="59"/>
@@ -11283,19 +11629,19 @@
       <c r="Z131" s="60"/>
       <c r="AA131" s="8" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>gcloud deployment-manager deployments create production --config appserver.yaml</v>
+        <v>gcloud deployment-manager deployments create echo-service --config config.yaml</v>
       </c>
       <c r="AB131" s="21" t="s">
         <v>234</v>
       </c>
       <c r="AC131" s="5" t="s">
-        <v>305</v>
+        <v>624</v>
       </c>
       <c r="AD131" s="21" t="s">
         <v>369</v>
       </c>
       <c r="AE131" s="5" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="AF131" s="2"/>
       <c r="AG131" s="2"/>
@@ -11466,13 +11812,13 @@
         <v>377</v>
       </c>
       <c r="AC134" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AD134" s="21" t="s">
         <v>369</v>
       </c>
       <c r="AE134" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AF134" s="2"/>
       <c r="AG134" s="2"/>
@@ -11489,7 +11835,7 @@
       <c r="AR134" s="2"/>
       <c r="AS134" s="2"/>
       <c r="AT134" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AU134" s="1"/>
     </row>
@@ -15352,8 +15698,8 @@
     <mergeCell ref="E131:Z131"/>
     <mergeCell ref="E132:Z132"/>
     <mergeCell ref="C77:Z77"/>
+    <mergeCell ref="D79:Z79"/>
     <mergeCell ref="D78:Z78"/>
-    <mergeCell ref="D79:Z79"/>
     <mergeCell ref="C137:Z137"/>
     <mergeCell ref="D138:Z138"/>
     <mergeCell ref="D133:Z133"/>
@@ -15548,12 +15894,292 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>736</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AS70"/>
+  <dimension ref="B1:AS69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15663,7 +16289,7 @@
       <c r="Y2" s="62"/>
       <c r="Z2" s="63"/>
       <c r="AA2" s="8" t="str">
-        <f t="shared" ref="AA2:AA48" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
+        <f t="shared" ref="AA2:AA49" ca="1" si="0">IFERROR(OFFSET(A2,0,MATCH("",B2:Z2,-1)),"")</f>
         <v>gsutil mb</v>
       </c>
       <c r="AB2" s="2" t="s">
@@ -15687,11 +16313,11 @@
       </c>
       <c r="AQ2" s="1"/>
     </row>
-    <row r="3" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+    <row r="3" spans="2:43" ht="45" hidden="1" outlineLevel="1">
       <c r="B3" s="10"/>
       <c r="C3" s="62" t="str">
         <f>B$2&amp;IF(ISBLANK(AE3),""," -l "&amp;AE3)&amp;" gs://"&amp;AC3</f>
-        <v>gsutil mb -l $LOCATION gs://$DEVSHELL_PROJECT_ID</v>
+        <v>gsutil mb gs://qwiklabs-gcp-5b57f7da0359cd75</v>
       </c>
       <c r="D3" s="62"/>
       <c r="E3" s="62"/>
@@ -15718,20 +16344,18 @@
       <c r="Z3" s="63"/>
       <c r="AA3" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>gsutil mb -l $LOCATION gs://$DEVSHELL_PROJECT_ID</v>
+        <v>gsutil mb gs://qwiklabs-gcp-5b57f7da0359cd75</v>
       </c>
       <c r="AB3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>217</v>
+        <v>623</v>
       </c>
       <c r="AD3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AE3" s="5" t="s">
-        <v>462</v>
-      </c>
+      <c r="AE3" s="5"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
@@ -15949,11 +16573,11 @@
         <v>382</v>
       </c>
     </row>
-    <row r="8" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+    <row r="8" spans="2:43" ht="45" hidden="1" outlineLevel="1">
       <c r="B8" s="12"/>
       <c r="C8" s="58" t="str">
         <f>"gsutil"&amp;IF(ISBLANK(AM8),""," -h "&amp;"'"&amp;SUBSTITUTE(AM8," ","' -h '")&amp;"'")&amp;IF(ISBLANK(AK8),""," -a "&amp;AK8)&amp;" cp "&amp;IF(AO8,"-v ","")&amp;IF(ISBLANK(AC8),"","gs://"&amp;AC8&amp;"/")&amp;AE8&amp;" "&amp;IF(ISBLANK(AG8),"","gs://"&amp;AG8&amp;"/")&amp;AI8</f>
-        <v>gsutil cp gs://cloud-training/archinfra/dm* .</v>
+        <v>gsutil -h 'Content-Type:application/gzip' -h 'Cache-Control:private' -a public-read cp echo-0.0.1.tar.gz gs://$MY_BUCKET/</v>
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="59"/>
@@ -15980,40 +16604,42 @@
       <c r="Z8" s="60"/>
       <c r="AA8" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>gsutil cp gs://cloud-training/archinfra/dm* .</v>
+        <v>gsutil -h 'Content-Type:application/gzip' -h 'Cache-Control:private' -a public-read cp echo-0.0.1.tar.gz gs://$MY_BUCKET/</v>
       </c>
       <c r="AB8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC8" s="5" t="s">
-        <v>601</v>
-      </c>
+      <c r="AC8" s="5"/>
       <c r="AD8" s="22" t="s">
         <v>56</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>602</v>
+        <v>738</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AG8" s="5"/>
+      <c r="AG8" s="5" t="s">
+        <v>739</v>
+      </c>
       <c r="AH8" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AI8" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="AI8" s="5"/>
       <c r="AJ8" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="AK8" s="5"/>
+      <c r="AK8" s="5" t="s">
+        <v>740</v>
+      </c>
       <c r="AL8" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="AM8" s="5"/>
+      <c r="AM8" s="5" t="s">
+        <v>741</v>
+      </c>
       <c r="AN8" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AO8" s="5"/>
       <c r="AP8" s="1" t="s">
@@ -16200,11 +16826,11 @@
       </c>
       <c r="AQ11" s="1"/>
     </row>
-    <row r="12" spans="2:43" hidden="1" outlineLevel="1">
-      <c r="B12" s="12"/>
+    <row r="12" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+      <c r="B12" s="50"/>
       <c r="C12" s="62" t="str">
-        <f>B$10&amp;" -l gs://"&amp;AC12&amp;"/"&amp;AE12</f>
-        <v>gsutil ls -l gs://ioso-bucket/image-dir/ada.jpg</v>
+        <f>B$10&amp;" -a gs://"&amp;AC12&amp;"/"&amp;AE12</f>
+        <v>gsutil ls -a gs://$BUCKET_NAME_1/setup.html</v>
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
@@ -16230,20 +16856,20 @@
       <c r="Y12" s="62"/>
       <c r="Z12" s="63"/>
       <c r="AA12" s="8" t="str">
-        <f t="shared" ref="AA12:AA15" ca="1" si="3">IFERROR(OFFSET(A12,0,MATCH("",B12:Z12,-1)),"")</f>
-        <v>gsutil ls -l gs://ioso-bucket/image-dir/ada.jpg</v>
+        <f t="shared" ref="AA12" ca="1" si="3">IFERROR(OFFSET(A12,0,MATCH("",B12:Z12,-1)),"")</f>
+        <v>gsutil ls -a gs://$BUCKET_NAME_1/setup.html</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>60</v>
+        <v>477</v>
       </c>
       <c r="AD12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>72</v>
+        <v>478</v>
       </c>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
@@ -16256,15 +16882,15 @@
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="1" t="s">
-        <v>69</v>
+        <v>498</v>
       </c>
       <c r="AQ12" s="1"/>
     </row>
-    <row r="13" spans="2:43" ht="30" hidden="1" outlineLevel="1">
-      <c r="B13" s="50"/>
+    <row r="13" spans="2:43" hidden="1" outlineLevel="1">
+      <c r="B13" s="12"/>
       <c r="C13" s="62" t="str">
-        <f>B$10&amp;" -a gs://"&amp;AC13&amp;"/"&amp;AE13</f>
-        <v>gsutil ls -a gs://$BUCKET_NAME_1/setup.html</v>
+        <f>B$10&amp;" -l gs://"&amp;AC13&amp;"/"&amp;AE13</f>
+        <v>gsutil ls -l gs://ioso-bucket/image-dir/ada.jpg</v>
       </c>
       <c r="D13" s="62"/>
       <c r="E13" s="62"/>
@@ -16290,20 +16916,20 @@
       <c r="Y13" s="62"/>
       <c r="Z13" s="63"/>
       <c r="AA13" s="8" t="str">
-        <f t="shared" ref="AA13" ca="1" si="4">IFERROR(OFFSET(A13,0,MATCH("",B13:Z13,-1)),"")</f>
-        <v>gsutil ls -a gs://$BUCKET_NAME_1/setup.html</v>
+        <f t="shared" ref="AA13:AA16" ca="1" si="4">IFERROR(OFFSET(A13,0,MATCH("",B13:Z13,-1)),"")</f>
+        <v>gsutil ls -l gs://ioso-bucket/image-dir/ada.jpg</v>
       </c>
       <c r="AB13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>478</v>
+        <v>60</v>
       </c>
       <c r="AD13" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>479</v>
+        <v>72</v>
       </c>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
@@ -16316,15 +16942,16 @@
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="1" t="s">
-        <v>500</v>
+        <v>69</v>
       </c>
       <c r="AQ13" s="1"/>
     </row>
-    <row r="14" spans="2:43" collapsed="1">
-      <c r="B14" s="61" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="62"/>
+    <row r="14" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+      <c r="B14" s="56"/>
+      <c r="C14" s="62" t="str">
+        <f>B$10&amp;" -L gs://"&amp;AC14&amp;"/"&amp;AE14</f>
+        <v>gsutil ls -L gs://$MY_BUCKET/echo-0.0.1.tar.gz</v>
+      </c>
       <c r="D14" s="62"/>
       <c r="E14" s="62"/>
       <c r="F14" s="62"/>
@@ -16349,15 +16976,21 @@
       <c r="Y14" s="62"/>
       <c r="Z14" s="63"/>
       <c r="AA14" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>gsutil rm</v>
+        <f t="shared" ref="AA14" ca="1" si="5">IFERROR(OFFSET(A14,0,MATCH("",B14:Z14,-1)),"")</f>
+        <v>gsutil ls -L gs://$MY_BUCKET/echo-0.0.1.tar.gz</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE14" s="5" t="s">
+        <v>738</v>
+      </c>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
@@ -16369,16 +17002,15 @@
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="1" t="s">
-        <v>73</v>
+        <v>742</v>
       </c>
       <c r="AQ14" s="1"/>
     </row>
-    <row r="15" spans="2:43" hidden="1" outlineLevel="1">
-      <c r="B15" s="12"/>
-      <c r="C15" s="62" t="str">
-        <f>B$14&amp;" gs://"&amp;AC15&amp;"/"&amp;AE15</f>
-        <v>gsutil rm gs://ioso-bucket/ada.jpg</v>
-      </c>
+    <row r="15" spans="2:43" collapsed="1">
+      <c r="B15" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="62"/>
       <c r="D15" s="62"/>
       <c r="E15" s="62"/>
       <c r="F15" s="62"/>
@@ -16403,21 +17035,15 @@
       <c r="Y15" s="62"/>
       <c r="Z15" s="63"/>
       <c r="AA15" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>gsutil rm gs://ioso-bucket/ada.jpg</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>gsutil rm</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
@@ -16429,13 +17055,16 @@
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AQ15" s="1"/>
     </row>
     <row r="16" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B16" s="12"/>
-      <c r="C16" s="62"/>
+      <c r="C16" s="62" t="str">
+        <f>B$15&amp;" gs://"&amp;AC16&amp;"/"&amp;AE16</f>
+        <v>gsutil rm gs://ioso-bucket/ada.jpg</v>
+      </c>
       <c r="D16" s="62"/>
       <c r="E16" s="62"/>
       <c r="F16" s="62"/>
@@ -16460,8 +17089,8 @@
       <c r="Y16" s="62"/>
       <c r="Z16" s="63"/>
       <c r="AA16" s="8" t="str">
-        <f t="shared" ref="AA16:AA21" ca="1" si="5">IFERROR(OFFSET(A16,0,MATCH("",B16:Z16,-1)),"")</f>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>gsutil rm gs://ioso-bucket/ada.jpg</v>
       </c>
       <c r="AB16" s="2" t="s">
         <v>14</v>
@@ -16485,13 +17114,13 @@
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
-      <c r="AP16" s="1"/>
+      <c r="AP16" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="AQ16" s="1"/>
     </row>
-    <row r="17" spans="2:45" ht="30" collapsed="1">
-      <c r="B17" s="61" t="s">
-        <v>75</v>
-      </c>
+    <row r="17" spans="2:45" hidden="1" outlineLevel="1">
+      <c r="B17" s="12"/>
       <c r="C17" s="62"/>
       <c r="D17" s="62"/>
       <c r="E17" s="62"/>
@@ -16517,15 +17146,21 @@
       <c r="Y17" s="62"/>
       <c r="Z17" s="63"/>
       <c r="AA17" s="8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>gsutil acl</v>
+        <f t="shared" ref="AA17:AA22" ca="1" si="6">IFERROR(OFFSET(A17,0,MATCH("",B17:Z17,-1)),"")</f>
+        <v/>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE17" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
@@ -16536,17 +17171,14 @@
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
-      <c r="AP17" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
     </row>
-    <row r="18" spans="2:45" hidden="1" outlineLevel="1">
-      <c r="B18" s="12"/>
-      <c r="C18" s="62" t="str">
-        <f>B$17&amp;" ch"</f>
-        <v>gsutil acl ch</v>
-      </c>
+    <row r="18" spans="2:45" ht="30" collapsed="1">
+      <c r="B18" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="62"/>
       <c r="D18" s="62"/>
       <c r="E18" s="62"/>
       <c r="F18" s="62"/>
@@ -16571,8 +17203,8 @@
       <c r="Y18" s="62"/>
       <c r="Z18" s="63"/>
       <c r="AA18" s="8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>gsutil acl ch</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>gsutil acl</v>
       </c>
       <c r="AB18" s="2" t="s">
         <v>6</v>
@@ -16590,16 +17222,18 @@
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
-      <c r="AP18" s="1"/>
+      <c r="AP18" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="AQ18" s="1"/>
     </row>
-    <row r="19" spans="2:45" ht="30" hidden="1" outlineLevel="2">
+    <row r="19" spans="2:45" hidden="1" outlineLevel="1">
       <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="62" t="str">
-        <f>C$18&amp;" -u AllUsers:R gs://"&amp;AC19&amp;"/"&amp;AE19</f>
-        <v>gsutil acl ch -u AllUsers:R gs://$BUCKET_NAME_1/setup.html</v>
-      </c>
+      <c r="C19" s="62" t="str">
+        <f>B$18&amp;" ch"</f>
+        <v>gsutil acl ch</v>
+      </c>
+      <c r="D19" s="62"/>
       <c r="E19" s="62"/>
       <c r="F19" s="62"/>
       <c r="G19" s="62"/>
@@ -16623,21 +17257,15 @@
       <c r="Y19" s="62"/>
       <c r="Z19" s="63"/>
       <c r="AA19" s="8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>gsutil acl ch -u AllUsers:R gs://$BUCKET_NAME_1/setup.html</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>gsutil acl ch</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="AD19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>479</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
@@ -16648,17 +17276,15 @@
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
-      <c r="AP19" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
     </row>
     <row r="20" spans="2:45" ht="30" hidden="1" outlineLevel="2">
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="62" t="str">
-        <f>C$18&amp;" -d AllUsers gs://"&amp;AC20&amp;"/"&amp;AE20</f>
-        <v>gsutil acl ch -d AllUsers gs://ioso-bucket/ada.jpg</v>
+        <f>C$19&amp;" -u AllUsers:R gs://"&amp;AC20&amp;"/"&amp;AE20</f>
+        <v>gsutil acl ch -u AllUsers:R gs://$BUCKET_NAME_1/setup.html</v>
       </c>
       <c r="E20" s="62"/>
       <c r="F20" s="62"/>
@@ -16683,20 +17309,20 @@
       <c r="Y20" s="62"/>
       <c r="Z20" s="63"/>
       <c r="AA20" s="8" t="str">
-        <f t="shared" ref="AA20" ca="1" si="6">IFERROR(OFFSET(A20,0,MATCH("",B20:Z20,-1)),"")</f>
-        <v>gsutil acl ch -d AllUsers gs://ioso-bucket/ada.jpg</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>gsutil acl ch -u AllUsers:R gs://$BUCKET_NAME_1/setup.html</v>
       </c>
       <c r="AB20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>60</v>
+        <v>477</v>
       </c>
       <c r="AD20" s="2" t="s">
         <v>66</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>59</v>
+        <v>478</v>
       </c>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
@@ -16709,17 +17335,17 @@
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
       <c r="AP20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ20" s="1"/>
     </row>
-    <row r="21" spans="2:45" ht="30" hidden="1" outlineLevel="1">
+    <row r="21" spans="2:45" ht="30" hidden="1" outlineLevel="2">
       <c r="B21" s="12"/>
-      <c r="C21" s="62" t="str">
-        <f>B$17&amp;" get gs://"&amp;AC21&amp;"/"&amp;AE21</f>
-        <v>gsutil acl get gs://$BUCKET_NAME_1/setup.html</v>
-      </c>
-      <c r="D21" s="62"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="62" t="str">
+        <f>C$19&amp;" -d AllUsers gs://"&amp;AC21&amp;"/"&amp;AE21</f>
+        <v>gsutil acl ch -d AllUsers gs://ioso-bucket/ada.jpg</v>
+      </c>
       <c r="E21" s="62"/>
       <c r="F21" s="62"/>
       <c r="G21" s="62"/>
@@ -16743,20 +17369,20 @@
       <c r="Y21" s="62"/>
       <c r="Z21" s="63"/>
       <c r="AA21" s="8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>gsutil acl get gs://$BUCKET_NAME_1/setup.html</v>
-      </c>
-      <c r="AB21" s="21" t="s">
+        <f t="shared" ref="AA21" ca="1" si="7">IFERROR(OFFSET(A21,0,MATCH("",B21:Z21,-1)),"")</f>
+        <v>gsutil acl ch -d AllUsers gs://ioso-bucket/ada.jpg</v>
+      </c>
+      <c r="AB21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>478</v>
+        <v>60</v>
       </c>
       <c r="AD21" s="2" t="s">
         <v>66</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>479</v>
+        <v>59</v>
       </c>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
@@ -16769,15 +17395,15 @@
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
       <c r="AP21" s="1" t="s">
-        <v>483</v>
+        <v>78</v>
       </c>
       <c r="AQ21" s="1"/>
     </row>
     <row r="22" spans="2:45" ht="30" hidden="1" outlineLevel="1">
-      <c r="B22" s="50"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="62" t="str">
-        <f>B$17&amp;" set "&amp;AC22&amp;" gs://"&amp;AE22&amp;"/"&amp;AG22</f>
-        <v>gsutil acl set private gs://$BUCKET_NAME_1/setup.html</v>
+        <f>B$18&amp;" get gs://"&amp;AC22&amp;"/"&amp;AE22</f>
+        <v>gsutil acl get gs://$BUCKET_NAME_1/setup.html</v>
       </c>
       <c r="D22" s="62"/>
       <c r="E22" s="62"/>
@@ -16803,27 +17429,23 @@
       <c r="Y22" s="62"/>
       <c r="Z22" s="63"/>
       <c r="AA22" s="8" t="str">
-        <f t="shared" ref="AA22:AA24" ca="1" si="7">IFERROR(OFFSET(A22,0,MATCH("",B22:Z22,-1)),"")</f>
-        <v>gsutil acl set private gs://$BUCKET_NAME_1/setup.html</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>gsutil acl get gs://$BUCKET_NAME_1/setup.html</v>
       </c>
       <c r="AB22" s="21" t="s">
-        <v>485</v>
+        <v>14</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="AF22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG22" s="5" t="s">
-        <v>479</v>
-      </c>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
@@ -16832,18 +17454,17 @@
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
-      <c r="AP22" s="2"/>
-      <c r="AQ22" s="2"/>
-      <c r="AR22" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="AS22" s="1"/>
-    </row>
-    <row r="23" spans="2:45" collapsed="1">
-      <c r="B23" s="61" t="s">
-        <v>480</v>
-      </c>
-      <c r="C23" s="62"/>
+      <c r="AP22" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="AQ22" s="1"/>
+    </row>
+    <row r="23" spans="2:45" ht="30" hidden="1" outlineLevel="1">
+      <c r="B23" s="50"/>
+      <c r="C23" s="62" t="str">
+        <f>B$18&amp;" set "&amp;AC23&amp;" gs://"&amp;AE23&amp;"/"&amp;AG23</f>
+        <v>gsutil acl set private gs://$BUCKET_NAME_1/setup.html</v>
+      </c>
       <c r="D23" s="62"/>
       <c r="E23" s="62"/>
       <c r="F23" s="62"/>
@@ -16868,17 +17489,27 @@
       <c r="Y23" s="62"/>
       <c r="Z23" s="63"/>
       <c r="AA23" s="8" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>gsutil rewrite</v>
-      </c>
-      <c r="AB23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC23" s="2"/>
-      <c r="AD23" s="2"/>
-      <c r="AE23" s="2"/>
-      <c r="AF23" s="2"/>
-      <c r="AG23" s="2"/>
+        <f t="shared" ref="AA23:AA25" ca="1" si="8">IFERROR(OFFSET(A23,0,MATCH("",B23:Z23,-1)),"")</f>
+        <v>gsutil acl set private gs://$BUCKET_NAME_1/setup.html</v>
+      </c>
+      <c r="AB23" s="21" t="s">
+        <v>484</v>
+      </c>
+      <c r="AC23" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE23" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG23" s="5" t="s">
+        <v>478</v>
+      </c>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
@@ -16887,17 +17518,18 @@
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
-      <c r="AP23" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AQ23" s="1"/>
-    </row>
-    <row r="24" spans="2:45" ht="30" hidden="1" outlineLevel="1">
-      <c r="B24" s="50"/>
-      <c r="C24" s="62" t="str">
-        <f>B$23&amp;" -k gs://"&amp;AC24&amp;"/"&amp;AE24</f>
-        <v>gsutil rewrite -k gs://$BUCKET_NAME_1/setup.html</v>
-      </c>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="AS23" s="1"/>
+    </row>
+    <row r="24" spans="2:45" collapsed="1">
+      <c r="B24" s="61" t="s">
+        <v>479</v>
+      </c>
+      <c r="C24" s="62"/>
       <c r="D24" s="62"/>
       <c r="E24" s="62"/>
       <c r="F24" s="62"/>
@@ -16922,21 +17554,15 @@
       <c r="Y24" s="62"/>
       <c r="Z24" s="63"/>
       <c r="AA24" s="8" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>gsutil rewrite -k gs://$BUCKET_NAME_1/setup.html</v>
-      </c>
-      <c r="AB24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC24" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="AD24" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE24" s="5" t="s">
-        <v>479</v>
-      </c>
+        <f t="shared" ca="1" si="8"/>
+        <v>gsutil rewrite</v>
+      </c>
+      <c r="AB24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
@@ -16948,15 +17574,16 @@
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
       <c r="AP24" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="AQ24" s="1"/>
     </row>
-    <row r="25" spans="2:45" collapsed="1">
-      <c r="B25" s="61" t="s">
-        <v>481</v>
-      </c>
-      <c r="C25" s="62"/>
+    <row r="25" spans="2:45" ht="30" hidden="1" outlineLevel="1">
+      <c r="B25" s="50"/>
+      <c r="C25" s="62" t="str">
+        <f>B$24&amp;" -k gs://"&amp;AC25&amp;"/"&amp;AE25</f>
+        <v>gsutil rewrite -k gs://$BUCKET_NAME_1/setup.html</v>
+      </c>
       <c r="D25" s="62"/>
       <c r="E25" s="62"/>
       <c r="F25" s="62"/>
@@ -16981,15 +17608,21 @@
       <c r="Y25" s="62"/>
       <c r="Z25" s="63"/>
       <c r="AA25" s="8" t="str">
-        <f t="shared" ref="AA25:AA26" ca="1" si="8">IFERROR(OFFSET(A25,0,MATCH("",B25:Z25,-1)),"")</f>
-        <v>gsutil lifecycle</v>
-      </c>
-      <c r="AB25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC25" s="2"/>
-      <c r="AD25" s="2"/>
-      <c r="AE25" s="2"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>gsutil rewrite -k gs://$BUCKET_NAME_1/setup.html</v>
+      </c>
+      <c r="AB25" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC25" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD25" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE25" s="5" t="s">
+        <v>478</v>
+      </c>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
@@ -17001,16 +17634,15 @@
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
       <c r="AP25" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="AQ25" s="1"/>
     </row>
-    <row r="26" spans="2:45" ht="30" hidden="1" outlineLevel="1">
-      <c r="B26" s="50"/>
-      <c r="C26" s="62" t="str">
-        <f>B$25&amp;" get gs://"&amp;AC26</f>
-        <v>gsutil lifecycle get gs://$BUCKET_NAME_1</v>
-      </c>
+    <row r="26" spans="2:45" collapsed="1">
+      <c r="B26" s="61" t="s">
+        <v>480</v>
+      </c>
+      <c r="C26" s="62"/>
       <c r="D26" s="62"/>
       <c r="E26" s="62"/>
       <c r="F26" s="62"/>
@@ -17035,15 +17667,13 @@
       <c r="Y26" s="62"/>
       <c r="Z26" s="63"/>
       <c r="AA26" s="8" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>gsutil lifecycle get gs://$BUCKET_NAME_1</v>
-      </c>
-      <c r="AB26" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC26" s="5" t="s">
-        <v>478</v>
-      </c>
+        <f t="shared" ref="AA26:AA27" ca="1" si="9">IFERROR(OFFSET(A26,0,MATCH("",B26:Z26,-1)),"")</f>
+        <v>gsutil lifecycle</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
@@ -17057,15 +17687,15 @@
       <c r="AN26" s="2"/>
       <c r="AO26" s="2"/>
       <c r="AP26" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="AQ26" s="1"/>
     </row>
     <row r="27" spans="2:45" ht="30" hidden="1" outlineLevel="1">
       <c r="B27" s="50"/>
       <c r="C27" s="62" t="str">
-        <f>B$25&amp;" set "&amp;AC27&amp;" gs://"&amp;AE27</f>
-        <v>gsutil lifecycle set life.json gs://$BUCKET_NAME_1</v>
+        <f>B$26&amp;" get gs://"&amp;AC27</f>
+        <v>gsutil lifecycle get gs://$BUCKET_NAME_1</v>
       </c>
       <c r="D27" s="62"/>
       <c r="E27" s="62"/>
@@ -17091,21 +17721,17 @@
       <c r="Y27" s="62"/>
       <c r="Z27" s="63"/>
       <c r="AA27" s="8" t="str">
-        <f t="shared" ref="AA27:AA29" ca="1" si="9">IFERROR(OFFSET(A27,0,MATCH("",B27:Z27,-1)),"")</f>
-        <v>gsutil lifecycle set life.json gs://$BUCKET_NAME_1</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>gsutil lifecycle get gs://$BUCKET_NAME_1</v>
       </c>
       <c r="AB27" s="21" t="s">
-        <v>491</v>
+        <v>14</v>
       </c>
       <c r="AC27" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="AD27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE27" s="5" t="s">
-        <v>478</v>
-      </c>
+        <v>477</v>
+      </c>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
@@ -17117,15 +17743,16 @@
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
       <c r="AP27" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="AQ27" s="1"/>
     </row>
-    <row r="28" spans="2:45" collapsed="1">
-      <c r="B28" s="61" t="s">
-        <v>482</v>
-      </c>
-      <c r="C28" s="62"/>
+    <row r="28" spans="2:45" ht="30" hidden="1" outlineLevel="1">
+      <c r="B28" s="50"/>
+      <c r="C28" s="62" t="str">
+        <f>B$26&amp;" set "&amp;AC28&amp;" gs://"&amp;AE28</f>
+        <v>gsutil lifecycle set life.json gs://$BUCKET_NAME_1</v>
+      </c>
       <c r="D28" s="62"/>
       <c r="E28" s="62"/>
       <c r="F28" s="62"/>
@@ -17150,15 +17777,21 @@
       <c r="Y28" s="62"/>
       <c r="Z28" s="63"/>
       <c r="AA28" s="8" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>gsutil versioning</v>
-      </c>
-      <c r="AB28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC28" s="2"/>
-      <c r="AD28" s="2"/>
-      <c r="AE28" s="2"/>
+        <f t="shared" ref="AA28:AA30" ca="1" si="10">IFERROR(OFFSET(A28,0,MATCH("",B28:Z28,-1)),"")</f>
+        <v>gsutil lifecycle set life.json gs://$BUCKET_NAME_1</v>
+      </c>
+      <c r="AB28" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="AC28" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="AD28" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE28" s="5" t="s">
+        <v>477</v>
+      </c>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
@@ -17174,12 +17807,11 @@
       </c>
       <c r="AQ28" s="1"/>
     </row>
-    <row r="29" spans="2:45" ht="30" hidden="1" outlineLevel="1">
-      <c r="B29" s="50"/>
-      <c r="C29" s="62" t="str">
-        <f>B$28&amp;" get gs://"&amp;AC29</f>
-        <v>gsutil versioning get gs://$BUCKET_NAME_1</v>
-      </c>
+    <row r="29" spans="2:45" collapsed="1">
+      <c r="B29" s="61" t="s">
+        <v>481</v>
+      </c>
+      <c r="C29" s="62"/>
       <c r="D29" s="62"/>
       <c r="E29" s="62"/>
       <c r="F29" s="62"/>
@@ -17204,15 +17836,13 @@
       <c r="Y29" s="62"/>
       <c r="Z29" s="63"/>
       <c r="AA29" s="8" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>gsutil versioning get gs://$BUCKET_NAME_1</v>
-      </c>
-      <c r="AB29" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC29" s="5" t="s">
-        <v>478</v>
-      </c>
+        <f t="shared" ca="1" si="10"/>
+        <v>gsutil versioning</v>
+      </c>
+      <c r="AB29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
@@ -17226,15 +17856,15 @@
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
       <c r="AP29" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="AQ29" s="1"/>
     </row>
     <row r="30" spans="2:45" ht="30" hidden="1" outlineLevel="1">
       <c r="B30" s="50"/>
       <c r="C30" s="62" t="str">
-        <f>B$28&amp;" set "&amp;IF(AC30,"on","off")&amp;" gs://"&amp;AE30</f>
-        <v>gsutil versioning set on gs://$BUCKET_NAME_1</v>
+        <f>B$29&amp;" get gs://"&amp;AC30</f>
+        <v>gsutil versioning get gs://$BUCKET_NAME_1</v>
       </c>
       <c r="D30" s="62"/>
       <c r="E30" s="62"/>
@@ -17260,21 +17890,17 @@
       <c r="Y30" s="62"/>
       <c r="Z30" s="63"/>
       <c r="AA30" s="8" t="str">
-        <f t="shared" ref="AA30:AA36" ca="1" si="10">IFERROR(OFFSET(A30,0,MATCH("",B30:Z30,-1)),"")</f>
-        <v>gsutil versioning set on gs://$BUCKET_NAME_1</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>gsutil versioning get gs://$BUCKET_NAME_1</v>
       </c>
       <c r="AB30" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="AC30" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD30" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="AE30" s="5" t="s">
-        <v>478</v>
-      </c>
+      <c r="AC30" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
@@ -17286,15 +17912,16 @@
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
       <c r="AP30" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="AQ30" s="1"/>
     </row>
-    <row r="31" spans="2:45" collapsed="1">
-      <c r="B31" s="61" t="s">
-        <v>501</v>
-      </c>
-      <c r="C31" s="62"/>
+    <row r="31" spans="2:45" ht="30" hidden="1" outlineLevel="1">
+      <c r="B31" s="50"/>
+      <c r="C31" s="62" t="str">
+        <f>B$29&amp;" set "&amp;IF(AC31,"on","off")&amp;" gs://"&amp;AE31</f>
+        <v>gsutil versioning set on gs://$BUCKET_NAME_1</v>
+      </c>
       <c r="D31" s="62"/>
       <c r="E31" s="62"/>
       <c r="F31" s="62"/>
@@ -17319,15 +17946,21 @@
       <c r="Y31" s="62"/>
       <c r="Z31" s="63"/>
       <c r="AA31" s="8" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>gsutil rsync</v>
-      </c>
-      <c r="AB31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC31" s="2"/>
-      <c r="AD31" s="2"/>
-      <c r="AE31" s="2"/>
+        <f t="shared" ref="AA31:AA37" ca="1" si="11">IFERROR(OFFSET(A31,0,MATCH("",B31:Z31,-1)),"")</f>
+        <v>gsutil versioning set on gs://$BUCKET_NAME_1</v>
+      </c>
+      <c r="AB31" s="21" t="s">
+        <v>495</v>
+      </c>
+      <c r="AC31" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE31" s="5" t="s">
+        <v>477</v>
+      </c>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
@@ -17339,16 +17972,15 @@
       <c r="AN31" s="2"/>
       <c r="AO31" s="2"/>
       <c r="AP31" s="1" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="AQ31" s="1"/>
     </row>
-    <row r="32" spans="2:45" ht="30" hidden="1" outlineLevel="1">
-      <c r="B32" s="50"/>
-      <c r="C32" s="62" t="str">
-        <f>B$31&amp;" "&amp;IF(ISBLANK(AC32),"","gs://"&amp;AC32&amp;"/")&amp;AE32&amp;" "&amp;IF(ISBLANK(AG32),"","gs://"&amp;AG32&amp;"/")&amp;AI32</f>
-        <v>gsutil rsync ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
-      </c>
+    <row r="32" spans="2:45" collapsed="1">
+      <c r="B32" s="61" t="s">
+        <v>499</v>
+      </c>
+      <c r="C32" s="62"/>
       <c r="D32" s="62"/>
       <c r="E32" s="62"/>
       <c r="F32" s="62"/>
@@ -17373,31 +18005,19 @@
       <c r="Y32" s="62"/>
       <c r="Z32" s="63"/>
       <c r="AA32" s="8" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>gsutil rsync ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>gsutil rsync</v>
       </c>
       <c r="AB32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE32" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="AF32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG32" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="AH32" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI32" s="5" t="s">
-        <v>505</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
       <c r="AJ32" s="2"/>
       <c r="AK32" s="2"/>
       <c r="AL32" s="2"/>
@@ -17405,15 +18025,15 @@
       <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
       <c r="AP32" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="AQ32" s="1"/>
     </row>
     <row r="33" spans="2:43" ht="30" hidden="1" outlineLevel="1">
       <c r="B33" s="50"/>
       <c r="C33" s="62" t="str">
-        <f>B$31&amp;" -r "&amp;IF(ISBLANK(AC33),"","gs://"&amp;AC33&amp;"/")&amp;AE33&amp;" "&amp;IF(ISBLANK(AG33),"","gs://"&amp;AG33&amp;"/")&amp;AI33</f>
-        <v>gsutil rsync -r ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
+        <f>B$32&amp;" "&amp;IF(ISBLANK(AC33),"","gs://"&amp;AC33&amp;"/")&amp;AE33&amp;" "&amp;IF(ISBLANK(AG33),"","gs://"&amp;AG33&amp;"/")&amp;AI33</f>
+        <v>gsutil rsync ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
       </c>
       <c r="D33" s="62"/>
       <c r="E33" s="62"/>
@@ -17439,8 +18059,8 @@
       <c r="Y33" s="62"/>
       <c r="Z33" s="63"/>
       <c r="AA33" s="8" t="str">
-        <f t="shared" ref="AA33" ca="1" si="11">IFERROR(OFFSET(A33,0,MATCH("",B33:Z33,-1)),"")</f>
-        <v>gsutil rsync -r ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>gsutil rsync ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
       </c>
       <c r="AB33" s="2" t="s">
         <v>55</v>
@@ -17450,19 +18070,19 @@
         <v>56</v>
       </c>
       <c r="AE33" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="AF33" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AG33" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AH33" s="22" t="s">
         <v>58</v>
       </c>
       <c r="AI33" s="5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="AJ33" s="2"/>
       <c r="AK33" s="2"/>
@@ -17471,15 +18091,16 @@
       <c r="AN33" s="2"/>
       <c r="AO33" s="2"/>
       <c r="AP33" s="1" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="AQ33" s="1"/>
     </row>
-    <row r="34" spans="2:43" s="44" customFormat="1" collapsed="1">
-      <c r="B34" s="61" t="s">
-        <v>507</v>
-      </c>
-      <c r="C34" s="62"/>
+    <row r="34" spans="2:43" ht="30" hidden="1" outlineLevel="1">
+      <c r="B34" s="50"/>
+      <c r="C34" s="62" t="str">
+        <f>B$32&amp;" -r "&amp;IF(ISBLANK(AC34),"","gs://"&amp;AC34&amp;"/")&amp;AE34&amp;" "&amp;IF(ISBLANK(AG34),"","gs://"&amp;AG34&amp;"/")&amp;AI34</f>
+        <v>gsutil rsync -r ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
+      </c>
       <c r="D34" s="62"/>
       <c r="E34" s="62"/>
       <c r="F34" s="62"/>
@@ -17503,37 +18124,48 @@
       <c r="X34" s="62"/>
       <c r="Y34" s="62"/>
       <c r="Z34" s="63"/>
-      <c r="AA34" s="43" t="str">
-        <f ca="1">IFERROR(OFFSET(A34,0,MATCH("",B34:Z34,-1)),"")</f>
-        <v>gsutil config</v>
-      </c>
-      <c r="AB34" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC34" s="22"/>
-      <c r="AD34" s="22"/>
-      <c r="AE34" s="22"/>
-      <c r="AF34" s="22"/>
-      <c r="AG34" s="22"/>
-      <c r="AH34" s="22"/>
-      <c r="AI34" s="22"/>
-      <c r="AJ34" s="22"/>
-      <c r="AK34" s="22"/>
-      <c r="AL34" s="22"/>
-      <c r="AM34" s="22"/>
-      <c r="AN34" s="22"/>
-      <c r="AO34" s="22"/>
+      <c r="AA34" s="8" t="str">
+        <f t="shared" ref="AA34" ca="1" si="12">IFERROR(OFFSET(A34,0,MATCH("",B34:Z34,-1)),"")</f>
+        <v>gsutil rsync -r ./firstlevel gs://$BUCKET_NAME_1/firstlevel</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE34" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="AF34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG34" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="AH34" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI34" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="AJ34" s="2"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
       <c r="AP34" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="AQ34" s="45"/>
-    </row>
-    <row r="35" spans="2:43" hidden="1" outlineLevel="1">
-      <c r="B35" s="50"/>
-      <c r="C35" s="62" t="str">
-        <f>B$34&amp;" -n"</f>
-        <v>gsutil config -n</v>
-      </c>
+        <v>504</v>
+      </c>
+      <c r="AQ34" s="1"/>
+    </row>
+    <row r="35" spans="2:43" s="44" customFormat="1" collapsed="1">
+      <c r="B35" s="61" t="s">
+        <v>505</v>
+      </c>
+      <c r="C35" s="62"/>
       <c r="D35" s="62"/>
       <c r="E35" s="62"/>
       <c r="F35" s="62"/>
@@ -17557,37 +18189,37 @@
       <c r="X35" s="62"/>
       <c r="Y35" s="62"/>
       <c r="Z35" s="63"/>
-      <c r="AA35" s="8" t="str">
-        <f t="shared" ref="AA35" ca="1" si="12">IFERROR(OFFSET(A35,0,MATCH("",B35:Z35,-1)),"")</f>
+      <c r="AA35" s="43" t="str">
+        <f ca="1">IFERROR(OFFSET(A35,0,MATCH("",B35:Z35,-1)),"")</f>
+        <v>gsutil config</v>
+      </c>
+      <c r="AB35" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC35" s="22"/>
+      <c r="AD35" s="22"/>
+      <c r="AE35" s="22"/>
+      <c r="AF35" s="22"/>
+      <c r="AG35" s="22"/>
+      <c r="AH35" s="22"/>
+      <c r="AI35" s="22"/>
+      <c r="AJ35" s="22"/>
+      <c r="AK35" s="22"/>
+      <c r="AL35" s="22"/>
+      <c r="AM35" s="22"/>
+      <c r="AN35" s="22"/>
+      <c r="AO35" s="22"/>
+      <c r="AP35" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AQ35" s="45"/>
+    </row>
+    <row r="36" spans="2:43" hidden="1" outlineLevel="1">
+      <c r="B36" s="50"/>
+      <c r="C36" s="62" t="str">
+        <f>B$35&amp;" -n"</f>
         <v>gsutil config -n</v>
       </c>
-      <c r="AB35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC35" s="22"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="2"/>
-      <c r="AG35" s="2"/>
-      <c r="AH35" s="2"/>
-      <c r="AI35" s="2"/>
-      <c r="AJ35" s="2"/>
-      <c r="AK35" s="2"/>
-      <c r="AL35" s="2"/>
-      <c r="AM35" s="2"/>
-      <c r="AN35" s="2"/>
-      <c r="AO35" s="2"/>
-      <c r="AP35" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="AQ35" s="1"/>
-    </row>
-    <row r="36" spans="2:43" ht="30">
-      <c r="B36" s="61" t="str">
-        <f>"gsutil cat gs://"&amp;AC36&amp;"/"&amp;AE36</f>
-        <v>gsutil cat gs://$BUCKET_NAME_2/$FILE_NAME</v>
-      </c>
-      <c r="C36" s="62"/>
       <c r="D36" s="62"/>
       <c r="E36" s="62"/>
       <c r="F36" s="62"/>
@@ -17612,21 +18244,15 @@
       <c r="Y36" s="62"/>
       <c r="Z36" s="63"/>
       <c r="AA36" s="8" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>gsutil cat gs://$BUCKET_NAME_2/$FILE_NAME</v>
-      </c>
-      <c r="AB36" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC36" s="5" t="s">
-        <v>511</v>
-      </c>
-      <c r="AD36" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE36" s="5" t="s">
-        <v>512</v>
-      </c>
+        <f t="shared" ref="AA36" ca="1" si="13">IFERROR(OFFSET(A36,0,MATCH("",B36:Z36,-1)),"")</f>
+        <v>gsutil config -n</v>
+      </c>
+      <c r="AB36" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC36" s="22"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="2"/>
       <c r="AH36" s="2"/>
@@ -17638,12 +18264,15 @@
       <c r="AN36" s="2"/>
       <c r="AO36" s="2"/>
       <c r="AP36" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="AQ36" s="1"/>
     </row>
-    <row r="37" spans="2:43" collapsed="1">
-      <c r="B37" s="61"/>
+    <row r="37" spans="2:43" ht="30">
+      <c r="B37" s="61" t="str">
+        <f>"gsutil cat gs://"&amp;AC37&amp;"/"&amp;AE37</f>
+        <v>gsutil cat gs://$BUCKET_NAME_2/$FILE_NAME</v>
+      </c>
       <c r="C37" s="62"/>
       <c r="D37" s="62"/>
       <c r="E37" s="62"/>
@@ -17669,15 +18298,21 @@
       <c r="Y37" s="62"/>
       <c r="Z37" s="63"/>
       <c r="AA37" s="8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC37" s="2"/>
-      <c r="AD37" s="2"/>
-      <c r="AE37" s="2"/>
+        <f t="shared" ca="1" si="11"/>
+        <v>gsutil cat gs://$BUCKET_NAME_2/$FILE_NAME</v>
+      </c>
+      <c r="AB37" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC37" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="AD37" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE37" s="5" t="s">
+        <v>510</v>
+      </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
@@ -17688,13 +18323,13 @@
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
-      <c r="AP37" s="1"/>
+      <c r="AP37" s="1" t="s">
+        <v>508</v>
+      </c>
       <c r="AQ37" s="1"/>
     </row>
     <row r="38" spans="2:43" collapsed="1">
-      <c r="B38" s="61" t="s">
-        <v>201</v>
-      </c>
+      <c r="B38" s="61"/>
       <c r="C38" s="62"/>
       <c r="D38" s="62"/>
       <c r="E38" s="62"/>
@@ -17721,7 +18356,7 @@
       <c r="Z38" s="63"/>
       <c r="AA38" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>gsutil -m cp -r gs://enron_corpus/allen-p .</v>
+        <v/>
       </c>
       <c r="AB38" s="2" t="s">
         <v>6</v>
@@ -17742,8 +18377,10 @@
       <c r="AP38" s="1"/>
       <c r="AQ38" s="1"/>
     </row>
-    <row r="39" spans="2:43" hidden="1" outlineLevel="1">
-      <c r="B39" s="10"/>
+    <row r="39" spans="2:43" collapsed="1">
+      <c r="B39" s="61" t="s">
+        <v>201</v>
+      </c>
       <c r="C39" s="62"/>
       <c r="D39" s="62"/>
       <c r="E39" s="62"/>
@@ -17770,7 +18407,7 @@
       <c r="Z39" s="63"/>
       <c r="AA39" s="8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>gsutil -m cp -r gs://enron_corpus/allen-p .</v>
       </c>
       <c r="AB39" s="2" t="s">
         <v>6</v>
@@ -17840,9 +18477,9 @@
       <c r="AP40" s="1"/>
       <c r="AQ40" s="1"/>
     </row>
-    <row r="41" spans="2:43" hidden="1" outlineLevel="2">
+    <row r="41" spans="2:43" hidden="1" outlineLevel="1">
       <c r="B41" s="10"/>
-      <c r="C41" s="9"/>
+      <c r="C41" s="62"/>
       <c r="D41" s="62"/>
       <c r="E41" s="62"/>
       <c r="F41" s="62"/>
@@ -17889,7 +18526,7 @@
       <c r="AP41" s="1"/>
       <c r="AQ41" s="1"/>
     </row>
-    <row r="42" spans="2:43" hidden="1" outlineLevel="2" collapsed="1">
+    <row r="42" spans="2:43" hidden="1" outlineLevel="2">
       <c r="B42" s="10"/>
       <c r="C42" s="9"/>
       <c r="D42" s="62"/>
@@ -17938,10 +18575,10 @@
       <c r="AP42" s="1"/>
       <c r="AQ42" s="1"/>
     </row>
-    <row r="43" spans="2:43" hidden="1" outlineLevel="3">
+    <row r="43" spans="2:43" hidden="1" outlineLevel="2" collapsed="1">
       <c r="B43" s="10"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="D43" s="62"/>
       <c r="E43" s="62"/>
       <c r="F43" s="62"/>
       <c r="G43" s="62"/>
@@ -18036,11 +18673,11 @@
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
     </row>
-    <row r="45" spans="2:43" hidden="1" outlineLevel="4">
+    <row r="45" spans="2:43" hidden="1" outlineLevel="3">
       <c r="B45" s="10"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
+      <c r="E45" s="62"/>
       <c r="F45" s="62"/>
       <c r="G45" s="62"/>
       <c r="H45" s="62"/>
@@ -18134,12 +18771,12 @@
       <c r="AP46" s="1"/>
       <c r="AQ46" s="1"/>
     </row>
-    <row r="47" spans="2:43" hidden="1" outlineLevel="5">
+    <row r="47" spans="2:43" hidden="1" outlineLevel="4">
       <c r="B47" s="10"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="F47" s="62"/>
       <c r="G47" s="62"/>
       <c r="H47" s="62"/>
       <c r="I47" s="62"/>
@@ -18232,13 +18869,13 @@
       <c r="AP48" s="1"/>
       <c r="AQ48" s="1"/>
     </row>
-    <row r="49" spans="2:43" hidden="1" outlineLevel="6">
+    <row r="49" spans="2:43" hidden="1" outlineLevel="5">
       <c r="B49" s="10"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="G49" s="62"/>
       <c r="H49" s="62"/>
       <c r="I49" s="62"/>
       <c r="J49" s="62"/>
@@ -18259,7 +18896,7 @@
       <c r="Y49" s="62"/>
       <c r="Z49" s="63"/>
       <c r="AA49" s="8" t="str">
-        <f t="shared" ref="AA49:AA67" ca="1" si="13">IFERROR(OFFSET(A49,0,MATCH("",B49:Z49,-1)),"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="AB49" s="2" t="s">
@@ -18308,7 +18945,7 @@
       <c r="Y50" s="62"/>
       <c r="Z50" s="63"/>
       <c r="AA50" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ref="AA50:AA66" ca="1" si="14">IFERROR(OFFSET(A50,0,MATCH("",B50:Z50,-1)),"")</f>
         <v/>
       </c>
       <c r="AB50" s="2" t="s">
@@ -18330,14 +18967,14 @@
       <c r="AP50" s="1"/>
       <c r="AQ50" s="1"/>
     </row>
-    <row r="51" spans="2:43" hidden="1" outlineLevel="7">
+    <row r="51" spans="2:43" hidden="1" outlineLevel="6">
       <c r="B51" s="10"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="H51" s="62"/>
       <c r="I51" s="62"/>
       <c r="J51" s="62"/>
       <c r="K51" s="62"/>
@@ -18357,7 +18994,7 @@
       <c r="Y51" s="62"/>
       <c r="Z51" s="63"/>
       <c r="AA51" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB51" s="2" t="s">
@@ -18406,7 +19043,7 @@
       <c r="Y52" s="62"/>
       <c r="Z52" s="63"/>
       <c r="AA52" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB52" s="2" t="s">
@@ -18428,14 +19065,14 @@
       <c r="AP52" s="1"/>
       <c r="AQ52" s="1"/>
     </row>
-    <row r="53" spans="2:43" hidden="1" outlineLevel="6">
+    <row r="53" spans="2:43" hidden="1" outlineLevel="7">
       <c r="B53" s="10"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
-      <c r="H53" s="62"/>
+      <c r="H53" s="9"/>
       <c r="I53" s="62"/>
       <c r="J53" s="62"/>
       <c r="K53" s="62"/>
@@ -18455,7 +19092,7 @@
       <c r="Y53" s="62"/>
       <c r="Z53" s="63"/>
       <c r="AA53" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB53" s="2" t="s">
@@ -18477,13 +19114,13 @@
       <c r="AP53" s="1"/>
       <c r="AQ53" s="1"/>
     </row>
-    <row r="54" spans="2:43" hidden="1" outlineLevel="5">
+    <row r="54" spans="2:43" hidden="1" outlineLevel="6">
       <c r="B54" s="10"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="62"/>
+      <c r="G54" s="9"/>
       <c r="H54" s="62"/>
       <c r="I54" s="62"/>
       <c r="J54" s="62"/>
@@ -18504,7 +19141,7 @@
       <c r="Y54" s="62"/>
       <c r="Z54" s="63"/>
       <c r="AA54" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB54" s="2" t="s">
@@ -18526,12 +19163,12 @@
       <c r="AP54" s="1"/>
       <c r="AQ54" s="1"/>
     </row>
-    <row r="55" spans="2:43" hidden="1" outlineLevel="4">
+    <row r="55" spans="2:43" hidden="1" outlineLevel="5">
       <c r="B55" s="10"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="62"/>
+      <c r="F55" s="9"/>
       <c r="G55" s="62"/>
       <c r="H55" s="62"/>
       <c r="I55" s="62"/>
@@ -18553,7 +19190,7 @@
       <c r="Y55" s="62"/>
       <c r="Z55" s="63"/>
       <c r="AA55" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB55" s="2" t="s">
@@ -18575,11 +19212,11 @@
       <c r="AP55" s="1"/>
       <c r="AQ55" s="1"/>
     </row>
-    <row r="56" spans="2:43" hidden="1" outlineLevel="3">
+    <row r="56" spans="2:43" hidden="1" outlineLevel="4">
       <c r="B56" s="10"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="62"/>
+      <c r="E56" s="9"/>
       <c r="F56" s="62"/>
       <c r="G56" s="62"/>
       <c r="H56" s="62"/>
@@ -18602,7 +19239,7 @@
       <c r="Y56" s="62"/>
       <c r="Z56" s="63"/>
       <c r="AA56" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB56" s="2" t="s">
@@ -18627,7 +19264,7 @@
     <row r="57" spans="2:43" hidden="1" outlineLevel="3">
       <c r="B57" s="10"/>
       <c r="C57" s="9"/>
-      <c r="D57" s="62"/>
+      <c r="D57" s="9"/>
       <c r="E57" s="62"/>
       <c r="F57" s="62"/>
       <c r="G57" s="62"/>
@@ -18651,7 +19288,7 @@
       <c r="Y57" s="62"/>
       <c r="Z57" s="63"/>
       <c r="AA57" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB57" s="2" t="s">
@@ -18673,9 +19310,9 @@
       <c r="AP57" s="1"/>
       <c r="AQ57" s="1"/>
     </row>
-    <row r="58" spans="2:43" hidden="1" outlineLevel="2">
+    <row r="58" spans="2:43" hidden="1" outlineLevel="3">
       <c r="B58" s="10"/>
-      <c r="C58" s="62"/>
+      <c r="C58" s="9"/>
       <c r="D58" s="62"/>
       <c r="E58" s="62"/>
       <c r="F58" s="62"/>
@@ -18700,7 +19337,7 @@
       <c r="Y58" s="62"/>
       <c r="Z58" s="63"/>
       <c r="AA58" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB58" s="2" t="s">
@@ -18722,8 +19359,8 @@
       <c r="AP58" s="1"/>
       <c r="AQ58" s="1"/>
     </row>
-    <row r="59" spans="2:43">
-      <c r="B59" s="61"/>
+    <row r="59" spans="2:43" hidden="1" outlineLevel="2">
+      <c r="B59" s="10"/>
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
       <c r="E59" s="62"/>
@@ -18749,7 +19386,7 @@
       <c r="Y59" s="62"/>
       <c r="Z59" s="63"/>
       <c r="AA59" s="8" t="str">
-        <f t="shared" ref="AA59:AA66" ca="1" si="14">IFERROR(OFFSET(A59,0,MATCH("",B59:Z59,-1)),"")</f>
+        <f t="shared" ca="1" si="14"/>
         <v/>
       </c>
       <c r="AB59" s="2" t="s">
@@ -18771,7 +19408,7 @@
       <c r="AP59" s="1"/>
       <c r="AQ59" s="1"/>
     </row>
-    <row r="60" spans="2:43">
+    <row r="60" spans="2:43" s="44" customFormat="1">
       <c r="B60" s="61"/>
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
@@ -18797,28 +19434,28 @@
       <c r="X60" s="62"/>
       <c r="Y60" s="62"/>
       <c r="Z60" s="63"/>
-      <c r="AA60" s="8" t="str">
-        <f t="shared" ca="1" si="14"/>
+      <c r="AA60" s="43" t="str">
+        <f t="shared" ref="AA60:AA65" ca="1" si="15">IFERROR(OFFSET(A60,0,MATCH("",B60:Z60,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB60" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="AC60" s="2"/>
-      <c r="AD60" s="2"/>
-      <c r="AE60" s="2"/>
-      <c r="AF60" s="2"/>
-      <c r="AG60" s="2"/>
-      <c r="AH60" s="2"/>
-      <c r="AI60" s="2"/>
-      <c r="AJ60" s="2"/>
-      <c r="AK60" s="2"/>
-      <c r="AL60" s="2"/>
-      <c r="AM60" s="2"/>
-      <c r="AN60" s="2"/>
-      <c r="AO60" s="2"/>
-      <c r="AP60" s="1"/>
-      <c r="AQ60" s="1"/>
+      <c r="AB60" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC60" s="22"/>
+      <c r="AD60" s="22"/>
+      <c r="AE60" s="22"/>
+      <c r="AF60" s="22"/>
+      <c r="AG60" s="22"/>
+      <c r="AH60" s="22"/>
+      <c r="AI60" s="22"/>
+      <c r="AJ60" s="22"/>
+      <c r="AK60" s="22"/>
+      <c r="AL60" s="22"/>
+      <c r="AM60" s="22"/>
+      <c r="AN60" s="22"/>
+      <c r="AO60" s="22"/>
+      <c r="AP60" s="45"/>
+      <c r="AQ60" s="45"/>
     </row>
     <row r="61" spans="2:43" s="44" customFormat="1">
       <c r="B61" s="61"/>
@@ -18847,7 +19484,7 @@
       <c r="Y61" s="62"/>
       <c r="Z61" s="63"/>
       <c r="AA61" s="43" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ref="AA61:AA62" ca="1" si="16">IFERROR(OFFSET(A61,0,MATCH("",B61:Z61,-1)),"")</f>
         <v/>
       </c>
       <c r="AB61" s="22" t="s">
@@ -18896,7 +19533,7 @@
       <c r="Y62" s="62"/>
       <c r="Z62" s="63"/>
       <c r="AA62" s="43" t="str">
-        <f t="shared" ref="AA62:AA63" ca="1" si="15">IFERROR(OFFSET(A62,0,MATCH("",B62:Z62,-1)),"")</f>
+        <f t="shared" ca="1" si="16"/>
         <v/>
       </c>
       <c r="AB62" s="22" t="s">
@@ -18918,7 +19555,7 @@
       <c r="AP62" s="45"/>
       <c r="AQ62" s="45"/>
     </row>
-    <row r="63" spans="2:43" s="44" customFormat="1">
+    <row r="63" spans="2:43">
       <c r="B63" s="61"/>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
@@ -18944,28 +19581,28 @@
       <c r="X63" s="62"/>
       <c r="Y63" s="62"/>
       <c r="Z63" s="63"/>
-      <c r="AA63" s="43" t="str">
-        <f t="shared" ca="1" si="15"/>
+      <c r="AA63" s="8" t="str">
+        <f t="shared" ref="AA63:AA64" ca="1" si="17">IFERROR(OFFSET(A63,0,MATCH("",B63:Z63,-1)),"")</f>
         <v/>
       </c>
-      <c r="AB63" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC63" s="22"/>
-      <c r="AD63" s="22"/>
-      <c r="AE63" s="22"/>
-      <c r="AF63" s="22"/>
-      <c r="AG63" s="22"/>
-      <c r="AH63" s="22"/>
-      <c r="AI63" s="22"/>
-      <c r="AJ63" s="22"/>
-      <c r="AK63" s="22"/>
-      <c r="AL63" s="22"/>
-      <c r="AM63" s="22"/>
-      <c r="AN63" s="22"/>
-      <c r="AO63" s="22"/>
-      <c r="AP63" s="45"/>
-      <c r="AQ63" s="45"/>
+      <c r="AB63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="2"/>
+      <c r="AE63" s="2"/>
+      <c r="AF63" s="2"/>
+      <c r="AG63" s="2"/>
+      <c r="AH63" s="2"/>
+      <c r="AI63" s="2"/>
+      <c r="AJ63" s="2"/>
+      <c r="AK63" s="2"/>
+      <c r="AL63" s="2"/>
+      <c r="AM63" s="2"/>
+      <c r="AN63" s="2"/>
+      <c r="AO63" s="2"/>
+      <c r="AP63" s="1"/>
+      <c r="AQ63" s="1"/>
     </row>
     <row r="64" spans="2:43">
       <c r="B64" s="61"/>
@@ -18994,7 +19631,7 @@
       <c r="Y64" s="62"/>
       <c r="Z64" s="63"/>
       <c r="AA64" s="8" t="str">
-        <f t="shared" ref="AA64:AA65" ca="1" si="16">IFERROR(OFFSET(A64,0,MATCH("",B64:Z64,-1)),"")</f>
+        <f t="shared" ca="1" si="17"/>
         <v/>
       </c>
       <c r="AB64" s="2" t="s">
@@ -19043,7 +19680,7 @@
       <c r="Y65" s="62"/>
       <c r="Z65" s="63"/>
       <c r="AA65" s="8" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="15"/>
         <v/>
       </c>
       <c r="AB65" s="2" t="s">
@@ -19114,85 +19751,34 @@
       <c r="AP66" s="1"/>
       <c r="AQ66" s="1"/>
     </row>
-    <row r="67" spans="2:43">
-      <c r="B67" s="61"/>
-      <c r="C67" s="62"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="62"/>
-      <c r="K67" s="62"/>
-      <c r="L67" s="62"/>
-      <c r="M67" s="62"/>
-      <c r="N67" s="62"/>
-      <c r="O67" s="62"/>
-      <c r="P67" s="62"/>
-      <c r="Q67" s="62"/>
-      <c r="R67" s="62"/>
-      <c r="S67" s="62"/>
-      <c r="T67" s="62"/>
-      <c r="U67" s="62"/>
-      <c r="V67" s="62"/>
-      <c r="W67" s="62"/>
-      <c r="X67" s="62"/>
-      <c r="Y67" s="62"/>
-      <c r="Z67" s="63"/>
-      <c r="AA67" s="8" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v/>
-      </c>
-      <c r="AB67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC67" s="2"/>
-      <c r="AD67" s="2"/>
-      <c r="AE67" s="2"/>
-      <c r="AF67" s="2"/>
-      <c r="AG67" s="2"/>
-      <c r="AH67" s="2"/>
-      <c r="AI67" s="2"/>
-      <c r="AJ67" s="2"/>
-      <c r="AK67" s="2"/>
-      <c r="AL67" s="2"/>
-      <c r="AM67" s="2"/>
-      <c r="AN67" s="2"/>
-      <c r="AO67" s="2"/>
-      <c r="AP67" s="1"/>
-      <c r="AQ67" s="1"/>
-    </row>
-    <row r="70" spans="2:43" ht="15" customHeight="1"/>
+    <row r="69" spans="2:43" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="B36:Z36"/>
-    <mergeCell ref="C13:Z13"/>
-    <mergeCell ref="B31:Z31"/>
-    <mergeCell ref="C32:Z32"/>
+  <mergeCells count="67">
+    <mergeCell ref="B37:Z37"/>
+    <mergeCell ref="C12:Z12"/>
+    <mergeCell ref="B32:Z32"/>
     <mergeCell ref="C33:Z33"/>
-    <mergeCell ref="C35:Z35"/>
+    <mergeCell ref="C34:Z34"/>
+    <mergeCell ref="C36:Z36"/>
+    <mergeCell ref="C28:Z28"/>
+    <mergeCell ref="B29:Z29"/>
+    <mergeCell ref="C30:Z30"/>
+    <mergeCell ref="C31:Z31"/>
+    <mergeCell ref="C23:Z23"/>
+    <mergeCell ref="B24:Z24"/>
+    <mergeCell ref="C25:Z25"/>
+    <mergeCell ref="B26:Z26"/>
     <mergeCell ref="C27:Z27"/>
-    <mergeCell ref="B28:Z28"/>
-    <mergeCell ref="C29:Z29"/>
-    <mergeCell ref="C30:Z30"/>
-    <mergeCell ref="C22:Z22"/>
-    <mergeCell ref="B23:Z23"/>
-    <mergeCell ref="C24:Z24"/>
-    <mergeCell ref="B25:Z25"/>
-    <mergeCell ref="C26:Z26"/>
-    <mergeCell ref="B34:Z34"/>
-    <mergeCell ref="B59:Z59"/>
+    <mergeCell ref="B35:Z35"/>
+    <mergeCell ref="B65:Z65"/>
+    <mergeCell ref="B63:Z63"/>
+    <mergeCell ref="B64:Z64"/>
     <mergeCell ref="B60:Z60"/>
-    <mergeCell ref="B66:Z66"/>
-    <mergeCell ref="B64:Z64"/>
-    <mergeCell ref="B65:Z65"/>
     <mergeCell ref="B61:Z61"/>
     <mergeCell ref="B62:Z62"/>
-    <mergeCell ref="B63:Z63"/>
-    <mergeCell ref="C18:Z18"/>
-    <mergeCell ref="D19:Z19"/>
+    <mergeCell ref="C19:Z19"/>
     <mergeCell ref="D20:Z20"/>
+    <mergeCell ref="D21:Z21"/>
     <mergeCell ref="B1:Z1"/>
     <mergeCell ref="AB1:AE1"/>
     <mergeCell ref="B7:Z7"/>
@@ -19202,38 +19788,39 @@
     <mergeCell ref="C3:Z3"/>
     <mergeCell ref="C4:Z4"/>
     <mergeCell ref="C5:Z5"/>
-    <mergeCell ref="G47:Z47"/>
+    <mergeCell ref="C14:Z14"/>
+    <mergeCell ref="G48:Z48"/>
     <mergeCell ref="C6:Z6"/>
-    <mergeCell ref="B37:Z37"/>
     <mergeCell ref="B38:Z38"/>
-    <mergeCell ref="C39:Z39"/>
+    <mergeCell ref="B39:Z39"/>
     <mergeCell ref="C40:Z40"/>
-    <mergeCell ref="D41:Z41"/>
+    <mergeCell ref="C41:Z41"/>
+    <mergeCell ref="D42:Z42"/>
     <mergeCell ref="B10:Z10"/>
     <mergeCell ref="C11:Z11"/>
-    <mergeCell ref="C12:Z12"/>
-    <mergeCell ref="B14:Z14"/>
-    <mergeCell ref="C15:Z15"/>
+    <mergeCell ref="C13:Z13"/>
+    <mergeCell ref="B15:Z15"/>
     <mergeCell ref="C16:Z16"/>
-    <mergeCell ref="B17:Z17"/>
-    <mergeCell ref="C21:Z21"/>
-    <mergeCell ref="D42:Z42"/>
-    <mergeCell ref="E43:Z43"/>
+    <mergeCell ref="C17:Z17"/>
+    <mergeCell ref="B18:Z18"/>
+    <mergeCell ref="C22:Z22"/>
+    <mergeCell ref="D43:Z43"/>
     <mergeCell ref="E44:Z44"/>
-    <mergeCell ref="F45:Z45"/>
+    <mergeCell ref="E45:Z45"/>
     <mergeCell ref="F46:Z46"/>
-    <mergeCell ref="B67:Z67"/>
-    <mergeCell ref="G48:Z48"/>
-    <mergeCell ref="H49:Z49"/>
+    <mergeCell ref="F47:Z47"/>
+    <mergeCell ref="B66:Z66"/>
+    <mergeCell ref="G49:Z49"/>
     <mergeCell ref="H50:Z50"/>
-    <mergeCell ref="I51:Z51"/>
+    <mergeCell ref="H51:Z51"/>
     <mergeCell ref="I52:Z52"/>
-    <mergeCell ref="H53:Z53"/>
-    <mergeCell ref="G54:Z54"/>
-    <mergeCell ref="F55:Z55"/>
-    <mergeCell ref="E56:Z56"/>
-    <mergeCell ref="D57:Z57"/>
-    <mergeCell ref="C58:Z58"/>
+    <mergeCell ref="I53:Z53"/>
+    <mergeCell ref="H54:Z54"/>
+    <mergeCell ref="G55:Z55"/>
+    <mergeCell ref="F56:Z56"/>
+    <mergeCell ref="E57:Z57"/>
+    <mergeCell ref="D58:Z58"/>
+    <mergeCell ref="C59:Z59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19378,7 +19965,7 @@
         <v>80</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="2"/>
@@ -19441,14 +20028,14 @@
         <v>237</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="AH3" s="2" t="s">
         <v>236</v>
       </c>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="AK3" s="5">
         <v>80</v>
@@ -19461,7 +20048,7 @@
         <v>229</v>
       </c>
       <c r="AQ3" s="1" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="4" spans="2:43" ht="30">
@@ -19501,13 +20088,13 @@
         <v>240</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="AD4" s="22" t="s">
         <v>239</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="AF4" s="2" t="s">
         <v>267</v>
@@ -19522,11 +20109,11 @@
       </c>
       <c r="AK4" s="5"/>
       <c r="AL4" s="2" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="AM4" s="5"/>
       <c r="AN4" s="2" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="AO4" s="5" t="b">
         <v>1</v>
@@ -19627,7 +20214,7 @@
         <v>244</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -20349,13 +20936,13 @@
         <v>240</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="AD19" s="22" t="s">
         <v>239</v>
       </c>
       <c r="AE19" s="5" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
@@ -21544,7 +22131,7 @@
     </row>
     <row r="40" spans="2:43">
       <c r="B40" s="61" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C40" s="62"/>
       <c r="D40" s="62"/>
@@ -21589,13 +22176,13 @@
       <c r="AN40" s="2"/>
       <c r="AO40" s="2"/>
       <c r="AP40" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AQ40" s="1"/>
     </row>
     <row r="41" spans="2:43" collapsed="1">
       <c r="B41" s="61" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C41" s="62"/>
       <c r="D41" s="62"/>
@@ -21640,7 +22227,7 @@
       <c r="AN41" s="2"/>
       <c r="AO41" s="2"/>
       <c r="AP41" s="1" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="AQ41" s="1"/>
     </row>
@@ -21700,7 +22287,7 @@
       <c r="AN42" s="2"/>
       <c r="AO42" s="2"/>
       <c r="AP42" s="1" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="AQ42" s="1"/>
     </row>
@@ -21741,7 +22328,7 @@
         <v>244</v>
       </c>
       <c r="AC43" s="5" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="AD43" s="2"/>
       <c r="AE43" s="2"/>
@@ -21756,7 +22343,7 @@
       <c r="AN43" s="2"/>
       <c r="AO43" s="2"/>
       <c r="AP43" s="1" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="AQ43" s="1"/>
     </row>
@@ -25893,10 +26480,10 @@
         <v>bq query "select string_field_10 as request, count(*) as requestcount from logdata.accesslog group by request order by requestcount desc"</v>
       </c>
       <c r="AB6" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="AC6" s="5" t="s">
         <v>470</v>
-      </c>
-      <c r="AC6" s="5" t="s">
-        <v>471</v>
       </c>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -25905,7 +26492,7 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AK6" s="1"/>
     </row>
@@ -30424,4 +31011,404 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A65"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection sqref="A1:A65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>695</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>